<commit_message>
wprowadzenie wyników kolejnych symulacji
</commit_message>
<xml_diff>
--- a/doc/projekt/Wyniki_symulacji/Symulacje_podsumowanie.xlsx
+++ b/doc/projekt/Wyniki_symulacji/Symulacje_podsumowanie.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrycja\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\SDSZ\doc\projekt\Wyniki_symulacji\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="594"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="594" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BEZ OŚWIETLENIA" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="10">
   <si>
     <t>Słonecznie</t>
   </si>
@@ -61,7 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,8 +97,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +188,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,19 +327,97 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -340,36 +432,37 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="4" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -654,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,279 +763,279 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="28"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="49"/>
     </row>
     <row r="2" spans="1:28" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5">
+      <c r="A2" s="1"/>
+      <c r="B2" s="54">
         <v>43871</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="7"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="56"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="9" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="10" t="s">
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="11"/>
+      <c r="U3" s="52"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
+      <c r="Z3" s="52"/>
+      <c r="AA3" s="52"/>
+      <c r="AB3" s="53"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="11">
         <v>8</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>9</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="11">
         <v>10</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="11">
         <v>11</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <v>12</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="11">
         <v>13</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="11">
         <v>14</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="11">
         <v>15</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="11">
         <v>16</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="12">
         <v>8</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="12">
         <v>9</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="12">
         <v>10</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="12">
         <v>11</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="12">
         <v>12</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="12">
         <v>13</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="Q4" s="12">
         <v>14</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="12">
         <v>15</v>
       </c>
-      <c r="S4" s="14">
+      <c r="S4" s="12">
         <v>16</v>
       </c>
-      <c r="T4" s="15">
+      <c r="T4" s="13">
         <v>8</v>
       </c>
-      <c r="U4" s="15">
+      <c r="U4" s="13">
         <v>9</v>
       </c>
-      <c r="V4" s="15">
+      <c r="V4" s="13">
         <v>10</v>
       </c>
-      <c r="W4" s="15">
+      <c r="W4" s="13">
         <v>11</v>
       </c>
-      <c r="X4" s="15">
+      <c r="X4" s="13">
         <v>12</v>
       </c>
-      <c r="Y4" s="15">
+      <c r="Y4" s="13">
         <v>13</v>
       </c>
-      <c r="Z4" s="15">
+      <c r="Z4" s="13">
         <v>14</v>
       </c>
-      <c r="AA4" s="15">
+      <c r="AA4" s="13">
         <v>15</v>
       </c>
-      <c r="AB4" s="16">
+      <c r="AB4" s="34">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="14">
         <v>306.97799318181796</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="14">
         <v>211.29017727272731</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="14">
         <v>239.95258636363621</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="14">
         <v>313.91405681818162</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="14">
         <v>408.96258181818206</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="14">
         <v>473.46798863636366</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="14">
         <v>2604.1693431818148</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="14">
         <v>2901.3150022727268</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="14">
         <v>366.50846363636373</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="15">
         <v>69.386988636363611</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="15">
         <v>93.679129545454458</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="15">
         <v>132.45580227272725</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="15">
         <v>171.48112045454562</v>
       </c>
-      <c r="O5" s="32">
+      <c r="O5" s="15">
         <v>209.04576590909082</v>
       </c>
-      <c r="P5" s="32">
+      <c r="P5" s="15">
         <v>226.30044090909084</v>
       </c>
-      <c r="Q5" s="32">
+      <c r="Q5" s="15">
         <v>531.4571431818182</v>
       </c>
-      <c r="R5" s="32">
+      <c r="R5" s="15">
         <v>532.87136590909108</v>
       </c>
-      <c r="S5" s="32">
+      <c r="S5" s="15">
         <v>93.756840909090897</v>
       </c>
-      <c r="T5" s="33">
+      <c r="T5" s="16">
         <v>39.318211363636358</v>
       </c>
-      <c r="U5" s="33">
+      <c r="U5" s="16">
         <v>75.418138636363608</v>
       </c>
-      <c r="V5" s="33">
+      <c r="V5" s="16">
         <v>103.71945909090908</v>
       </c>
-      <c r="W5" s="33">
+      <c r="W5" s="16">
         <v>119.95691136363632</v>
       </c>
-      <c r="X5" s="33">
+      <c r="X5" s="16">
         <v>123.98602954545447</v>
       </c>
-      <c r="Y5" s="33">
+      <c r="Y5" s="16">
         <v>115.66398863636357</v>
       </c>
-      <c r="Z5" s="33">
+      <c r="Z5" s="16">
         <v>99.071650000000076</v>
       </c>
-      <c r="AA5" s="33">
+      <c r="AA5" s="16">
         <v>68.95575227272721</v>
       </c>
-      <c r="AB5" s="34">
+      <c r="AB5" s="35">
         <v>33.024054545454518</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="17">
@@ -1023,12 +1116,12 @@
       <c r="AA6" s="19">
         <v>25.210435518714977</v>
       </c>
-      <c r="AB6" s="20">
+      <c r="AB6" s="36">
         <v>11.748475128766062</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="17">
@@ -1109,12 +1202,12 @@
       <c r="AA7" s="19">
         <v>21.390999999999998</v>
       </c>
-      <c r="AB7" s="20">
+      <c r="AB7" s="36">
         <v>9.1509999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="17">
@@ -1195,372 +1288,372 @@
       <c r="AA8" s="19">
         <v>155.14699999999999</v>
       </c>
-      <c r="AB8" s="20">
+      <c r="AB8" s="36">
         <v>76.641000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="22"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="37"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="22"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="37"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="22"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="37"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="21"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="21"/>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="22"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="37"/>
     </row>
     <row r="13" spans="1:28" ht="21" x14ac:dyDescent="0.4">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5">
+      <c r="A13" s="1"/>
+      <c r="B13" s="57">
         <v>43961</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6"/>
-      <c r="AB13" s="7"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="58"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="58"/>
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="59"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="9" t="s">
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="10" t="s">
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14" s="11"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
+      <c r="X14" s="45"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="45"/>
+      <c r="AA14" s="45"/>
+      <c r="AB14" s="46"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="11">
         <v>8</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="11">
         <v>9</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="11">
         <v>10</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="11">
         <v>11</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="11">
         <v>12</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="11">
         <v>13</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="11">
         <v>14</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="11">
         <v>15</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="11">
         <v>16</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="12">
         <v>8</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="12">
         <v>9</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15" s="12">
         <v>10</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15" s="12">
         <v>11</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15" s="12">
         <v>12</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="12">
         <v>13</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="Q15" s="12">
         <v>14</v>
       </c>
-      <c r="R15" s="14">
+      <c r="R15" s="12">
         <v>15</v>
       </c>
-      <c r="S15" s="14">
+      <c r="S15" s="12">
         <v>16</v>
       </c>
-      <c r="T15" s="15">
+      <c r="T15" s="13">
         <v>8</v>
       </c>
-      <c r="U15" s="15">
+      <c r="U15" s="13">
         <v>9</v>
       </c>
-      <c r="V15" s="15">
+      <c r="V15" s="13">
         <v>10</v>
       </c>
-      <c r="W15" s="15">
+      <c r="W15" s="13">
         <v>11</v>
       </c>
-      <c r="X15" s="15">
+      <c r="X15" s="13">
         <v>12</v>
       </c>
-      <c r="Y15" s="15">
+      <c r="Y15" s="13">
         <v>13</v>
       </c>
-      <c r="Z15" s="15">
+      <c r="Z15" s="13">
         <v>14</v>
       </c>
-      <c r="AA15" s="15">
+      <c r="AA15" s="13">
         <v>15</v>
       </c>
-      <c r="AB15" s="16">
+      <c r="AB15" s="34">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="14">
         <v>366.55165909090891</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="14">
         <v>447.25880909090944</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="14">
         <v>596.81263863636389</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="14">
         <v>752.88176590909131</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="14">
         <v>828.32497272727221</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="14">
         <v>854.63904772727267</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="14">
         <v>856.20616818181838</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="14">
         <v>828.15132272727294</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="14">
         <v>1007.342143181818</v>
       </c>
-      <c r="K16" s="32">
+      <c r="K16" s="15">
         <v>186.10482500000001</v>
       </c>
-      <c r="L16" s="32">
+      <c r="L16" s="15">
         <v>189.55283409090924</v>
       </c>
-      <c r="M16" s="32">
+      <c r="M16" s="15">
         <v>199.81122499999989</v>
       </c>
-      <c r="N16" s="32">
+      <c r="N16" s="15">
         <v>220.70051818181813</v>
       </c>
-      <c r="O16" s="32">
+      <c r="O16" s="15">
         <v>252.89508863636374</v>
       </c>
-      <c r="P16" s="32">
+      <c r="P16" s="15">
         <v>320.84143409090905</v>
       </c>
-      <c r="Q16" s="32">
+      <c r="Q16" s="15">
         <v>407.65040454545436</v>
       </c>
-      <c r="R16" s="32">
+      <c r="R16" s="15">
         <v>473.73586136363627</v>
       </c>
-      <c r="S16" s="32">
+      <c r="S16" s="15">
         <v>487.91660454545445</v>
       </c>
-      <c r="T16" s="33">
+      <c r="T16" s="16">
         <v>182.41482500000001</v>
       </c>
-      <c r="U16" s="33">
+      <c r="U16" s="16">
         <v>213.42037954545438</v>
       </c>
-      <c r="V16" s="33">
+      <c r="V16" s="16">
         <v>238.82496590909091</v>
       </c>
-      <c r="W16" s="33">
+      <c r="W16" s="16">
         <v>248.18396136363643</v>
       </c>
-      <c r="X16" s="33">
+      <c r="X16" s="16">
         <v>251.72076363636353</v>
       </c>
-      <c r="Y16" s="33">
+      <c r="Y16" s="16">
         <v>241.72190000000001</v>
       </c>
-      <c r="Z16" s="33">
+      <c r="Z16" s="16">
         <v>223.18317272727296</v>
       </c>
-      <c r="AA16" s="33">
+      <c r="AA16" s="16">
         <v>192.22997045454582</v>
       </c>
-      <c r="AB16" s="34">
+      <c r="AB16" s="35">
         <v>157.02362045454555</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="17">
@@ -1641,12 +1734,12 @@
       <c r="AA17" s="19">
         <v>68.17713482572087</v>
       </c>
-      <c r="AB17" s="20">
+      <c r="AB17" s="36">
         <v>55.289349101375237</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="17">
@@ -1727,12 +1820,12 @@
       <c r="AA18" s="19">
         <v>73.078999999999994</v>
       </c>
-      <c r="AB18" s="20">
+      <c r="AB18" s="36">
         <v>56.448999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="17">
@@ -1813,129 +1906,129 @@
       <c r="AA19" s="19">
         <v>434.27600000000001</v>
       </c>
-      <c r="AB19" s="20">
+      <c r="AB19" s="36">
         <v>360.88400000000001</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="22"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="4"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
-      <c r="AB21" s="22"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="4"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="22"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="4"/>
     </row>
     <row r="23" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="24"/>
-      <c r="AB23" s="25"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1955,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB17"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y46" sqref="Y46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1969,1098 +2062,2879 @@
     <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="3"/>
-    </row>
-    <row r="2" spans="1:28" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+    <row r="1" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="60">
+        <v>43871</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="62"/>
+    </row>
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="55">
         <v>10</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="7"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="56"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="9" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="10" t="s">
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="11"/>
+      <c r="U3" s="52"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
+      <c r="Z3" s="52"/>
+      <c r="AA3" s="52"/>
+      <c r="AB3" s="53"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="21">
         <v>8</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="21">
         <v>9</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="21">
         <v>10</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="21">
         <v>11</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="21">
         <v>12</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="21">
         <v>13</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="21">
         <v>14</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="21">
         <v>15</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="21">
         <v>16</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="22">
         <v>8</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="22">
         <v>9</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="22">
         <v>10</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="22">
         <v>11</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="22">
         <v>12</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="22">
         <v>13</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="Q4" s="22">
         <v>14</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="22">
         <v>15</v>
       </c>
-      <c r="S4" s="14">
+      <c r="S4" s="22">
         <v>16</v>
       </c>
-      <c r="T4" s="15">
+      <c r="T4" s="23">
         <v>8</v>
       </c>
-      <c r="U4" s="15">
+      <c r="U4" s="23">
         <v>9</v>
       </c>
-      <c r="V4" s="15">
+      <c r="V4" s="23">
         <v>10</v>
       </c>
-      <c r="W4" s="15">
+      <c r="W4" s="23">
         <v>11</v>
       </c>
-      <c r="X4" s="15">
+      <c r="X4" s="23">
         <v>12</v>
       </c>
-      <c r="Y4" s="15">
+      <c r="Y4" s="23">
         <v>13</v>
       </c>
-      <c r="Z4" s="15">
+      <c r="Z4" s="23">
         <v>14</v>
       </c>
-      <c r="AA4" s="15">
+      <c r="AA4" s="23">
         <v>15</v>
       </c>
-      <c r="AB4" s="16">
+      <c r="AB4" s="30">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="10">
         <v>485.76221363636319</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="10">
         <v>398.20669318181848</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="10">
         <v>422.31838636363653</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="10">
         <v>495.98754772727244</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="10">
         <v>582.59455227272701</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="10">
         <v>646.1752431818187</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="10">
         <v>2769.4831045454553</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="10">
         <v>3077.7944772727301</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="10">
         <v>553.58102499999995</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="24">
         <v>258.54030681818205</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="24">
         <v>283.58884090909078</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="24">
         <v>319.97347500000018</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="24">
         <v>359.5538931818183</v>
       </c>
-      <c r="O5" s="32">
+      <c r="O5" s="24">
         <v>394.3079659090908</v>
       </c>
-      <c r="P5" s="32">
+      <c r="P5" s="24">
         <v>412.65190227272785</v>
       </c>
-      <c r="Q5" s="32">
+      <c r="Q5" s="24">
         <v>717.51509772727286</v>
       </c>
-      <c r="R5" s="32">
+      <c r="R5" s="24">
         <v>717.19315681818171</v>
       </c>
-      <c r="S5" s="32">
+      <c r="S5" s="24">
         <v>283.80481818181806</v>
       </c>
-      <c r="T5" s="33">
+      <c r="T5" s="25">
         <v>230.11202045454536</v>
       </c>
-      <c r="U5" s="33">
+      <c r="U5" s="25">
         <v>265.75268409090916</v>
       </c>
-      <c r="V5" s="33">
+      <c r="V5" s="25">
         <v>292.52396590909109</v>
       </c>
-      <c r="W5" s="33">
+      <c r="W5" s="25">
         <v>308.86150227272714</v>
       </c>
-      <c r="X5" s="33">
+      <c r="X5" s="25">
         <v>313.68701590909058</v>
       </c>
-      <c r="Y5" s="33">
+      <c r="Y5" s="25">
         <v>306.74312500000002</v>
       </c>
-      <c r="Z5" s="33">
+      <c r="Z5" s="25">
         <v>289.13227500000028</v>
       </c>
-      <c r="AA5" s="33">
+      <c r="AA5" s="25">
         <v>260.41307954545465</v>
       </c>
-      <c r="AB5" s="34">
+      <c r="AB5" s="31">
         <v>223.94552045454543</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="26">
         <v>311.9830077480101</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="26">
         <v>52.09011984726677</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="26">
         <v>46.873161800841693</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="26">
         <v>44.89025093055502</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="26">
         <v>52.057253383231021</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="26">
         <v>73.959903282829728</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="26">
         <v>3361.815305495008</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="26">
         <v>2247.2409727964932</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="26">
         <v>344.53489365945387</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="27">
         <v>40.250131238980423</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="27">
         <v>27.01203468121717</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="27">
         <v>27.738655329341608</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="27">
         <v>27.828693909781812</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="27">
         <v>32.184255812738471</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="27">
         <v>35.173223928810344</v>
       </c>
-      <c r="Q6" s="18">
+      <c r="Q6" s="27">
         <v>510.34320640743294</v>
       </c>
-      <c r="R6" s="18">
+      <c r="R6" s="27">
         <v>333.89098633604351</v>
       </c>
-      <c r="S6" s="18">
+      <c r="S6" s="27">
         <v>56.508154906221613</v>
       </c>
-      <c r="T6" s="19">
+      <c r="T6" s="28">
         <v>20.966160161008858</v>
       </c>
-      <c r="U6" s="19">
+      <c r="U6" s="28">
         <v>18.450423542069444</v>
       </c>
-      <c r="V6" s="19">
+      <c r="V6" s="28">
         <v>20.974515157609368</v>
       </c>
-      <c r="W6" s="19">
+      <c r="W6" s="28">
         <v>25.677669279303903</v>
       </c>
-      <c r="X6" s="19">
+      <c r="X6" s="28">
         <v>26.256477245114372</v>
       </c>
-      <c r="Y6" s="19">
+      <c r="Y6" s="28">
         <v>25.482701109413803</v>
       </c>
-      <c r="Z6" s="19">
+      <c r="Z6" s="28">
         <v>20.307585751880719</v>
       </c>
-      <c r="AA6" s="19">
+      <c r="AA6" s="28">
         <v>18.260486361164585</v>
       </c>
-      <c r="AB6" s="20">
+      <c r="AB6" s="32">
         <v>22.014702749162382</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="26">
         <v>297.95499999999998</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="26">
         <v>268.09199999999998</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="26">
         <v>298.10500000000002</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="26">
         <v>365.73</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="26">
         <v>441.22199999999998</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="26">
         <v>456.553</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="26">
         <v>492.637</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="26">
         <v>442.00599999999997</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="26">
         <v>283.05200000000002</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="27">
         <v>203.23</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="27">
         <v>200.52799999999999</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="27">
         <v>247.74100000000001</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="27">
         <v>301.31700000000001</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="27">
         <v>313.56900000000002</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="27">
         <v>319.00299999999999</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="Q7" s="27">
         <v>319.92099999999999</v>
       </c>
-      <c r="R7" s="18">
+      <c r="R7" s="27">
         <v>268.26600000000002</v>
       </c>
-      <c r="S7" s="18">
+      <c r="S7" s="27">
         <v>200.63399999999999</v>
       </c>
-      <c r="T7" s="19">
+      <c r="T7" s="28">
         <v>180.405</v>
       </c>
-      <c r="U7" s="19">
+      <c r="U7" s="28">
         <v>211.23699999999999</v>
       </c>
-      <c r="V7" s="19">
+      <c r="V7" s="28">
         <v>236.18899999999999</v>
       </c>
-      <c r="W7" s="19">
+      <c r="W7" s="28">
         <v>251.83</v>
       </c>
-      <c r="X7" s="19">
+      <c r="X7" s="28">
         <v>247.20599999999999</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="Y7" s="28">
         <v>240.851</v>
       </c>
-      <c r="Z7" s="19">
+      <c r="Z7" s="28">
         <v>238.80699999999999</v>
       </c>
-      <c r="AA7" s="19">
+      <c r="AA7" s="28">
         <v>206.61699999999999</v>
       </c>
-      <c r="AB7" s="20">
+      <c r="AB7" s="32">
         <v>167.08</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="26">
         <v>1628.664</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="26">
         <v>578.827</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="26">
         <v>561.38</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="26">
         <v>630.17499999999995</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="26">
         <v>767.81</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="26">
         <v>884.64300000000003</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="26">
         <v>8325.7060000000001</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="26">
         <v>5317.3879999999999</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="26">
         <v>1476.42</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="27">
         <v>395.64100000000002</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="27">
         <v>373.21600000000001</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="27">
         <v>412.70400000000001</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="27">
         <v>458.73700000000002</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="27">
         <v>527.80399999999997</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="27">
         <v>520.34699999999998</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="27">
         <v>1612.0340000000001</v>
       </c>
-      <c r="R8" s="18">
+      <c r="R8" s="27">
         <v>1078.596</v>
       </c>
-      <c r="S8" s="18">
+      <c r="S8" s="27">
         <v>442.31099999999998</v>
       </c>
-      <c r="T8" s="19">
+      <c r="T8" s="28">
         <v>281.05900000000003</v>
       </c>
-      <c r="U8" s="19">
+      <c r="U8" s="28">
         <v>315.18400000000003</v>
       </c>
-      <c r="V8" s="19">
+      <c r="V8" s="28">
         <v>365.04899999999998</v>
       </c>
-      <c r="W8" s="19">
+      <c r="W8" s="28">
         <v>408.71100000000001</v>
       </c>
-      <c r="X8" s="19">
+      <c r="X8" s="28">
         <v>410.678</v>
       </c>
-      <c r="Y8" s="19">
+      <c r="Y8" s="28">
         <v>414.75700000000001</v>
       </c>
-      <c r="Z8" s="19">
+      <c r="Z8" s="28">
         <v>358.197</v>
       </c>
-      <c r="AA8" s="19">
+      <c r="AA8" s="28">
         <v>309.90699999999998</v>
       </c>
-      <c r="AB8" s="20">
+      <c r="AB8" s="32">
         <v>271.40100000000001</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="22"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="33"/>
     </row>
     <row r="10" spans="1:28" ht="21" x14ac:dyDescent="0.4">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="55">
+        <v>15</v>
+      </c>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="55"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="55"/>
+      <c r="U10" s="55"/>
+      <c r="V10" s="55"/>
+      <c r="W10" s="55"/>
+      <c r="X10" s="55"/>
+      <c r="Y10" s="55"/>
+      <c r="Z10" s="55"/>
+      <c r="AA10" s="55"/>
+      <c r="AB10" s="56"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="U11" s="52"/>
+      <c r="V11" s="52"/>
+      <c r="W11" s="52"/>
+      <c r="X11" s="52"/>
+      <c r="Y11" s="52"/>
+      <c r="Z11" s="52"/>
+      <c r="AA11" s="52"/>
+      <c r="AB11" s="53"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="21">
+        <v>8</v>
+      </c>
+      <c r="C12" s="21">
+        <v>9</v>
+      </c>
+      <c r="D12" s="21">
+        <v>10</v>
+      </c>
+      <c r="E12" s="21">
+        <v>11</v>
+      </c>
+      <c r="F12" s="21">
+        <v>12</v>
+      </c>
+      <c r="G12" s="21">
+        <v>13</v>
+      </c>
+      <c r="H12" s="21">
+        <v>14</v>
+      </c>
+      <c r="I12" s="21">
+        <v>15</v>
+      </c>
+      <c r="J12" s="21">
+        <v>16</v>
+      </c>
+      <c r="K12" s="22">
+        <v>8</v>
+      </c>
+      <c r="L12" s="22">
+        <v>9</v>
+      </c>
+      <c r="M12" s="22">
+        <v>10</v>
+      </c>
+      <c r="N12" s="22">
+        <v>11</v>
+      </c>
+      <c r="O12" s="22">
+        <v>12</v>
+      </c>
+      <c r="P12" s="22">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="22">
+        <v>14</v>
+      </c>
+      <c r="R12" s="22">
+        <v>15</v>
+      </c>
+      <c r="S12" s="22">
+        <v>16</v>
+      </c>
+      <c r="T12" s="23">
+        <v>8</v>
+      </c>
+      <c r="U12" s="23">
+        <v>9</v>
+      </c>
+      <c r="V12" s="23">
+        <v>10</v>
+      </c>
+      <c r="W12" s="23">
+        <v>11</v>
+      </c>
+      <c r="X12" s="23">
+        <v>12</v>
+      </c>
+      <c r="Y12" s="23">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="23">
+        <v>14</v>
+      </c>
+      <c r="AA12" s="23">
+        <v>15</v>
+      </c>
+      <c r="AB12" s="30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="10">
+        <v>547.8486772727274</v>
+      </c>
+      <c r="C13" s="10">
+        <v>474.53577045454603</v>
+      </c>
+      <c r="D13" s="10">
+        <v>499.27968181818198</v>
+      </c>
+      <c r="E13" s="10">
+        <v>576.78293409090907</v>
+      </c>
+      <c r="F13" s="10">
+        <v>669.28821136363638</v>
+      </c>
+      <c r="G13" s="10">
+        <v>715.70930454545419</v>
+      </c>
+      <c r="H13" s="10">
+        <v>2845.6722181818177</v>
+      </c>
+      <c r="I13" s="10">
+        <v>3157.7726522727289</v>
+      </c>
+      <c r="J13" s="10">
+        <v>628.62182727272727</v>
+      </c>
+      <c r="K13" s="24">
+        <v>346.24552272727266</v>
+      </c>
+      <c r="L13" s="24">
+        <v>364.83776136363701</v>
+      </c>
+      <c r="M13" s="24">
+        <v>398.99494545454536</v>
+      </c>
+      <c r="N13" s="24">
+        <v>435.35074545454552</v>
+      </c>
+      <c r="O13" s="24">
+        <v>470.01009090909071</v>
+      </c>
+      <c r="P13" s="24">
+        <v>484.15430000000026</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>791.25547045454516</v>
+      </c>
+      <c r="R13" s="24">
+        <v>797.80969999999991</v>
+      </c>
+      <c r="S13" s="24">
+        <v>372.81232727272715</v>
+      </c>
+      <c r="T13" s="25">
+        <v>321.51098636363639</v>
+      </c>
+      <c r="U13" s="25">
+        <v>351.31402272727274</v>
+      </c>
+      <c r="V13" s="25">
+        <v>373.49639545454528</v>
+      </c>
+      <c r="W13" s="25">
+        <v>387.29820227272745</v>
+      </c>
+      <c r="X13" s="25">
+        <v>392.03668409090898</v>
+      </c>
+      <c r="Y13" s="25">
+        <v>385.49954545454563</v>
+      </c>
+      <c r="Z13" s="25">
+        <v>369.67566363636394</v>
+      </c>
+      <c r="AA13" s="25">
+        <v>347.05817499999989</v>
+      </c>
+      <c r="AB13" s="31">
+        <v>316.3978886363634</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="26">
+        <v>294.51450008226453</v>
+      </c>
+      <c r="C14" s="26">
+        <v>67.628705959809736</v>
+      </c>
+      <c r="D14" s="26">
+        <v>58.028069047400969</v>
+      </c>
+      <c r="E14" s="26">
+        <v>54.731135411800949</v>
+      </c>
+      <c r="F14" s="26">
+        <v>56.358329017323868</v>
+      </c>
+      <c r="G14" s="26">
+        <v>62.279845090667315</v>
+      </c>
+      <c r="H14" s="26">
+        <v>3347.0513171746102</v>
+      </c>
+      <c r="I14" s="26">
+        <v>2258.20873080621</v>
+      </c>
+      <c r="J14" s="26">
+        <v>349.62221271962011</v>
+      </c>
+      <c r="K14" s="27">
+        <v>46.073065833003326</v>
+      </c>
+      <c r="L14" s="27">
+        <v>43.37182966596388</v>
+      </c>
+      <c r="M14" s="27">
+        <v>41.590059055264788</v>
+      </c>
+      <c r="N14" s="27">
+        <v>39.495971058605043</v>
+      </c>
+      <c r="O14" s="27">
+        <v>38.326154287154132</v>
+      </c>
+      <c r="P14" s="27">
+        <v>34.886587353346002</v>
+      </c>
+      <c r="Q14" s="27">
+        <v>494.67168364795828</v>
+      </c>
+      <c r="R14" s="27">
+        <v>346.67178301233116</v>
+      </c>
+      <c r="S14" s="27">
+        <v>69.592678696683123</v>
+      </c>
+      <c r="T14" s="28">
+        <v>41.976567214801335</v>
+      </c>
+      <c r="U14" s="28">
+        <v>35.53178766010749</v>
+      </c>
+      <c r="V14" s="28">
+        <v>32.919554479765083</v>
+      </c>
+      <c r="W14" s="28">
+        <v>30.605330882701317</v>
+      </c>
+      <c r="X14" s="28">
+        <v>31.962020650907537</v>
+      </c>
+      <c r="Y14" s="28">
+        <v>32.059549122582176</v>
+      </c>
+      <c r="Z14" s="28">
+        <v>31.386772367144097</v>
+      </c>
+      <c r="AA14" s="28">
+        <v>36.537757963590259</v>
+      </c>
+      <c r="AB14" s="32">
+        <v>43.147260558603755</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="26">
+        <v>341.33100000000002</v>
+      </c>
+      <c r="C15" s="26">
+        <v>331.04300000000001</v>
+      </c>
+      <c r="D15" s="26">
+        <v>353.709</v>
+      </c>
+      <c r="E15" s="26">
+        <v>425.846</v>
+      </c>
+      <c r="F15" s="26">
+        <v>519.47799999999995</v>
+      </c>
+      <c r="G15" s="26">
+        <v>552.50699999999995</v>
+      </c>
+      <c r="H15" s="26">
+        <v>592.76700000000005</v>
+      </c>
+      <c r="I15" s="26">
+        <v>506.53300000000002</v>
+      </c>
+      <c r="J15" s="26">
+        <v>332.90499999999997</v>
+      </c>
+      <c r="K15" s="27">
+        <v>253.273</v>
+      </c>
+      <c r="L15" s="27">
+        <v>262.71199999999999</v>
+      </c>
+      <c r="M15" s="27">
+        <v>300.02699999999999</v>
+      </c>
+      <c r="N15" s="27">
+        <v>319.81900000000002</v>
+      </c>
+      <c r="O15" s="27">
+        <v>350.529</v>
+      </c>
+      <c r="P15" s="27">
+        <v>395.03100000000001</v>
+      </c>
+      <c r="Q15" s="27">
+        <v>400.35899999999998</v>
+      </c>
+      <c r="R15" s="27">
+        <v>334.25900000000001</v>
+      </c>
+      <c r="S15" s="27">
+        <v>258.70400000000001</v>
+      </c>
+      <c r="T15" s="28">
+        <v>227.43</v>
+      </c>
+      <c r="U15" s="28">
+        <v>263.11500000000001</v>
+      </c>
+      <c r="V15" s="28">
+        <v>278.834</v>
+      </c>
+      <c r="W15" s="28">
+        <v>307.34100000000001</v>
+      </c>
+      <c r="X15" s="28">
+        <v>311.50799999999998</v>
+      </c>
+      <c r="Y15" s="28">
+        <v>299.19099999999997</v>
+      </c>
+      <c r="Z15" s="28">
+        <v>286.42399999999998</v>
+      </c>
+      <c r="AA15" s="28">
+        <v>251.88900000000001</v>
+      </c>
+      <c r="AB15" s="32">
+        <v>226.77600000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="26">
+        <v>1632.4849999999999</v>
+      </c>
+      <c r="C16" s="26">
+        <v>679.87699999999995</v>
+      </c>
+      <c r="D16" s="26">
+        <v>711.15300000000002</v>
+      </c>
+      <c r="E16" s="26">
+        <v>760.59400000000005</v>
+      </c>
+      <c r="F16" s="26">
+        <v>864.85599999999999</v>
+      </c>
+      <c r="G16" s="26">
+        <v>957.46699999999998</v>
+      </c>
+      <c r="H16" s="26">
+        <v>8399.7980000000007</v>
+      </c>
+      <c r="I16" s="26">
+        <v>5398.24</v>
+      </c>
+      <c r="J16" s="26">
+        <v>1563.9570000000001</v>
+      </c>
+      <c r="K16" s="27">
+        <v>449.88600000000002</v>
+      </c>
+      <c r="L16" s="27">
+        <v>475.96</v>
+      </c>
+      <c r="M16" s="27">
+        <v>509.38200000000001</v>
+      </c>
+      <c r="N16" s="27">
+        <v>542.47400000000005</v>
+      </c>
+      <c r="O16" s="27">
+        <v>593.04499999999996</v>
+      </c>
+      <c r="P16" s="27">
+        <v>604.05700000000002</v>
+      </c>
+      <c r="Q16" s="27">
+        <v>1670.1769999999999</v>
+      </c>
+      <c r="R16" s="27">
+        <v>1198.798</v>
+      </c>
+      <c r="S16" s="27">
+        <v>550.15700000000004</v>
+      </c>
+      <c r="T16" s="28">
+        <v>409.72500000000002</v>
+      </c>
+      <c r="U16" s="28">
+        <v>433.80700000000002</v>
+      </c>
+      <c r="V16" s="28">
+        <v>451.05099999999999</v>
+      </c>
+      <c r="W16" s="28">
+        <v>472.50200000000001</v>
+      </c>
+      <c r="X16" s="28">
+        <v>474.09500000000003</v>
+      </c>
+      <c r="Y16" s="28">
+        <v>475.97899999999998</v>
+      </c>
+      <c r="Z16" s="28">
+        <v>448.57299999999998</v>
+      </c>
+      <c r="AA16" s="28">
+        <v>445.98500000000001</v>
+      </c>
+      <c r="AB16" s="32">
+        <v>410.68700000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="29"/>
+      <c r="AB17" s="33"/>
+    </row>
+    <row r="18" spans="1:28" ht="21" x14ac:dyDescent="0.4">
+      <c r="A18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="55">
         <v>20</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="7"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="8" t="s">
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
+      <c r="U18" s="55"/>
+      <c r="V18" s="55"/>
+      <c r="W18" s="55"/>
+      <c r="X18" s="55"/>
+      <c r="Y18" s="55"/>
+      <c r="Z18" s="55"/>
+      <c r="AA18" s="55"/>
+      <c r="AB18" s="56"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="9" t="s">
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="10" t="s">
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="10"/>
-      <c r="AB11" s="11"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="U19" s="52"/>
+      <c r="V19" s="52"/>
+      <c r="W19" s="52"/>
+      <c r="X19" s="52"/>
+      <c r="Y19" s="52"/>
+      <c r="Z19" s="52"/>
+      <c r="AA19" s="52"/>
+      <c r="AB19" s="53"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B20" s="21">
         <v>8</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C20" s="21">
         <v>9</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D20" s="21">
         <v>10</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E20" s="21">
         <v>11</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F20" s="21">
         <v>12</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G20" s="21">
         <v>13</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H20" s="21">
         <v>14</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I20" s="21">
         <v>15</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J20" s="21">
         <v>16</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K20" s="22">
         <v>8</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L20" s="22">
         <v>9</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M20" s="22">
         <v>10</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N20" s="22">
         <v>11</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O20" s="22">
         <v>12</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P20" s="22">
         <v>13</v>
       </c>
-      <c r="Q12" s="14">
+      <c r="Q20" s="22">
         <v>14</v>
       </c>
-      <c r="R12" s="14">
+      <c r="R20" s="22">
         <v>15</v>
       </c>
-      <c r="S12" s="14">
+      <c r="S20" s="22">
         <v>16</v>
       </c>
-      <c r="T12" s="15">
+      <c r="T20" s="23">
         <v>8</v>
       </c>
-      <c r="U12" s="15">
+      <c r="U20" s="23">
         <v>9</v>
       </c>
-      <c r="V12" s="15">
+      <c r="V20" s="23">
         <v>10</v>
       </c>
-      <c r="W12" s="15">
+      <c r="W20" s="23">
         <v>11</v>
       </c>
-      <c r="X12" s="15">
+      <c r="X20" s="23">
         <v>12</v>
       </c>
-      <c r="Y12" s="15">
+      <c r="Y20" s="23">
         <v>13</v>
       </c>
-      <c r="Z12" s="15">
+      <c r="Z20" s="23">
         <v>14</v>
       </c>
-      <c r="AA12" s="15">
+      <c r="AA20" s="23">
         <v>15</v>
       </c>
-      <c r="AB12" s="16">
+      <c r="AB20" s="30">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B21" s="10">
         <v>676.71386136363594</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C21" s="10">
         <v>586.53245454545413</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D21" s="10">
         <v>614.01075227272759</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E21" s="10">
         <v>686.09765909090913</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F21" s="10">
         <v>771.24303863636328</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G21" s="10">
         <v>832.13181136363607</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H21" s="10">
         <v>2960.5927386363605</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I21" s="10">
         <v>3267.4820454545429</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J21" s="10">
         <v>740.69885454545465</v>
       </c>
-      <c r="K13" s="32">
+      <c r="K21" s="24">
         <v>420.70145454545485</v>
       </c>
-      <c r="L13" s="32">
+      <c r="L21" s="24">
         <v>456.59014090909096</v>
       </c>
-      <c r="M13" s="32">
+      <c r="M21" s="24">
         <v>482.40016590909107</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N21" s="24">
         <v>500.50382500000029</v>
       </c>
-      <c r="O13" s="32">
+      <c r="O21" s="24">
         <v>505.33353863636319</v>
       </c>
-      <c r="P13" s="32">
+      <c r="P21" s="24">
         <v>497.76450454545449</v>
       </c>
-      <c r="Q13" s="32">
+      <c r="Q21" s="24">
         <v>480.49092954545466</v>
       </c>
-      <c r="R13" s="32">
+      <c r="R21" s="24">
         <v>451.64454545454572</v>
       </c>
-      <c r="S13" s="32">
+      <c r="S21" s="24">
         <v>414.67259772727311</v>
       </c>
-      <c r="T13" s="33">
+      <c r="T21" s="25">
         <v>420.91791136363628</v>
       </c>
-      <c r="U13" s="33">
+      <c r="U21" s="25">
         <v>456.61468636363628</v>
       </c>
-      <c r="V13" s="33">
+      <c r="V21" s="25">
         <v>483.75562045454552</v>
       </c>
-      <c r="W13" s="33">
+      <c r="W21" s="25">
         <v>499.76808636363666</v>
       </c>
-      <c r="X13" s="33">
+      <c r="X21" s="25">
         <v>504.0010204545456</v>
       </c>
-      <c r="Y13" s="33">
+      <c r="Y21" s="25">
         <v>497.47239318181852</v>
       </c>
-      <c r="Z13" s="33">
+      <c r="Z21" s="25">
         <v>479.84251818181804</v>
       </c>
-      <c r="AA13" s="33">
+      <c r="AA21" s="25">
         <v>451.32945909090887</v>
       </c>
-      <c r="AB13" s="34">
+      <c r="AB21" s="31">
         <v>414.59771590909065</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B22" s="26">
         <v>294.70962175022612</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C22" s="26">
         <v>76.466547030445113</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D22" s="26">
         <v>67.433037154471577</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E22" s="26">
         <v>64.050426161457978</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F22" s="26">
         <v>57.30455910389589</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G22" s="26">
         <v>68.80269310194555</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H22" s="26">
         <v>3341.0628496692843</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I22" s="26">
         <v>2267.4167534333537</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J22" s="26">
         <v>355.40791843315776</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K22" s="27">
         <v>49.700885369824185</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L22" s="27">
         <v>42.050532242040262</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M22" s="27">
         <v>39.135446323687027</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N22" s="27">
         <v>36.954734434805246</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O22" s="27">
         <v>36.388874772272459</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P22" s="27">
         <v>35.886178905116147</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="Q22" s="27">
         <v>38.284111873499604</v>
       </c>
-      <c r="R14" s="18">
+      <c r="R22" s="27">
         <v>43.511795450209704</v>
       </c>
-      <c r="S14" s="18">
+      <c r="S22" s="27">
         <v>51.29702671117527</v>
       </c>
-      <c r="T14" s="19">
+      <c r="T22" s="28">
         <v>50.243057274791205</v>
       </c>
-      <c r="U14" s="19">
+      <c r="U22" s="28">
         <v>42.291854620114776</v>
       </c>
-      <c r="V14" s="19">
+      <c r="V22" s="28">
         <v>39.158065984582088</v>
       </c>
-      <c r="W14" s="19">
+      <c r="W22" s="28">
         <v>36.288229029874728</v>
       </c>
-      <c r="X14" s="19">
+      <c r="X22" s="28">
         <v>34.832617080033302</v>
       </c>
-      <c r="Y14" s="19">
+      <c r="Y22" s="28">
         <v>38.580367357292545</v>
       </c>
-      <c r="Z14" s="19">
+      <c r="Z22" s="28">
         <v>39.004294557189439</v>
       </c>
-      <c r="AA14" s="19">
+      <c r="AA22" s="28">
         <v>43.493517361256302</v>
       </c>
-      <c r="AB14" s="20">
+      <c r="AB22" s="32">
         <v>51.180642156330251</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B23" s="26">
         <v>456.19200000000001</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C23" s="26">
         <v>404.887</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D23" s="26">
         <v>455.488</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E23" s="26">
         <v>505.53800000000001</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F23" s="26">
         <v>597.66899999999998</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G23" s="26">
         <v>582.42200000000003</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H23" s="26">
         <v>705.61400000000003</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I23" s="26">
         <v>595.37699999999995</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J23" s="26">
         <v>432.87</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K23" s="27">
         <v>306.49400000000003</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L23" s="27">
         <v>334.49900000000002</v>
       </c>
-      <c r="M15" s="18">
+      <c r="M23" s="27">
         <v>377.49700000000001</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N23" s="27">
         <v>397.25099999999998</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O23" s="27">
         <v>397.505</v>
       </c>
-      <c r="P15" s="18">
+      <c r="P23" s="27">
         <v>385.64800000000002</v>
       </c>
-      <c r="Q15" s="18">
+      <c r="Q23" s="27">
         <v>377.04599999999999</v>
       </c>
-      <c r="R15" s="18">
+      <c r="R23" s="27">
         <v>339.59800000000001</v>
       </c>
-      <c r="S15" s="18">
+      <c r="S23" s="27">
         <v>303.12299999999999</v>
       </c>
-      <c r="T15" s="19">
+      <c r="T23" s="28">
         <v>310.27</v>
       </c>
-      <c r="U15" s="19">
+      <c r="U23" s="28">
         <v>344.92200000000003</v>
       </c>
-      <c r="V15" s="19">
+      <c r="V23" s="28">
         <v>373.63</v>
       </c>
-      <c r="W15" s="19">
+      <c r="W23" s="28">
         <v>375.55</v>
       </c>
-      <c r="X15" s="19">
+      <c r="X23" s="28">
         <v>398.81599999999997</v>
       </c>
-      <c r="Y15" s="19">
+      <c r="Y23" s="28">
         <v>376.42</v>
       </c>
-      <c r="Z15" s="19">
+      <c r="Z23" s="28">
         <v>374.98399999999998</v>
       </c>
-      <c r="AA15" s="19">
+      <c r="AA23" s="28">
         <v>339.99700000000001</v>
       </c>
-      <c r="AB15" s="20">
+      <c r="AB23" s="32">
         <v>307.80500000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+    <row r="24" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B24" s="39">
         <v>1752.1659999999999</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C24" s="39">
         <v>859.62900000000002</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D24" s="39">
         <v>785.10400000000004</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E24" s="39">
         <v>873.68700000000001</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F24" s="39">
         <v>928.58799999999997</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G24" s="39">
         <v>1065.7829999999999</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H24" s="39">
         <v>8535.7939999999999</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I24" s="39">
         <v>5550.165</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J24" s="39">
         <v>1724.2460000000001</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K24" s="40">
         <v>521.99699999999996</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L24" s="40">
         <v>559.81100000000004</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M24" s="40">
         <v>584.08199999999999</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N24" s="40">
         <v>600.27099999999996</v>
       </c>
-      <c r="O16" s="18">
+      <c r="O24" s="40">
         <v>596.17200000000003</v>
       </c>
-      <c r="P16" s="18">
+      <c r="P24" s="40">
         <v>594.52599999999995</v>
       </c>
-      <c r="Q16" s="18">
+      <c r="Q24" s="40">
         <v>582.65300000000002</v>
       </c>
-      <c r="R16" s="18">
+      <c r="R24" s="40">
         <v>556.38499999999999</v>
       </c>
-      <c r="S16" s="18">
+      <c r="S24" s="40">
         <v>519.774</v>
       </c>
-      <c r="T16" s="19">
+      <c r="T24" s="41">
         <v>528.78399999999999</v>
       </c>
-      <c r="U16" s="19">
+      <c r="U24" s="41">
         <v>561.029</v>
       </c>
-      <c r="V16" s="19">
+      <c r="V24" s="41">
         <v>572.63300000000004</v>
       </c>
-      <c r="W16" s="19">
+      <c r="W24" s="41">
         <v>587.83900000000006</v>
       </c>
-      <c r="X16" s="19">
+      <c r="X24" s="41">
         <v>587.755</v>
       </c>
-      <c r="Y16" s="19">
+      <c r="Y24" s="41">
         <v>594.93299999999999</v>
       </c>
-      <c r="Z16" s="19">
+      <c r="Z24" s="41">
         <v>576.65599999999995</v>
       </c>
-      <c r="AA16" s="19">
+      <c r="AA24" s="41">
         <v>543.64200000000005</v>
       </c>
-      <c r="AB16" s="20">
+      <c r="AB24" s="42">
         <v>517.197</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="25"/>
+    <row r="26" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A27" s="60">
+        <v>43961</v>
+      </c>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="68"/>
+      <c r="T27" s="64"/>
+      <c r="U27" s="64"/>
+      <c r="V27" s="64"/>
+      <c r="W27" s="64"/>
+      <c r="X27" s="64"/>
+      <c r="Y27" s="64"/>
+      <c r="Z27" s="64"/>
+      <c r="AA27" s="64"/>
+      <c r="AB27" s="64"/>
+    </row>
+    <row r="28" spans="1:28" ht="21" x14ac:dyDescent="0.4">
+      <c r="A28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="55">
+        <v>10</v>
+      </c>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="65"/>
+      <c r="V28" s="65"/>
+      <c r="W28" s="65"/>
+      <c r="X28" s="65"/>
+      <c r="Y28" s="65"/>
+      <c r="Z28" s="65"/>
+      <c r="AA28" s="65"/>
+      <c r="AB28" s="65"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="52"/>
+      <c r="S29" s="53"/>
+      <c r="T29" s="66"/>
+      <c r="U29" s="66"/>
+      <c r="V29" s="66"/>
+      <c r="W29" s="66"/>
+      <c r="X29" s="66"/>
+      <c r="Y29" s="66"/>
+      <c r="Z29" s="66"/>
+      <c r="AA29" s="66"/>
+      <c r="AB29" s="66"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="22">
+        <v>8</v>
+      </c>
+      <c r="C30" s="22">
+        <v>9</v>
+      </c>
+      <c r="D30" s="22">
+        <v>10</v>
+      </c>
+      <c r="E30" s="22">
+        <v>11</v>
+      </c>
+      <c r="F30" s="22">
+        <v>12</v>
+      </c>
+      <c r="G30" s="22">
+        <v>13</v>
+      </c>
+      <c r="H30" s="22">
+        <v>14</v>
+      </c>
+      <c r="I30" s="22">
+        <v>15</v>
+      </c>
+      <c r="J30" s="22">
+        <v>16</v>
+      </c>
+      <c r="K30" s="23">
+        <v>8</v>
+      </c>
+      <c r="L30" s="23">
+        <v>9</v>
+      </c>
+      <c r="M30" s="23">
+        <v>10</v>
+      </c>
+      <c r="N30" s="23">
+        <v>11</v>
+      </c>
+      <c r="O30" s="23">
+        <v>12</v>
+      </c>
+      <c r="P30" s="23">
+        <v>13</v>
+      </c>
+      <c r="Q30" s="23">
+        <v>14</v>
+      </c>
+      <c r="R30" s="23">
+        <v>15</v>
+      </c>
+      <c r="S30" s="30">
+        <v>16</v>
+      </c>
+      <c r="T30" s="66"/>
+      <c r="U30" s="66"/>
+      <c r="V30" s="66"/>
+      <c r="W30" s="66"/>
+      <c r="X30" s="66"/>
+      <c r="Y30" s="66"/>
+      <c r="Z30" s="66"/>
+      <c r="AA30" s="66"/>
+      <c r="AB30" s="66"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="24">
+        <v>332.13288409090939</v>
+      </c>
+      <c r="C31" s="24">
+        <v>362.17868181818221</v>
+      </c>
+      <c r="D31" s="24">
+        <v>379.36322500000006</v>
+      </c>
+      <c r="E31" s="24">
+        <v>391.29670227272732</v>
+      </c>
+      <c r="F31" s="24">
+        <v>393.75616363636379</v>
+      </c>
+      <c r="G31" s="24">
+        <v>383.81751590909101</v>
+      </c>
+      <c r="H31" s="24">
+        <v>364.36914090909096</v>
+      </c>
+      <c r="I31" s="24">
+        <v>341.47414545454575</v>
+      </c>
+      <c r="J31" s="24">
+        <v>307.75097272727277</v>
+      </c>
+      <c r="K31" s="25">
+        <v>332.33948181818187</v>
+      </c>
+      <c r="L31" s="25">
+        <v>359.20507045454565</v>
+      </c>
+      <c r="M31" s="25">
+        <v>377.9994977272724</v>
+      </c>
+      <c r="N31" s="25">
+        <v>390.49356363636321</v>
+      </c>
+      <c r="O31" s="25">
+        <v>390.96323863636326</v>
+      </c>
+      <c r="P31" s="25">
+        <v>383.94589090909062</v>
+      </c>
+      <c r="Q31" s="25">
+        <v>367.18801590909106</v>
+      </c>
+      <c r="R31" s="25">
+        <v>339.10874772727254</v>
+      </c>
+      <c r="S31" s="31">
+        <v>309.0274340909092</v>
+      </c>
+      <c r="T31" s="66"/>
+      <c r="U31" s="66"/>
+      <c r="V31" s="66"/>
+      <c r="W31" s="66"/>
+      <c r="X31" s="66"/>
+      <c r="Y31" s="66"/>
+      <c r="Z31" s="66"/>
+      <c r="AA31" s="66"/>
+      <c r="AB31" s="66"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="27">
+        <v>36.451713933881166</v>
+      </c>
+      <c r="C32" s="27">
+        <v>47.177797181469195</v>
+      </c>
+      <c r="D32" s="27">
+        <v>50.9208102835942</v>
+      </c>
+      <c r="E32" s="27">
+        <v>58.416872448040543</v>
+      </c>
+      <c r="F32" s="27">
+        <v>56.185737627591806</v>
+      </c>
+      <c r="G32" s="27">
+        <v>52.394869335882682</v>
+      </c>
+      <c r="H32" s="27">
+        <v>46.89534594956605</v>
+      </c>
+      <c r="I32" s="27">
+        <v>39.667690356168933</v>
+      </c>
+      <c r="J32" s="27">
+        <v>28.713533034053118</v>
+      </c>
+      <c r="K32" s="28">
+        <v>37.574008579085877</v>
+      </c>
+      <c r="L32" s="28">
+        <v>46.266936031737892</v>
+      </c>
+      <c r="M32" s="28">
+        <v>50.929137278183774</v>
+      </c>
+      <c r="N32" s="28">
+        <v>54.858247893346217</v>
+      </c>
+      <c r="O32" s="28">
+        <v>56.453732220644866</v>
+      </c>
+      <c r="P32" s="28">
+        <v>53.737555424824095</v>
+      </c>
+      <c r="Q32" s="28">
+        <v>48.309033102095938</v>
+      </c>
+      <c r="R32" s="28">
+        <v>37.665705170107216</v>
+      </c>
+      <c r="S32" s="32">
+        <v>29.222638006118618</v>
+      </c>
+      <c r="T32" s="66"/>
+      <c r="U32" s="66"/>
+      <c r="V32" s="66"/>
+      <c r="W32" s="66"/>
+      <c r="X32" s="66"/>
+      <c r="Y32" s="66"/>
+      <c r="Z32" s="66"/>
+      <c r="AA32" s="66"/>
+      <c r="AB32" s="66"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="27">
+        <v>257.87700000000001</v>
+      </c>
+      <c r="C33" s="27">
+        <v>250.05799999999999</v>
+      </c>
+      <c r="D33" s="27">
+        <v>265.73500000000001</v>
+      </c>
+      <c r="E33" s="27">
+        <v>289.08800000000002</v>
+      </c>
+      <c r="F33" s="27">
+        <v>264.65699999999998</v>
+      </c>
+      <c r="G33" s="27">
+        <v>281.52300000000002</v>
+      </c>
+      <c r="H33" s="27">
+        <v>266.75400000000002</v>
+      </c>
+      <c r="I33" s="27">
+        <v>265.916</v>
+      </c>
+      <c r="J33" s="27">
+        <v>243.797</v>
+      </c>
+      <c r="K33" s="28">
+        <v>250.75299999999999</v>
+      </c>
+      <c r="L33" s="28">
+        <v>262.41899999999998</v>
+      </c>
+      <c r="M33" s="28">
+        <v>250.91200000000001</v>
+      </c>
+      <c r="N33" s="28">
+        <v>281.51</v>
+      </c>
+      <c r="O33" s="28">
+        <v>271.54399999999998</v>
+      </c>
+      <c r="P33" s="28">
+        <v>272.51499999999999</v>
+      </c>
+      <c r="Q33" s="28">
+        <v>268.45</v>
+      </c>
+      <c r="R33" s="28">
+        <v>255.44300000000001</v>
+      </c>
+      <c r="S33" s="32">
+        <v>238.083</v>
+      </c>
+      <c r="T33" s="66"/>
+      <c r="U33" s="66"/>
+      <c r="V33" s="66"/>
+      <c r="W33" s="66"/>
+      <c r="X33" s="66"/>
+      <c r="Y33" s="66"/>
+      <c r="Z33" s="66"/>
+      <c r="AA33" s="66"/>
+      <c r="AB33" s="66"/>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="27">
+        <v>506.17200000000003</v>
+      </c>
+      <c r="C34" s="27">
+        <v>592.69200000000001</v>
+      </c>
+      <c r="D34" s="27">
+        <v>593.279</v>
+      </c>
+      <c r="E34" s="27">
+        <v>627.95500000000004</v>
+      </c>
+      <c r="F34" s="27">
+        <v>631.38300000000004</v>
+      </c>
+      <c r="G34" s="27">
+        <v>600.91999999999996</v>
+      </c>
+      <c r="H34" s="27">
+        <v>565.99800000000005</v>
+      </c>
+      <c r="I34" s="27">
+        <v>480.00299999999999</v>
+      </c>
+      <c r="J34" s="27">
+        <v>420.14299999999997</v>
+      </c>
+      <c r="K34" s="28">
+        <v>530.36400000000003</v>
+      </c>
+      <c r="L34" s="28">
+        <v>585.13599999999997</v>
+      </c>
+      <c r="M34" s="28">
+        <v>566.024</v>
+      </c>
+      <c r="N34" s="28">
+        <v>612.51400000000001</v>
+      </c>
+      <c r="O34" s="28">
+        <v>623.74199999999996</v>
+      </c>
+      <c r="P34" s="28">
+        <v>599.24</v>
+      </c>
+      <c r="Q34" s="28">
+        <v>562.33000000000004</v>
+      </c>
+      <c r="R34" s="28">
+        <v>505.47500000000002</v>
+      </c>
+      <c r="S34" s="32">
+        <v>427.13</v>
+      </c>
+      <c r="T34" s="66"/>
+      <c r="U34" s="66"/>
+      <c r="V34" s="66"/>
+      <c r="W34" s="66"/>
+      <c r="X34" s="66"/>
+      <c r="Y34" s="66"/>
+      <c r="Z34" s="66"/>
+      <c r="AA34" s="66"/>
+      <c r="AB34" s="66"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="29"/>
+      <c r="R35" s="29"/>
+      <c r="S35" s="33"/>
+      <c r="T35" s="67"/>
+      <c r="U35" s="67"/>
+      <c r="V35" s="67"/>
+      <c r="W35" s="67"/>
+      <c r="X35" s="67"/>
+      <c r="Y35" s="67"/>
+      <c r="Z35" s="67"/>
+      <c r="AA35" s="67"/>
+      <c r="AB35" s="67"/>
+    </row>
+    <row r="36" spans="1:28" ht="21" x14ac:dyDescent="0.4">
+      <c r="A36" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="55">
+        <v>15</v>
+      </c>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="55"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="56"/>
+      <c r="T36" s="65"/>
+      <c r="U36" s="65"/>
+      <c r="V36" s="65"/>
+      <c r="W36" s="65"/>
+      <c r="X36" s="65"/>
+      <c r="Y36" s="65"/>
+      <c r="Z36" s="65"/>
+      <c r="AA36" s="65"/>
+      <c r="AB36" s="65"/>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="52"/>
+      <c r="O37" s="52"/>
+      <c r="P37" s="52"/>
+      <c r="Q37" s="52"/>
+      <c r="R37" s="52"/>
+      <c r="S37" s="53"/>
+      <c r="T37" s="66"/>
+      <c r="U37" s="66"/>
+      <c r="V37" s="66"/>
+      <c r="W37" s="66"/>
+      <c r="X37" s="66"/>
+      <c r="Y37" s="66"/>
+      <c r="Z37" s="66"/>
+      <c r="AA37" s="66"/>
+      <c r="AB37" s="66"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="22">
+        <v>8</v>
+      </c>
+      <c r="C38" s="22">
+        <v>9</v>
+      </c>
+      <c r="D38" s="22">
+        <v>10</v>
+      </c>
+      <c r="E38" s="22">
+        <v>11</v>
+      </c>
+      <c r="F38" s="22">
+        <v>12</v>
+      </c>
+      <c r="G38" s="22">
+        <v>13</v>
+      </c>
+      <c r="H38" s="22">
+        <v>14</v>
+      </c>
+      <c r="I38" s="22">
+        <v>15</v>
+      </c>
+      <c r="J38" s="22">
+        <v>16</v>
+      </c>
+      <c r="K38" s="23">
+        <v>8</v>
+      </c>
+      <c r="L38" s="23">
+        <v>9</v>
+      </c>
+      <c r="M38" s="23">
+        <v>10</v>
+      </c>
+      <c r="N38" s="23">
+        <v>11</v>
+      </c>
+      <c r="O38" s="23">
+        <v>12</v>
+      </c>
+      <c r="P38" s="23">
+        <v>13</v>
+      </c>
+      <c r="Q38" s="23">
+        <v>14</v>
+      </c>
+      <c r="R38" s="23">
+        <v>15</v>
+      </c>
+      <c r="S38" s="30">
+        <v>16</v>
+      </c>
+      <c r="T38" s="66"/>
+      <c r="U38" s="66"/>
+      <c r="V38" s="66"/>
+      <c r="W38" s="66"/>
+      <c r="X38" s="66"/>
+      <c r="Y38" s="66"/>
+      <c r="Z38" s="66"/>
+      <c r="AA38" s="66"/>
+      <c r="AB38" s="66"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="24">
+        <v>430.31132272727268</v>
+      </c>
+      <c r="C39" s="24">
+        <v>457.45759090909041</v>
+      </c>
+      <c r="D39" s="24">
+        <v>475.49808181818219</v>
+      </c>
+      <c r="E39" s="24">
+        <v>487.55087272727235</v>
+      </c>
+      <c r="F39" s="24">
+        <v>487.94480227272732</v>
+      </c>
+      <c r="G39" s="24">
+        <v>481.53907272727236</v>
+      </c>
+      <c r="H39" s="24">
+        <v>462.52495454545459</v>
+      </c>
+      <c r="I39" s="24">
+        <v>435.45125227272717</v>
+      </c>
+      <c r="J39" s="24">
+        <v>404.72012954545465</v>
+      </c>
+      <c r="K39" s="25">
+        <v>429.76478181818231</v>
+      </c>
+      <c r="L39" s="25">
+        <v>456.90946590909152</v>
+      </c>
+      <c r="M39" s="25">
+        <v>477.00306136363639</v>
+      </c>
+      <c r="N39" s="25">
+        <v>489.00567272727295</v>
+      </c>
+      <c r="O39" s="25">
+        <v>492.62599318181793</v>
+      </c>
+      <c r="P39" s="25">
+        <v>479.49771818181807</v>
+      </c>
+      <c r="Q39" s="25">
+        <v>462.92050454545421</v>
+      </c>
+      <c r="R39" s="25">
+        <v>437.90932045454491</v>
+      </c>
+      <c r="S39" s="31">
+        <v>403.40456818181798</v>
+      </c>
+      <c r="T39" s="66"/>
+      <c r="U39" s="66"/>
+      <c r="V39" s="66"/>
+      <c r="W39" s="66"/>
+      <c r="X39" s="66"/>
+      <c r="Y39" s="66"/>
+      <c r="Z39" s="66"/>
+      <c r="AA39" s="66"/>
+      <c r="AB39" s="66"/>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="27">
+        <v>36.205490784143038</v>
+      </c>
+      <c r="C40" s="27">
+        <v>42.774357445927663</v>
+      </c>
+      <c r="D40" s="27">
+        <v>47.720595678886184</v>
+      </c>
+      <c r="E40" s="27">
+        <v>51.094139370939324</v>
+      </c>
+      <c r="F40" s="27">
+        <v>49.725492735560174</v>
+      </c>
+      <c r="G40" s="27">
+        <v>45.798762428537145</v>
+      </c>
+      <c r="H40" s="27">
+        <v>42.874676013255943</v>
+      </c>
+      <c r="I40" s="27">
+        <v>36.123447915960689</v>
+      </c>
+      <c r="J40" s="27">
+        <v>31.853859096052979</v>
+      </c>
+      <c r="K40" s="28">
+        <v>35.395249682598923</v>
+      </c>
+      <c r="L40" s="28">
+        <v>41.164076449049176</v>
+      </c>
+      <c r="M40" s="28">
+        <v>47.952080866042422</v>
+      </c>
+      <c r="N40" s="28">
+        <v>49.983987503077692</v>
+      </c>
+      <c r="O40" s="28">
+        <v>49.124688548166809</v>
+      </c>
+      <c r="P40" s="28">
+        <v>46.728156416104873</v>
+      </c>
+      <c r="Q40" s="28">
+        <v>42.227022990633145</v>
+      </c>
+      <c r="R40" s="28">
+        <v>37.387097592503473</v>
+      </c>
+      <c r="S40" s="32">
+        <v>31.702348627164156</v>
+      </c>
+      <c r="T40" s="66"/>
+      <c r="U40" s="66"/>
+      <c r="V40" s="66"/>
+      <c r="W40" s="66"/>
+      <c r="X40" s="66"/>
+      <c r="Y40" s="66"/>
+      <c r="Z40" s="66"/>
+      <c r="AA40" s="66"/>
+      <c r="AB40" s="66"/>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="27">
+        <v>326.577</v>
+      </c>
+      <c r="C41" s="27">
+        <v>364.68799999999999</v>
+      </c>
+      <c r="D41" s="27">
+        <v>357.45499999999998</v>
+      </c>
+      <c r="E41" s="27">
+        <v>386.07400000000001</v>
+      </c>
+      <c r="F41" s="27">
+        <v>362.21300000000002</v>
+      </c>
+      <c r="G41" s="27">
+        <v>378.99900000000002</v>
+      </c>
+      <c r="H41" s="27">
+        <v>334.87</v>
+      </c>
+      <c r="I41" s="27">
+        <v>352.03300000000002</v>
+      </c>
+      <c r="J41" s="27">
+        <v>320.779</v>
+      </c>
+      <c r="K41" s="28">
+        <v>325.95699999999999</v>
+      </c>
+      <c r="L41" s="28">
+        <v>345.73</v>
+      </c>
+      <c r="M41" s="28">
+        <v>356.21699999999998</v>
+      </c>
+      <c r="N41" s="28">
+        <v>374.60199999999998</v>
+      </c>
+      <c r="O41" s="28">
+        <v>374.00099999999998</v>
+      </c>
+      <c r="P41" s="28">
+        <v>372.81400000000002</v>
+      </c>
+      <c r="Q41" s="28">
+        <v>367.37700000000001</v>
+      </c>
+      <c r="R41" s="28">
+        <v>336.15199999999999</v>
+      </c>
+      <c r="S41" s="32">
+        <v>321.42500000000001</v>
+      </c>
+      <c r="T41" s="66"/>
+      <c r="U41" s="66"/>
+      <c r="V41" s="66"/>
+      <c r="W41" s="66"/>
+      <c r="X41" s="66"/>
+      <c r="Y41" s="66"/>
+      <c r="Z41" s="66"/>
+      <c r="AA41" s="66"/>
+      <c r="AB41" s="66"/>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="27">
+        <v>531.42600000000004</v>
+      </c>
+      <c r="C42" s="27">
+        <v>620.40800000000002</v>
+      </c>
+      <c r="D42" s="27">
+        <v>647.79700000000003</v>
+      </c>
+      <c r="E42" s="27">
+        <v>697.875</v>
+      </c>
+      <c r="F42" s="27">
+        <v>693.87900000000002</v>
+      </c>
+      <c r="G42" s="27">
+        <v>657.38</v>
+      </c>
+      <c r="H42" s="27">
+        <v>615.39099999999996</v>
+      </c>
+      <c r="I42" s="27">
+        <v>581.68700000000001</v>
+      </c>
+      <c r="J42" s="27">
+        <v>494.11799999999999</v>
+      </c>
+      <c r="K42" s="28">
+        <v>559.851</v>
+      </c>
+      <c r="L42" s="28">
+        <v>620.60500000000002</v>
+      </c>
+      <c r="M42" s="28">
+        <v>649.15499999999997</v>
+      </c>
+      <c r="N42" s="28">
+        <v>699.12199999999996</v>
+      </c>
+      <c r="O42" s="28">
+        <v>693.07399999999996</v>
+      </c>
+      <c r="P42" s="28">
+        <v>654.45299999999997</v>
+      </c>
+      <c r="Q42" s="28">
+        <v>631.41499999999996</v>
+      </c>
+      <c r="R42" s="28">
+        <v>553.53399999999999</v>
+      </c>
+      <c r="S42" s="32">
+        <v>483.89400000000001</v>
+      </c>
+      <c r="T42" s="66"/>
+      <c r="U42" s="66"/>
+      <c r="V42" s="66"/>
+      <c r="W42" s="66"/>
+      <c r="X42" s="66"/>
+      <c r="Y42" s="66"/>
+      <c r="Z42" s="66"/>
+      <c r="AA42" s="66"/>
+      <c r="AB42" s="66"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="33"/>
+      <c r="T43" s="67"/>
+      <c r="U43" s="67"/>
+      <c r="V43" s="67"/>
+      <c r="W43" s="67"/>
+      <c r="X43" s="67"/>
+      <c r="Y43" s="67"/>
+      <c r="Z43" s="67"/>
+      <c r="AA43" s="67"/>
+      <c r="AB43" s="67"/>
+    </row>
+    <row r="44" spans="1:28" ht="21" x14ac:dyDescent="0.4">
+      <c r="A44" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="55">
+        <v>20</v>
+      </c>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="55"/>
+      <c r="N44" s="55"/>
+      <c r="O44" s="55"/>
+      <c r="P44" s="55"/>
+      <c r="Q44" s="55"/>
+      <c r="R44" s="55"/>
+      <c r="S44" s="56"/>
+      <c r="T44" s="65"/>
+      <c r="U44" s="65"/>
+      <c r="V44" s="65"/>
+      <c r="W44" s="65"/>
+      <c r="X44" s="65"/>
+      <c r="Y44" s="65"/>
+      <c r="Z44" s="65"/>
+      <c r="AA44" s="65"/>
+      <c r="AB44" s="65"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="L45" s="52"/>
+      <c r="M45" s="52"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="52"/>
+      <c r="P45" s="52"/>
+      <c r="Q45" s="52"/>
+      <c r="R45" s="52"/>
+      <c r="S45" s="53"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="22">
+        <v>8</v>
+      </c>
+      <c r="C46" s="22">
+        <v>9</v>
+      </c>
+      <c r="D46" s="22">
+        <v>10</v>
+      </c>
+      <c r="E46" s="22">
+        <v>11</v>
+      </c>
+      <c r="F46" s="22">
+        <v>12</v>
+      </c>
+      <c r="G46" s="22">
+        <v>13</v>
+      </c>
+      <c r="H46" s="22">
+        <v>14</v>
+      </c>
+      <c r="I46" s="22">
+        <v>15</v>
+      </c>
+      <c r="J46" s="22">
+        <v>16</v>
+      </c>
+      <c r="K46" s="23">
+        <v>8</v>
+      </c>
+      <c r="L46" s="23">
+        <v>9</v>
+      </c>
+      <c r="M46" s="23">
+        <v>10</v>
+      </c>
+      <c r="N46" s="23">
+        <v>11</v>
+      </c>
+      <c r="O46" s="23">
+        <v>12</v>
+      </c>
+      <c r="P46" s="23">
+        <v>13</v>
+      </c>
+      <c r="Q46" s="23">
+        <v>14</v>
+      </c>
+      <c r="R46" s="23">
+        <v>15</v>
+      </c>
+      <c r="S46" s="30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="24">
+        <v>525.08316590909112</v>
+      </c>
+      <c r="C47" s="24">
+        <v>550.89456136363663</v>
+      </c>
+      <c r="D47" s="24">
+        <v>570.02955000000065</v>
+      </c>
+      <c r="E47" s="24">
+        <v>583.95627954545466</v>
+      </c>
+      <c r="F47" s="24">
+        <v>583.97686363636376</v>
+      </c>
+      <c r="G47" s="24">
+        <v>575.84795681818218</v>
+      </c>
+      <c r="H47" s="24">
+        <v>555.57507727272719</v>
+      </c>
+      <c r="I47" s="24">
+        <v>533.62614090909028</v>
+      </c>
+      <c r="J47" s="24">
+        <v>501.4881386363636</v>
+      </c>
+      <c r="K47" s="25">
+        <v>526.51852727272683</v>
+      </c>
+      <c r="L47" s="25">
+        <v>554.20766818181778</v>
+      </c>
+      <c r="M47" s="25">
+        <v>571.63085681818188</v>
+      </c>
+      <c r="N47" s="25">
+        <v>584.10781136363642</v>
+      </c>
+      <c r="O47" s="25">
+        <v>585.27269545454544</v>
+      </c>
+      <c r="P47" s="25">
+        <v>573.8878590909095</v>
+      </c>
+      <c r="Q47" s="25">
+        <v>559.39101818181814</v>
+      </c>
+      <c r="R47" s="25">
+        <v>533.08956590909099</v>
+      </c>
+      <c r="S47" s="31">
+        <v>501.68265227272741</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="27">
+        <v>42.841827471685214</v>
+      </c>
+      <c r="C48" s="27">
+        <v>43.64724354692423</v>
+      </c>
+      <c r="D48" s="27">
+        <v>47.505521723151709</v>
+      </c>
+      <c r="E48" s="27">
+        <v>46.835401130294287</v>
+      </c>
+      <c r="F48" s="27">
+        <v>50.394776589338434</v>
+      </c>
+      <c r="G48" s="27">
+        <v>49.370043437779614</v>
+      </c>
+      <c r="H48" s="27">
+        <v>45.033264878941281</v>
+      </c>
+      <c r="I48" s="27">
+        <v>42.036835137868621</v>
+      </c>
+      <c r="J48" s="27">
+        <v>43.128061692261724</v>
+      </c>
+      <c r="K48" s="28">
+        <v>42.467578464859017</v>
+      </c>
+      <c r="L48" s="28">
+        <v>42.605222473883401</v>
+      </c>
+      <c r="M48" s="28">
+        <v>49.273647230205079</v>
+      </c>
+      <c r="N48" s="28">
+        <v>47.167045314475871</v>
+      </c>
+      <c r="O48" s="28">
+        <v>49.952019896344623</v>
+      </c>
+      <c r="P48" s="28">
+        <v>47.896663809928675</v>
+      </c>
+      <c r="Q48" s="28">
+        <v>43.858293501621581</v>
+      </c>
+      <c r="R48" s="28">
+        <v>42.641309629465169</v>
+      </c>
+      <c r="S48" s="32">
+        <v>43.446098651920771</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="27">
+        <v>422.21600000000001</v>
+      </c>
+      <c r="C49" s="27">
+        <v>417.00700000000001</v>
+      </c>
+      <c r="D49" s="27">
+        <v>450.73700000000002</v>
+      </c>
+      <c r="E49" s="27">
+        <v>446.82799999999997</v>
+      </c>
+      <c r="F49" s="27">
+        <v>455.42899999999997</v>
+      </c>
+      <c r="G49" s="27">
+        <v>442.22800000000001</v>
+      </c>
+      <c r="H49" s="27">
+        <v>440.238</v>
+      </c>
+      <c r="I49" s="27">
+        <v>390.04300000000001</v>
+      </c>
+      <c r="J49" s="27">
+        <v>378.85899999999998</v>
+      </c>
+      <c r="K49" s="28">
+        <v>397.64699999999999</v>
+      </c>
+      <c r="L49" s="28">
+        <v>415.60500000000002</v>
+      </c>
+      <c r="M49" s="28">
+        <v>448.77800000000002</v>
+      </c>
+      <c r="N49" s="28">
+        <v>469.53399999999999</v>
+      </c>
+      <c r="O49" s="28">
+        <v>459.911</v>
+      </c>
+      <c r="P49" s="28">
+        <v>457.80099999999999</v>
+      </c>
+      <c r="Q49" s="28">
+        <v>449.935</v>
+      </c>
+      <c r="R49" s="28">
+        <v>412.78899999999999</v>
+      </c>
+      <c r="S49" s="32">
+        <v>374.73899999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="40">
+        <v>620.96</v>
+      </c>
+      <c r="C50" s="40">
+        <v>673.11300000000006</v>
+      </c>
+      <c r="D50" s="40">
+        <v>718.01400000000001</v>
+      </c>
+      <c r="E50" s="40">
+        <v>722.87099999999998</v>
+      </c>
+      <c r="F50" s="40">
+        <v>802.41200000000003</v>
+      </c>
+      <c r="G50" s="40">
+        <v>738.07799999999997</v>
+      </c>
+      <c r="H50" s="40">
+        <v>675.55399999999997</v>
+      </c>
+      <c r="I50" s="40">
+        <v>637.471</v>
+      </c>
+      <c r="J50" s="40">
+        <v>614.20100000000002</v>
+      </c>
+      <c r="K50" s="41">
+        <v>627.23299999999995</v>
+      </c>
+      <c r="L50" s="41">
+        <v>666.399</v>
+      </c>
+      <c r="M50" s="41">
+        <v>723.96900000000005</v>
+      </c>
+      <c r="N50" s="41">
+        <v>754.17700000000002</v>
+      </c>
+      <c r="O50" s="41">
+        <v>742.27499999999998</v>
+      </c>
+      <c r="P50" s="41">
+        <v>732.94100000000003</v>
+      </c>
+      <c r="Q50" s="41">
+        <v>690.452</v>
+      </c>
+      <c r="R50" s="41">
+        <v>644.50300000000004</v>
+      </c>
+      <c r="S50" s="42">
+        <v>601.95500000000004</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="23">
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="K45:S45"/>
+    <mergeCell ref="A27:S27"/>
+    <mergeCell ref="B28:S28"/>
+    <mergeCell ref="B36:S36"/>
+    <mergeCell ref="B44:S44"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="K37:S37"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="K29:S29"/>
+    <mergeCell ref="A1:AB1"/>
+    <mergeCell ref="B2:AB2"/>
+    <mergeCell ref="B18:AB18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="K19:S19"/>
+    <mergeCell ref="T19:AB19"/>
     <mergeCell ref="B10:AB10"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="K11:S11"/>
@@ -3068,8 +4942,8 @@
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="K3:S3"/>
     <mergeCell ref="T3:AB3"/>
-    <mergeCell ref="B2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dodanie wyników symulacji dla drugiej konfiguracji opraw oświetleniowych
</commit_message>
<xml_diff>
--- a/doc/projekt/Wyniki_symulacji/Symulacje_podsumowanie.xlsx
+++ b/doc/projekt/Wyniki_symulacji/Symulacje_podsumowanie.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="594" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="594" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BEZ OŚWIETLENIA" sheetId="2" r:id="rId1"/>
-    <sheet name="Z OŚWIETLENIEM" sheetId="3" r:id="rId2"/>
+    <sheet name="Z OŚWIETLENIEM_1" sheetId="3" r:id="rId2"/>
+    <sheet name="Z OŚWIETLENIEM_2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="10">
   <si>
     <t>Słonecznie</t>
   </si>
@@ -407,6 +408,12 @@
     <xf numFmtId="1" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -447,22 +454,16 @@
     <xf numFmtId="16" fontId="4" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="4" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -763,104 +764,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="49"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="53"/>
     </row>
     <row r="2" spans="1:28" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
-      <c r="B2" s="54">
+      <c r="B2" s="58">
         <v>43871</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="56"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="60"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="51" t="s">
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="52" t="s">
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="53"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="57"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1414,71 +1415,71 @@
     </row>
     <row r="13" spans="1:28" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="1"/>
-      <c r="B13" s="57">
+      <c r="B13" s="61">
         <v>43961</v>
       </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="58"/>
-      <c r="R13" s="58"/>
-      <c r="S13" s="58"/>
-      <c r="T13" s="58"/>
-      <c r="U13" s="58"/>
-      <c r="V13" s="58"/>
-      <c r="W13" s="58"/>
-      <c r="X13" s="58"/>
-      <c r="Y13" s="58"/>
-      <c r="Z13" s="58"/>
-      <c r="AA13" s="58"/>
-      <c r="AB13" s="59"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62"/>
+      <c r="T13" s="62"/>
+      <c r="U13" s="62"/>
+      <c r="V13" s="62"/>
+      <c r="W13" s="62"/>
+      <c r="X13" s="62"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="63"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="44" t="s">
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="44"/>
-      <c r="T14" s="45" t="s">
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="U14" s="45"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="45"/>
-      <c r="X14" s="45"/>
-      <c r="Y14" s="45"/>
-      <c r="Z14" s="45"/>
-      <c r="AA14" s="45"/>
-      <c r="AB14" s="46"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="49"/>
+      <c r="Z14" s="49"/>
+      <c r="AA14" s="49"/>
+      <c r="AB14" s="50"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -2050,7 +2051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Y46" sqref="Y46"/>
     </sheetView>
   </sheetViews>
@@ -2063,106 +2064,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="60">
+      <c r="A1" s="64">
         <v>43871</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="62"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="68"/>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="59">
         <v>10</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="56"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="60"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="51" t="s">
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="52" t="s">
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="53"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="57"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -2628,71 +2629,71 @@
       <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="59">
         <v>15</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="55"/>
-      <c r="S10" s="55"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="55"/>
-      <c r="V10" s="55"/>
-      <c r="W10" s="55"/>
-      <c r="X10" s="55"/>
-      <c r="Y10" s="55"/>
-      <c r="Z10" s="55"/>
-      <c r="AA10" s="55"/>
-      <c r="AB10" s="56"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="59"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="59"/>
+      <c r="W10" s="59"/>
+      <c r="X10" s="59"/>
+      <c r="Y10" s="59"/>
+      <c r="Z10" s="59"/>
+      <c r="AA10" s="59"/>
+      <c r="AB10" s="60"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="51" t="s">
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="51"/>
-      <c r="T11" s="52" t="s">
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="U11" s="52"/>
-      <c r="V11" s="52"/>
-      <c r="W11" s="52"/>
-      <c r="X11" s="52"/>
-      <c r="Y11" s="52"/>
-      <c r="Z11" s="52"/>
-      <c r="AA11" s="52"/>
-      <c r="AB11" s="53"/>
+      <c r="U11" s="56"/>
+      <c r="V11" s="56"/>
+      <c r="W11" s="56"/>
+      <c r="X11" s="56"/>
+      <c r="Y11" s="56"/>
+      <c r="Z11" s="56"/>
+      <c r="AA11" s="56"/>
+      <c r="AB11" s="57"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -3158,71 +3159,71 @@
       <c r="A18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="55">
+      <c r="B18" s="59">
         <v>20</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="55"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="55"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="55"/>
-      <c r="S18" s="55"/>
-      <c r="T18" s="55"/>
-      <c r="U18" s="55"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="55"/>
-      <c r="X18" s="55"/>
-      <c r="Y18" s="55"/>
-      <c r="Z18" s="55"/>
-      <c r="AA18" s="55"/>
-      <c r="AB18" s="56"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="59"/>
+      <c r="S18" s="59"/>
+      <c r="T18" s="59"/>
+      <c r="U18" s="59"/>
+      <c r="V18" s="59"/>
+      <c r="W18" s="59"/>
+      <c r="X18" s="59"/>
+      <c r="Y18" s="59"/>
+      <c r="Z18" s="59"/>
+      <c r="AA18" s="59"/>
+      <c r="AB18" s="60"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="51" t="s">
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="52" t="s">
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="55"/>
+      <c r="T19" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="U19" s="52"/>
-      <c r="V19" s="52"/>
-      <c r="W19" s="52"/>
-      <c r="X19" s="52"/>
-      <c r="Y19" s="52"/>
-      <c r="Z19" s="52"/>
-      <c r="AA19" s="52"/>
-      <c r="AB19" s="53"/>
+      <c r="U19" s="56"/>
+      <c r="V19" s="56"/>
+      <c r="W19" s="56"/>
+      <c r="X19" s="56"/>
+      <c r="Y19" s="56"/>
+      <c r="Z19" s="56"/>
+      <c r="AA19" s="56"/>
+      <c r="AB19" s="57"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -3656,104 +3657,104 @@
     </row>
     <row r="26" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A27" s="60">
+      <c r="A27" s="64">
         <v>43961</v>
       </c>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="63"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="63"/>
-      <c r="O27" s="63"/>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="63"/>
-      <c r="S27" s="68"/>
-      <c r="T27" s="64"/>
-      <c r="U27" s="64"/>
-      <c r="V27" s="64"/>
-      <c r="W27" s="64"/>
-      <c r="X27" s="64"/>
-      <c r="Y27" s="64"/>
-      <c r="Z27" s="64"/>
-      <c r="AA27" s="64"/>
-      <c r="AB27" s="64"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="66"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="43"/>
+      <c r="Y27" s="43"/>
+      <c r="Z27" s="43"/>
+      <c r="AA27" s="43"/>
+      <c r="AB27" s="43"/>
     </row>
     <row r="28" spans="1:28" ht="21" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="55">
+      <c r="B28" s="59">
         <v>10</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="56"/>
-      <c r="T28" s="65"/>
-      <c r="U28" s="65"/>
-      <c r="V28" s="65"/>
-      <c r="W28" s="65"/>
-      <c r="X28" s="65"/>
-      <c r="Y28" s="65"/>
-      <c r="Z28" s="65"/>
-      <c r="AA28" s="65"/>
-      <c r="AB28" s="65"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="59"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="60"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="44"/>
+      <c r="V28" s="44"/>
+      <c r="W28" s="44"/>
+      <c r="X28" s="44"/>
+      <c r="Y28" s="44"/>
+      <c r="Z28" s="44"/>
+      <c r="AA28" s="44"/>
+      <c r="AB28" s="44"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="52" t="s">
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="52"/>
-      <c r="O29" s="52"/>
-      <c r="P29" s="52"/>
-      <c r="Q29" s="52"/>
-      <c r="R29" s="52"/>
-      <c r="S29" s="53"/>
-      <c r="T29" s="66"/>
-      <c r="U29" s="66"/>
-      <c r="V29" s="66"/>
-      <c r="W29" s="66"/>
-      <c r="X29" s="66"/>
-      <c r="Y29" s="66"/>
-      <c r="Z29" s="66"/>
-      <c r="AA29" s="66"/>
-      <c r="AB29" s="66"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="57"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
+      <c r="W29" s="45"/>
+      <c r="X29" s="45"/>
+      <c r="Y29" s="45"/>
+      <c r="Z29" s="45"/>
+      <c r="AA29" s="45"/>
+      <c r="AB29" s="45"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -3813,15 +3814,15 @@
       <c r="S30" s="30">
         <v>16</v>
       </c>
-      <c r="T30" s="66"/>
-      <c r="U30" s="66"/>
-      <c r="V30" s="66"/>
-      <c r="W30" s="66"/>
-      <c r="X30" s="66"/>
-      <c r="Y30" s="66"/>
-      <c r="Z30" s="66"/>
-      <c r="AA30" s="66"/>
-      <c r="AB30" s="66"/>
+      <c r="T30" s="45"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="45"/>
+      <c r="W30" s="45"/>
+      <c r="X30" s="45"/>
+      <c r="Y30" s="45"/>
+      <c r="Z30" s="45"/>
+      <c r="AA30" s="45"/>
+      <c r="AB30" s="45"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -3881,15 +3882,15 @@
       <c r="S31" s="31">
         <v>309.0274340909092</v>
       </c>
-      <c r="T31" s="66"/>
-      <c r="U31" s="66"/>
-      <c r="V31" s="66"/>
-      <c r="W31" s="66"/>
-      <c r="X31" s="66"/>
-      <c r="Y31" s="66"/>
-      <c r="Z31" s="66"/>
-      <c r="AA31" s="66"/>
-      <c r="AB31" s="66"/>
+      <c r="T31" s="45"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="45"/>
+      <c r="W31" s="45"/>
+      <c r="X31" s="45"/>
+      <c r="Y31" s="45"/>
+      <c r="Z31" s="45"/>
+      <c r="AA31" s="45"/>
+      <c r="AB31" s="45"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -3949,15 +3950,15 @@
       <c r="S32" s="32">
         <v>29.222638006118618</v>
       </c>
-      <c r="T32" s="66"/>
-      <c r="U32" s="66"/>
-      <c r="V32" s="66"/>
-      <c r="W32" s="66"/>
-      <c r="X32" s="66"/>
-      <c r="Y32" s="66"/>
-      <c r="Z32" s="66"/>
-      <c r="AA32" s="66"/>
-      <c r="AB32" s="66"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="45"/>
+      <c r="Y32" s="45"/>
+      <c r="Z32" s="45"/>
+      <c r="AA32" s="45"/>
+      <c r="AB32" s="45"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -4017,15 +4018,15 @@
       <c r="S33" s="32">
         <v>238.083</v>
       </c>
-      <c r="T33" s="66"/>
-      <c r="U33" s="66"/>
-      <c r="V33" s="66"/>
-      <c r="W33" s="66"/>
-      <c r="X33" s="66"/>
-      <c r="Y33" s="66"/>
-      <c r="Z33" s="66"/>
-      <c r="AA33" s="66"/>
-      <c r="AB33" s="66"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="45"/>
+      <c r="W33" s="45"/>
+      <c r="X33" s="45"/>
+      <c r="Y33" s="45"/>
+      <c r="Z33" s="45"/>
+      <c r="AA33" s="45"/>
+      <c r="AB33" s="45"/>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
@@ -4085,15 +4086,15 @@
       <c r="S34" s="32">
         <v>427.13</v>
       </c>
-      <c r="T34" s="66"/>
-      <c r="U34" s="66"/>
-      <c r="V34" s="66"/>
-      <c r="W34" s="66"/>
-      <c r="X34" s="66"/>
-      <c r="Y34" s="66"/>
-      <c r="Z34" s="66"/>
-      <c r="AA34" s="66"/>
-      <c r="AB34" s="66"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="45"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="45"/>
+      <c r="AB34" s="45"/>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
@@ -4115,83 +4116,83 @@
       <c r="Q35" s="29"/>
       <c r="R35" s="29"/>
       <c r="S35" s="33"/>
-      <c r="T35" s="67"/>
-      <c r="U35" s="67"/>
-      <c r="V35" s="67"/>
-      <c r="W35" s="67"/>
-      <c r="X35" s="67"/>
-      <c r="Y35" s="67"/>
-      <c r="Z35" s="67"/>
-      <c r="AA35" s="67"/>
-      <c r="AB35" s="67"/>
+      <c r="T35" s="46"/>
+      <c r="U35" s="46"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="46"/>
+      <c r="X35" s="46"/>
+      <c r="Y35" s="46"/>
+      <c r="Z35" s="46"/>
+      <c r="AA35" s="46"/>
+      <c r="AB35" s="46"/>
     </row>
     <row r="36" spans="1:28" ht="21" x14ac:dyDescent="0.4">
       <c r="A36" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="55">
+      <c r="B36" s="59">
         <v>15</v>
       </c>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="55"/>
-      <c r="S36" s="56"/>
-      <c r="T36" s="65"/>
-      <c r="U36" s="65"/>
-      <c r="V36" s="65"/>
-      <c r="W36" s="65"/>
-      <c r="X36" s="65"/>
-      <c r="Y36" s="65"/>
-      <c r="Z36" s="65"/>
-      <c r="AA36" s="65"/>
-      <c r="AB36" s="65"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="59"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="59"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="59"/>
+      <c r="N36" s="59"/>
+      <c r="O36" s="59"/>
+      <c r="P36" s="59"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="59"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="44"/>
+      <c r="X36" s="44"/>
+      <c r="Y36" s="44"/>
+      <c r="Z36" s="44"/>
+      <c r="AA36" s="44"/>
+      <c r="AB36" s="44"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="51" t="s">
+      <c r="B37" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="52" t="s">
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="L37" s="52"/>
-      <c r="M37" s="52"/>
-      <c r="N37" s="52"/>
-      <c r="O37" s="52"/>
-      <c r="P37" s="52"/>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="52"/>
-      <c r="S37" s="53"/>
-      <c r="T37" s="66"/>
-      <c r="U37" s="66"/>
-      <c r="V37" s="66"/>
-      <c r="W37" s="66"/>
-      <c r="X37" s="66"/>
-      <c r="Y37" s="66"/>
-      <c r="Z37" s="66"/>
-      <c r="AA37" s="66"/>
-      <c r="AB37" s="66"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="56"/>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="56"/>
+      <c r="R37" s="56"/>
+      <c r="S37" s="57"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
+      <c r="AA37" s="45"/>
+      <c r="AB37" s="45"/>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
@@ -4251,15 +4252,15 @@
       <c r="S38" s="30">
         <v>16</v>
       </c>
-      <c r="T38" s="66"/>
-      <c r="U38" s="66"/>
-      <c r="V38" s="66"/>
-      <c r="W38" s="66"/>
-      <c r="X38" s="66"/>
-      <c r="Y38" s="66"/>
-      <c r="Z38" s="66"/>
-      <c r="AA38" s="66"/>
-      <c r="AB38" s="66"/>
+      <c r="T38" s="45"/>
+      <c r="U38" s="45"/>
+      <c r="V38" s="45"/>
+      <c r="W38" s="45"/>
+      <c r="X38" s="45"/>
+      <c r="Y38" s="45"/>
+      <c r="Z38" s="45"/>
+      <c r="AA38" s="45"/>
+      <c r="AB38" s="45"/>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
@@ -4319,15 +4320,15 @@
       <c r="S39" s="31">
         <v>403.40456818181798</v>
       </c>
-      <c r="T39" s="66"/>
-      <c r="U39" s="66"/>
-      <c r="V39" s="66"/>
-      <c r="W39" s="66"/>
-      <c r="X39" s="66"/>
-      <c r="Y39" s="66"/>
-      <c r="Z39" s="66"/>
-      <c r="AA39" s="66"/>
-      <c r="AB39" s="66"/>
+      <c r="T39" s="45"/>
+      <c r="U39" s="45"/>
+      <c r="V39" s="45"/>
+      <c r="W39" s="45"/>
+      <c r="X39" s="45"/>
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45"/>
+      <c r="AA39" s="45"/>
+      <c r="AB39" s="45"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
@@ -4387,15 +4388,15 @@
       <c r="S40" s="32">
         <v>31.702348627164156</v>
       </c>
-      <c r="T40" s="66"/>
-      <c r="U40" s="66"/>
-      <c r="V40" s="66"/>
-      <c r="W40" s="66"/>
-      <c r="X40" s="66"/>
-      <c r="Y40" s="66"/>
-      <c r="Z40" s="66"/>
-      <c r="AA40" s="66"/>
-      <c r="AB40" s="66"/>
+      <c r="T40" s="45"/>
+      <c r="U40" s="45"/>
+      <c r="V40" s="45"/>
+      <c r="W40" s="45"/>
+      <c r="X40" s="45"/>
+      <c r="Y40" s="45"/>
+      <c r="Z40" s="45"/>
+      <c r="AA40" s="45"/>
+      <c r="AB40" s="45"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
@@ -4455,15 +4456,15 @@
       <c r="S41" s="32">
         <v>321.42500000000001</v>
       </c>
-      <c r="T41" s="66"/>
-      <c r="U41" s="66"/>
-      <c r="V41" s="66"/>
-      <c r="W41" s="66"/>
-      <c r="X41" s="66"/>
-      <c r="Y41" s="66"/>
-      <c r="Z41" s="66"/>
-      <c r="AA41" s="66"/>
-      <c r="AB41" s="66"/>
+      <c r="T41" s="45"/>
+      <c r="U41" s="45"/>
+      <c r="V41" s="45"/>
+      <c r="W41" s="45"/>
+      <c r="X41" s="45"/>
+      <c r="Y41" s="45"/>
+      <c r="Z41" s="45"/>
+      <c r="AA41" s="45"/>
+      <c r="AB41" s="45"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
@@ -4523,15 +4524,15 @@
       <c r="S42" s="32">
         <v>483.89400000000001</v>
       </c>
-      <c r="T42" s="66"/>
-      <c r="U42" s="66"/>
-      <c r="V42" s="66"/>
-      <c r="W42" s="66"/>
-      <c r="X42" s="66"/>
-      <c r="Y42" s="66"/>
-      <c r="Z42" s="66"/>
-      <c r="AA42" s="66"/>
-      <c r="AB42" s="66"/>
+      <c r="T42" s="45"/>
+      <c r="U42" s="45"/>
+      <c r="V42" s="45"/>
+      <c r="W42" s="45"/>
+      <c r="X42" s="45"/>
+      <c r="Y42" s="45"/>
+      <c r="Z42" s="45"/>
+      <c r="AA42" s="45"/>
+      <c r="AB42" s="45"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
@@ -4553,74 +4554,74 @@
       <c r="Q43" s="29"/>
       <c r="R43" s="29"/>
       <c r="S43" s="33"/>
-      <c r="T43" s="67"/>
-      <c r="U43" s="67"/>
-      <c r="V43" s="67"/>
-      <c r="W43" s="67"/>
-      <c r="X43" s="67"/>
-      <c r="Y43" s="67"/>
-      <c r="Z43" s="67"/>
-      <c r="AA43" s="67"/>
-      <c r="AB43" s="67"/>
+      <c r="T43" s="46"/>
+      <c r="U43" s="46"/>
+      <c r="V43" s="46"/>
+      <c r="W43" s="46"/>
+      <c r="X43" s="46"/>
+      <c r="Y43" s="46"/>
+      <c r="Z43" s="46"/>
+      <c r="AA43" s="46"/>
+      <c r="AB43" s="46"/>
     </row>
     <row r="44" spans="1:28" ht="21" x14ac:dyDescent="0.4">
       <c r="A44" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="55">
+      <c r="B44" s="59">
         <v>20</v>
       </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="55"/>
-      <c r="M44" s="55"/>
-      <c r="N44" s="55"/>
-      <c r="O44" s="55"/>
-      <c r="P44" s="55"/>
-      <c r="Q44" s="55"/>
-      <c r="R44" s="55"/>
-      <c r="S44" s="56"/>
-      <c r="T44" s="65"/>
-      <c r="U44" s="65"/>
-      <c r="V44" s="65"/>
-      <c r="W44" s="65"/>
-      <c r="X44" s="65"/>
-      <c r="Y44" s="65"/>
-      <c r="Z44" s="65"/>
-      <c r="AA44" s="65"/>
-      <c r="AB44" s="65"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
+      <c r="L44" s="59"/>
+      <c r="M44" s="59"/>
+      <c r="N44" s="59"/>
+      <c r="O44" s="59"/>
+      <c r="P44" s="59"/>
+      <c r="Q44" s="59"/>
+      <c r="R44" s="59"/>
+      <c r="S44" s="60"/>
+      <c r="T44" s="44"/>
+      <c r="U44" s="44"/>
+      <c r="V44" s="44"/>
+      <c r="W44" s="44"/>
+      <c r="X44" s="44"/>
+      <c r="Y44" s="44"/>
+      <c r="Z44" s="44"/>
+      <c r="AA44" s="44"/>
+      <c r="AB44" s="44"/>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="B45" s="51" t="s">
+      <c r="B45" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="51"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="52" t="s">
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="L45" s="52"/>
-      <c r="M45" s="52"/>
-      <c r="N45" s="52"/>
-      <c r="O45" s="52"/>
-      <c r="P45" s="52"/>
-      <c r="Q45" s="52"/>
-      <c r="R45" s="52"/>
-      <c r="S45" s="53"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="O45" s="56"/>
+      <c r="P45" s="56"/>
+      <c r="Q45" s="56"/>
+      <c r="R45" s="56"/>
+      <c r="S45" s="57"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
@@ -4919,16 +4920,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B45:J45"/>
-    <mergeCell ref="K45:S45"/>
-    <mergeCell ref="A27:S27"/>
-    <mergeCell ref="B28:S28"/>
-    <mergeCell ref="B36:S36"/>
-    <mergeCell ref="B44:S44"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="K37:S37"/>
-    <mergeCell ref="B29:J29"/>
-    <mergeCell ref="K29:S29"/>
     <mergeCell ref="A1:AB1"/>
     <mergeCell ref="B2:AB2"/>
     <mergeCell ref="B18:AB18"/>
@@ -4942,6 +4933,2918 @@
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="K3:S3"/>
     <mergeCell ref="T3:AB3"/>
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="K45:S45"/>
+    <mergeCell ref="A27:S27"/>
+    <mergeCell ref="B28:S28"/>
+    <mergeCell ref="B36:S36"/>
+    <mergeCell ref="B44:S44"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="K37:S37"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="K29:S29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z38" sqref="Z38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="64">
+        <v>43871</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="68"/>
+    </row>
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="59">
+        <v>10</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="60"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="57"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="21">
+        <v>8</v>
+      </c>
+      <c r="C4" s="21">
+        <v>9</v>
+      </c>
+      <c r="D4" s="21">
+        <v>10</v>
+      </c>
+      <c r="E4" s="21">
+        <v>11</v>
+      </c>
+      <c r="F4" s="21">
+        <v>12</v>
+      </c>
+      <c r="G4" s="21">
+        <v>13</v>
+      </c>
+      <c r="H4" s="21">
+        <v>14</v>
+      </c>
+      <c r="I4" s="21">
+        <v>15</v>
+      </c>
+      <c r="J4" s="21">
+        <v>16</v>
+      </c>
+      <c r="K4" s="22">
+        <v>8</v>
+      </c>
+      <c r="L4" s="22">
+        <v>9</v>
+      </c>
+      <c r="M4" s="22">
+        <v>10</v>
+      </c>
+      <c r="N4" s="22">
+        <v>11</v>
+      </c>
+      <c r="O4" s="22">
+        <v>12</v>
+      </c>
+      <c r="P4" s="22">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="22">
+        <v>14</v>
+      </c>
+      <c r="R4" s="22">
+        <v>15</v>
+      </c>
+      <c r="S4" s="22">
+        <v>16</v>
+      </c>
+      <c r="T4" s="23">
+        <v>8</v>
+      </c>
+      <c r="U4" s="23">
+        <v>9</v>
+      </c>
+      <c r="V4" s="23">
+        <v>10</v>
+      </c>
+      <c r="W4" s="23">
+        <v>11</v>
+      </c>
+      <c r="X4" s="23">
+        <v>12</v>
+      </c>
+      <c r="Y4" s="23">
+        <v>13</v>
+      </c>
+      <c r="Z4" s="23">
+        <v>14</v>
+      </c>
+      <c r="AA4" s="23">
+        <v>15</v>
+      </c>
+      <c r="AB4" s="30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10">
+        <v>511.24669090909111</v>
+      </c>
+      <c r="C5" s="10">
+        <v>434.53692954545477</v>
+      </c>
+      <c r="D5" s="10">
+        <v>460.09405909090913</v>
+      </c>
+      <c r="E5" s="10">
+        <v>535.81467272727252</v>
+      </c>
+      <c r="F5" s="10">
+        <v>623.10072954545444</v>
+      </c>
+      <c r="G5" s="10">
+        <v>672.91457045454592</v>
+      </c>
+      <c r="H5" s="10">
+        <v>2799.1284522727269</v>
+      </c>
+      <c r="I5" s="10">
+        <v>3108.1761386363655</v>
+      </c>
+      <c r="J5" s="10">
+        <v>591.01364090909101</v>
+      </c>
+      <c r="K5" s="24">
+        <v>507.46347045454507</v>
+      </c>
+      <c r="L5" s="24">
+        <v>438.13881363636386</v>
+      </c>
+      <c r="M5" s="24">
+        <v>460.09569999999951</v>
+      </c>
+      <c r="N5" s="24">
+        <v>531.24007272727317</v>
+      </c>
+      <c r="O5" s="24">
+        <v>621.36957499999971</v>
+      </c>
+      <c r="P5" s="24">
+        <v>671.15724318181844</v>
+      </c>
+      <c r="Q5" s="24">
+        <v>2801.3484363636339</v>
+      </c>
+      <c r="R5" s="24">
+        <v>3110.9478477272733</v>
+      </c>
+      <c r="S5" s="24">
+        <v>589.08129318181818</v>
+      </c>
+      <c r="T5" s="25">
+        <v>284.92667954545482</v>
+      </c>
+      <c r="U5" s="25">
+        <v>314.57305681818184</v>
+      </c>
+      <c r="V5" s="25">
+        <v>336.1092340909093</v>
+      </c>
+      <c r="W5" s="25">
+        <v>350.35633409090912</v>
+      </c>
+      <c r="X5" s="25">
+        <v>353.32548636363589</v>
+      </c>
+      <c r="Y5" s="25">
+        <v>348.45041590909102</v>
+      </c>
+      <c r="Z5" s="25">
+        <v>332.62960681818197</v>
+      </c>
+      <c r="AA5" s="25">
+        <v>310.04734090909096</v>
+      </c>
+      <c r="AB5" s="31">
+        <v>279.52842272727264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="26">
+        <v>310.60229782737372</v>
+      </c>
+      <c r="C6" s="26">
+        <v>47.392311616806538</v>
+      </c>
+      <c r="D6" s="26">
+        <v>39.964352454849717</v>
+      </c>
+      <c r="E6" s="26">
+        <v>43.638397029664354</v>
+      </c>
+      <c r="F6" s="26">
+        <v>62.147440693621782</v>
+      </c>
+      <c r="G6" s="26">
+        <v>83.260120503396735</v>
+      </c>
+      <c r="H6" s="26">
+        <v>3384.7714155306767</v>
+      </c>
+      <c r="I6" s="26">
+        <v>2235.0423606089626</v>
+      </c>
+      <c r="J6" s="26">
+        <v>330.35615354577067</v>
+      </c>
+      <c r="K6" s="27">
+        <v>311.1756852749466</v>
+      </c>
+      <c r="L6" s="27">
+        <v>49.54087755161904</v>
+      </c>
+      <c r="M6" s="27">
+        <v>40.938433190153866</v>
+      </c>
+      <c r="N6" s="27">
+        <v>44.048195236252397</v>
+      </c>
+      <c r="O6" s="27">
+        <v>60.846859061371887</v>
+      </c>
+      <c r="P6" s="27">
+        <v>85.093945356307628</v>
+      </c>
+      <c r="Q6" s="27">
+        <v>3387.9101732187551</v>
+      </c>
+      <c r="R6" s="27">
+        <v>2231.5414789391025</v>
+      </c>
+      <c r="S6" s="27">
+        <v>329.19271792211686</v>
+      </c>
+      <c r="T6" s="28">
+        <v>21.268747885551946</v>
+      </c>
+      <c r="U6" s="28">
+        <v>30.475401369727145</v>
+      </c>
+      <c r="V6" s="28">
+        <v>38.573443405138988</v>
+      </c>
+      <c r="W6" s="28">
+        <v>43.504335102865561</v>
+      </c>
+      <c r="X6" s="28">
+        <v>46.28859573369899</v>
+      </c>
+      <c r="Y6" s="28">
+        <v>42.714184973942849</v>
+      </c>
+      <c r="Z6" s="28">
+        <v>37.184106095244708</v>
+      </c>
+      <c r="AA6" s="28">
+        <v>28.785237568094267</v>
+      </c>
+      <c r="AB6" s="32">
+        <v>19.199178008420756</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="26">
+        <v>322.39</v>
+      </c>
+      <c r="C7" s="26">
+        <v>335.51600000000002</v>
+      </c>
+      <c r="D7" s="26">
+        <v>361.94299999999998</v>
+      </c>
+      <c r="E7" s="26">
+        <v>416.51299999999998</v>
+      </c>
+      <c r="F7" s="26">
+        <v>459.92500000000001</v>
+      </c>
+      <c r="G7" s="26">
+        <v>473.64800000000002</v>
+      </c>
+      <c r="H7" s="26">
+        <v>491.19499999999999</v>
+      </c>
+      <c r="I7" s="26">
+        <v>413.98899999999998</v>
+      </c>
+      <c r="J7" s="26">
+        <v>338.03500000000003</v>
+      </c>
+      <c r="K7" s="27">
+        <v>304.59899999999999</v>
+      </c>
+      <c r="L7" s="27">
+        <v>323.93200000000002</v>
+      </c>
+      <c r="M7" s="27">
+        <v>342.80500000000001</v>
+      </c>
+      <c r="N7" s="27">
+        <v>405.988</v>
+      </c>
+      <c r="O7" s="27">
+        <v>413.45800000000003</v>
+      </c>
+      <c r="P7" s="27">
+        <v>477.339</v>
+      </c>
+      <c r="Q7" s="27">
+        <v>483.57400000000001</v>
+      </c>
+      <c r="R7" s="27">
+        <v>430.245</v>
+      </c>
+      <c r="S7" s="27">
+        <v>356.87900000000002</v>
+      </c>
+      <c r="T7" s="28">
+        <v>239.57599999999999</v>
+      </c>
+      <c r="U7" s="28">
+        <v>262.32900000000001</v>
+      </c>
+      <c r="V7" s="28">
+        <v>262.79300000000001</v>
+      </c>
+      <c r="W7" s="28">
+        <v>273.77300000000002</v>
+      </c>
+      <c r="X7" s="28">
+        <v>276.30799999999999</v>
+      </c>
+      <c r="Y7" s="28">
+        <v>267.67500000000001</v>
+      </c>
+      <c r="Z7" s="28">
+        <v>268.31900000000002</v>
+      </c>
+      <c r="AA7" s="28">
+        <v>256.334</v>
+      </c>
+      <c r="AB7" s="32">
+        <v>245.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1642.615</v>
+      </c>
+      <c r="C8" s="26">
+        <v>586.60299999999995</v>
+      </c>
+      <c r="D8" s="26">
+        <v>571.62699999999995</v>
+      </c>
+      <c r="E8" s="26">
+        <v>708.68499999999995</v>
+      </c>
+      <c r="F8" s="26">
+        <v>846.56899999999996</v>
+      </c>
+      <c r="G8" s="26">
+        <v>929.1</v>
+      </c>
+      <c r="H8" s="26">
+        <v>8435.482</v>
+      </c>
+      <c r="I8" s="26">
+        <v>5281.1610000000001</v>
+      </c>
+      <c r="J8" s="26">
+        <v>1485.865</v>
+      </c>
+      <c r="K8" s="27">
+        <v>1731.027</v>
+      </c>
+      <c r="L8" s="27">
+        <v>614.50699999999995</v>
+      </c>
+      <c r="M8" s="27">
+        <v>598.072</v>
+      </c>
+      <c r="N8" s="27">
+        <v>672.47699999999998</v>
+      </c>
+      <c r="O8" s="27">
+        <v>820.89</v>
+      </c>
+      <c r="P8" s="27">
+        <v>944.66700000000003</v>
+      </c>
+      <c r="Q8" s="27">
+        <v>8443.0740000000005</v>
+      </c>
+      <c r="R8" s="27">
+        <v>5302.9960000000001</v>
+      </c>
+      <c r="S8" s="27">
+        <v>1479.0070000000001</v>
+      </c>
+      <c r="T8" s="28">
+        <v>336.02600000000001</v>
+      </c>
+      <c r="U8" s="28">
+        <v>404.71499999999997</v>
+      </c>
+      <c r="V8" s="28">
+        <v>446.72300000000001</v>
+      </c>
+      <c r="W8" s="28">
+        <v>504.06099999999998</v>
+      </c>
+      <c r="X8" s="28">
+        <v>504.839</v>
+      </c>
+      <c r="Y8" s="28">
+        <v>486.851</v>
+      </c>
+      <c r="Z8" s="28">
+        <v>453.51499999999999</v>
+      </c>
+      <c r="AA8" s="28">
+        <v>398.685</v>
+      </c>
+      <c r="AB8" s="32">
+        <v>325.09899999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="33"/>
+    </row>
+    <row r="10" spans="1:28" ht="21" x14ac:dyDescent="0.4">
+      <c r="A10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="59">
+        <v>15</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="59"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="59"/>
+      <c r="W10" s="59"/>
+      <c r="X10" s="59"/>
+      <c r="Y10" s="59"/>
+      <c r="Z10" s="59"/>
+      <c r="AA10" s="59"/>
+      <c r="AB10" s="60"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="U11" s="56"/>
+      <c r="V11" s="56"/>
+      <c r="W11" s="56"/>
+      <c r="X11" s="56"/>
+      <c r="Y11" s="56"/>
+      <c r="Z11" s="56"/>
+      <c r="AA11" s="56"/>
+      <c r="AB11" s="57"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="21">
+        <v>8</v>
+      </c>
+      <c r="C12" s="21">
+        <v>9</v>
+      </c>
+      <c r="D12" s="21">
+        <v>10</v>
+      </c>
+      <c r="E12" s="21">
+        <v>11</v>
+      </c>
+      <c r="F12" s="21">
+        <v>12</v>
+      </c>
+      <c r="G12" s="21">
+        <v>13</v>
+      </c>
+      <c r="H12" s="21">
+        <v>14</v>
+      </c>
+      <c r="I12" s="21">
+        <v>15</v>
+      </c>
+      <c r="J12" s="21">
+        <v>16</v>
+      </c>
+      <c r="K12" s="22">
+        <v>8</v>
+      </c>
+      <c r="L12" s="22">
+        <v>9</v>
+      </c>
+      <c r="M12" s="22">
+        <v>10</v>
+      </c>
+      <c r="N12" s="22">
+        <v>11</v>
+      </c>
+      <c r="O12" s="22">
+        <v>12</v>
+      </c>
+      <c r="P12" s="22">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="22">
+        <v>14</v>
+      </c>
+      <c r="R12" s="22">
+        <v>15</v>
+      </c>
+      <c r="S12" s="22">
+        <v>16</v>
+      </c>
+      <c r="T12" s="23">
+        <v>8</v>
+      </c>
+      <c r="U12" s="23">
+        <v>9</v>
+      </c>
+      <c r="V12" s="23">
+        <v>10</v>
+      </c>
+      <c r="W12" s="23">
+        <v>11</v>
+      </c>
+      <c r="X12" s="23">
+        <v>12</v>
+      </c>
+      <c r="Y12" s="23">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="23">
+        <v>14</v>
+      </c>
+      <c r="AA12" s="23">
+        <v>15</v>
+      </c>
+      <c r="AB12" s="30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="10">
+        <v>631.24065681818263</v>
+      </c>
+      <c r="C13" s="10">
+        <v>559.12979318181783</v>
+      </c>
+      <c r="D13" s="10">
+        <v>585.24224772727234</v>
+      </c>
+      <c r="E13" s="10">
+        <v>663.04679318181843</v>
+      </c>
+      <c r="F13" s="10">
+        <v>754.18356590909161</v>
+      </c>
+      <c r="G13" s="10">
+        <v>797.65533409090858</v>
+      </c>
+      <c r="H13" s="10">
+        <v>2926.450004545452</v>
+      </c>
+      <c r="I13" s="10">
+        <v>3235.0194318181821</v>
+      </c>
+      <c r="J13" s="10">
+        <v>718.55398863636378</v>
+      </c>
+      <c r="K13" s="24">
+        <v>411.2405499999997</v>
+      </c>
+      <c r="L13" s="24">
+        <v>440.77440909090922</v>
+      </c>
+      <c r="M13" s="24">
+        <v>462.57894318181809</v>
+      </c>
+      <c r="N13" s="24">
+        <v>475.44435681818175</v>
+      </c>
+      <c r="O13" s="24">
+        <v>481.47893409090887</v>
+      </c>
+      <c r="P13" s="24">
+        <v>475.12503636363664</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>459.86006363636329</v>
+      </c>
+      <c r="R13" s="24">
+        <v>435.26703409090942</v>
+      </c>
+      <c r="S13" s="24">
+        <v>406.15855454545436</v>
+      </c>
+      <c r="T13" s="25">
+        <v>411.53037727272755</v>
+      </c>
+      <c r="U13" s="25">
+        <v>440.69836363636318</v>
+      </c>
+      <c r="V13" s="25">
+        <v>464.62141363636357</v>
+      </c>
+      <c r="W13" s="25">
+        <v>477.2481227272728</v>
+      </c>
+      <c r="X13" s="25">
+        <v>480.10830454545442</v>
+      </c>
+      <c r="Y13" s="25">
+        <v>475.28654545454555</v>
+      </c>
+      <c r="Z13" s="25">
+        <v>459.64615000000003</v>
+      </c>
+      <c r="AA13" s="25">
+        <v>435.36286590909111</v>
+      </c>
+      <c r="AB13" s="31">
+        <v>405.96872954545415</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="26">
+        <v>308.6101358813022</v>
+      </c>
+      <c r="C14" s="26">
+        <v>49.829117223938809</v>
+      </c>
+      <c r="D14" s="26">
+        <v>45.0388050170315</v>
+      </c>
+      <c r="E14" s="26">
+        <v>53.601490765447132</v>
+      </c>
+      <c r="F14" s="26">
+        <v>62.300309906176764</v>
+      </c>
+      <c r="G14" s="26">
+        <v>89.319918570880262</v>
+      </c>
+      <c r="H14" s="26">
+        <v>3386.2343237499917</v>
+      </c>
+      <c r="I14" s="26">
+        <v>2229.2496638794055</v>
+      </c>
+      <c r="J14" s="26">
+        <v>324.44402199905977</v>
+      </c>
+      <c r="K14" s="27">
+        <v>27.372436876081746</v>
+      </c>
+      <c r="L14" s="27">
+        <v>34.943121051059293</v>
+      </c>
+      <c r="M14" s="27">
+        <v>42.738020632292304</v>
+      </c>
+      <c r="N14" s="27">
+        <v>47.540808054848263</v>
+      </c>
+      <c r="O14" s="27">
+        <v>47.948359462176569</v>
+      </c>
+      <c r="P14" s="27">
+        <v>46.779099078444531</v>
+      </c>
+      <c r="Q14" s="27">
+        <v>41.095023374279947</v>
+      </c>
+      <c r="R14" s="27">
+        <v>32.99968191074997</v>
+      </c>
+      <c r="S14" s="27">
+        <v>26.203909479429385</v>
+      </c>
+      <c r="T14" s="28">
+        <v>27.414406121864403</v>
+      </c>
+      <c r="U14" s="28">
+        <v>34.742558896916854</v>
+      </c>
+      <c r="V14" s="28">
+        <v>43.166234295663905</v>
+      </c>
+      <c r="W14" s="28">
+        <v>46.853016449506271</v>
+      </c>
+      <c r="X14" s="28">
+        <v>48.406974637272889</v>
+      </c>
+      <c r="Y14" s="28">
+        <v>46.768633904144444</v>
+      </c>
+      <c r="Z14" s="28">
+        <v>42.351340160815262</v>
+      </c>
+      <c r="AA14" s="28">
+        <v>34.627296376671289</v>
+      </c>
+      <c r="AB14" s="32">
+        <v>26.237542317766231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="26">
+        <v>435.005</v>
+      </c>
+      <c r="C15" s="26">
+        <v>438.47399999999999</v>
+      </c>
+      <c r="D15" s="26">
+        <v>477.721</v>
+      </c>
+      <c r="E15" s="26">
+        <v>535.38900000000001</v>
+      </c>
+      <c r="F15" s="26">
+        <v>604.48500000000001</v>
+      </c>
+      <c r="G15" s="26">
+        <v>585.78300000000002</v>
+      </c>
+      <c r="H15" s="26">
+        <v>586.72900000000004</v>
+      </c>
+      <c r="I15" s="26">
+        <v>534.34699999999998</v>
+      </c>
+      <c r="J15" s="26">
+        <v>451.17899999999997</v>
+      </c>
+      <c r="K15" s="27">
+        <v>353.23399999999998</v>
+      </c>
+      <c r="L15" s="27">
+        <v>384.58800000000002</v>
+      </c>
+      <c r="M15" s="27">
+        <v>387.68200000000002</v>
+      </c>
+      <c r="N15" s="27">
+        <v>388.52600000000001</v>
+      </c>
+      <c r="O15" s="27">
+        <v>392.572</v>
+      </c>
+      <c r="P15" s="27">
+        <v>391.78100000000001</v>
+      </c>
+      <c r="Q15" s="27">
+        <v>382.86399999999998</v>
+      </c>
+      <c r="R15" s="27">
+        <v>375.22</v>
+      </c>
+      <c r="S15" s="27">
+        <v>341.89600000000002</v>
+      </c>
+      <c r="T15" s="28">
+        <v>348.47500000000002</v>
+      </c>
+      <c r="U15" s="28">
+        <v>369.89400000000001</v>
+      </c>
+      <c r="V15" s="28">
+        <v>383.709</v>
+      </c>
+      <c r="W15" s="28">
+        <v>392.39299999999997</v>
+      </c>
+      <c r="X15" s="28">
+        <v>395.94099999999997</v>
+      </c>
+      <c r="Y15" s="28">
+        <v>396.24</v>
+      </c>
+      <c r="Z15" s="28">
+        <v>381.738</v>
+      </c>
+      <c r="AA15" s="28">
+        <v>374.25700000000001</v>
+      </c>
+      <c r="AB15" s="32">
+        <v>341.62700000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="26">
+        <v>1745.4739999999999</v>
+      </c>
+      <c r="C16" s="26">
+        <v>745.245</v>
+      </c>
+      <c r="D16" s="26">
+        <v>731.54</v>
+      </c>
+      <c r="E16" s="26">
+        <v>822.62199999999996</v>
+      </c>
+      <c r="F16" s="26">
+        <v>920.72799999999995</v>
+      </c>
+      <c r="G16" s="26">
+        <v>1069.3140000000001</v>
+      </c>
+      <c r="H16" s="26">
+        <v>8617.5220000000008</v>
+      </c>
+      <c r="I16" s="26">
+        <v>5429.8869999999997</v>
+      </c>
+      <c r="J16" s="26">
+        <v>1571.027</v>
+      </c>
+      <c r="K16" s="27">
+        <v>474.74</v>
+      </c>
+      <c r="L16" s="27">
+        <v>530.12099999999998</v>
+      </c>
+      <c r="M16" s="27">
+        <v>577.09900000000005</v>
+      </c>
+      <c r="N16" s="27">
+        <v>613.42499999999995</v>
+      </c>
+      <c r="O16" s="27">
+        <v>617.31399999999996</v>
+      </c>
+      <c r="P16" s="27">
+        <v>608.92999999999995</v>
+      </c>
+      <c r="Q16" s="27">
+        <v>585.55700000000002</v>
+      </c>
+      <c r="R16" s="27">
+        <v>516.07100000000003</v>
+      </c>
+      <c r="S16" s="27">
+        <v>465.91500000000002</v>
+      </c>
+      <c r="T16" s="28">
+        <v>478.01600000000002</v>
+      </c>
+      <c r="U16" s="28">
+        <v>530.42899999999997</v>
+      </c>
+      <c r="V16" s="28">
+        <v>593.09900000000005</v>
+      </c>
+      <c r="W16" s="28">
+        <v>619.32799999999997</v>
+      </c>
+      <c r="X16" s="28">
+        <v>629.61400000000003</v>
+      </c>
+      <c r="Y16" s="28">
+        <v>626.30999999999995</v>
+      </c>
+      <c r="Z16" s="28">
+        <v>601.50599999999997</v>
+      </c>
+      <c r="AA16" s="28">
+        <v>529.79899999999998</v>
+      </c>
+      <c r="AB16" s="32">
+        <v>468.44600000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="29"/>
+      <c r="AB17" s="33"/>
+    </row>
+    <row r="18" spans="1:28" ht="21" x14ac:dyDescent="0.4">
+      <c r="A18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="59">
+        <v>20</v>
+      </c>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="59"/>
+      <c r="S18" s="59"/>
+      <c r="T18" s="59"/>
+      <c r="U18" s="59"/>
+      <c r="V18" s="59"/>
+      <c r="W18" s="59"/>
+      <c r="X18" s="59"/>
+      <c r="Y18" s="59"/>
+      <c r="Z18" s="59"/>
+      <c r="AA18" s="59"/>
+      <c r="AB18" s="60"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="55"/>
+      <c r="T19" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="U19" s="56"/>
+      <c r="V19" s="56"/>
+      <c r="W19" s="56"/>
+      <c r="X19" s="56"/>
+      <c r="Y19" s="56"/>
+      <c r="Z19" s="56"/>
+      <c r="AA19" s="56"/>
+      <c r="AB19" s="57"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="21">
+        <v>8</v>
+      </c>
+      <c r="C20" s="21">
+        <v>9</v>
+      </c>
+      <c r="D20" s="21">
+        <v>10</v>
+      </c>
+      <c r="E20" s="21">
+        <v>11</v>
+      </c>
+      <c r="F20" s="21">
+        <v>12</v>
+      </c>
+      <c r="G20" s="21">
+        <v>13</v>
+      </c>
+      <c r="H20" s="21">
+        <v>14</v>
+      </c>
+      <c r="I20" s="21">
+        <v>15</v>
+      </c>
+      <c r="J20" s="21">
+        <v>16</v>
+      </c>
+      <c r="K20" s="22">
+        <v>8</v>
+      </c>
+      <c r="L20" s="22">
+        <v>9</v>
+      </c>
+      <c r="M20" s="22">
+        <v>10</v>
+      </c>
+      <c r="N20" s="22">
+        <v>11</v>
+      </c>
+      <c r="O20" s="22">
+        <v>12</v>
+      </c>
+      <c r="P20" s="22">
+        <v>13</v>
+      </c>
+      <c r="Q20" s="22">
+        <v>14</v>
+      </c>
+      <c r="R20" s="22">
+        <v>15</v>
+      </c>
+      <c r="S20" s="22">
+        <v>16</v>
+      </c>
+      <c r="T20" s="23">
+        <v>8</v>
+      </c>
+      <c r="U20" s="23">
+        <v>9</v>
+      </c>
+      <c r="V20" s="23">
+        <v>10</v>
+      </c>
+      <c r="W20" s="23">
+        <v>11</v>
+      </c>
+      <c r="X20" s="23">
+        <v>12</v>
+      </c>
+      <c r="Y20" s="23">
+        <v>13</v>
+      </c>
+      <c r="Z20" s="23">
+        <v>14</v>
+      </c>
+      <c r="AA20" s="23">
+        <v>15</v>
+      </c>
+      <c r="AB20" s="30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="10">
+        <v>758.91729772727228</v>
+      </c>
+      <c r="C21" s="10">
+        <v>683.70676136363647</v>
+      </c>
+      <c r="D21" s="10">
+        <v>713.31473409090927</v>
+      </c>
+      <c r="E21" s="10">
+        <v>789.00545909090931</v>
+      </c>
+      <c r="F21" s="10">
+        <v>874.16133863636367</v>
+      </c>
+      <c r="G21" s="10">
+        <v>927.01048636363635</v>
+      </c>
+      <c r="H21" s="10">
+        <v>3050.8289477272679</v>
+      </c>
+      <c r="I21" s="10">
+        <v>3358.5965613636372</v>
+      </c>
+      <c r="J21" s="10">
+        <v>843.34162500000002</v>
+      </c>
+      <c r="K21" s="24">
+        <v>560.63654090909131</v>
+      </c>
+      <c r="L21" s="24">
+        <v>579.4903636363631</v>
+      </c>
+      <c r="M21" s="24">
+        <v>614.19576590909094</v>
+      </c>
+      <c r="N21" s="24">
+        <v>649.96257727272791</v>
+      </c>
+      <c r="O21" s="24">
+        <v>685.15548181818235</v>
+      </c>
+      <c r="P21" s="24">
+        <v>699.39272500000004</v>
+      </c>
+      <c r="Q21" s="24">
+        <v>1004.9410568181816</v>
+      </c>
+      <c r="R21" s="24">
+        <v>1014.5408522727279</v>
+      </c>
+      <c r="S21" s="24">
+        <v>587.68363636363642</v>
+      </c>
+      <c r="T21" s="25">
+        <v>537.37855681818223</v>
+      </c>
+      <c r="U21" s="25">
+        <v>566.98949545454536</v>
+      </c>
+      <c r="V21" s="25">
+        <v>589.22972272727293</v>
+      </c>
+      <c r="W21" s="25">
+        <v>602.74228181818171</v>
+      </c>
+      <c r="X21" s="25">
+        <v>606.73766818181866</v>
+      </c>
+      <c r="Y21" s="25">
+        <v>600.78019772727271</v>
+      </c>
+      <c r="Z21" s="25">
+        <v>585.87507045454561</v>
+      </c>
+      <c r="AA21" s="25">
+        <v>562.53224545454543</v>
+      </c>
+      <c r="AB21" s="31">
+        <v>532.52038181818159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="26">
+        <v>305.09208271568724</v>
+      </c>
+      <c r="C22" s="26">
+        <v>53.131615874881433</v>
+      </c>
+      <c r="D22" s="26">
+        <v>49.900123578208451</v>
+      </c>
+      <c r="E22" s="26">
+        <v>50.698665497105431</v>
+      </c>
+      <c r="F22" s="26">
+        <v>65.399461113056816</v>
+      </c>
+      <c r="G22" s="26">
+        <v>88.754107169591506</v>
+      </c>
+      <c r="H22" s="26">
+        <v>3385.1155761642958</v>
+      </c>
+      <c r="I22" s="26">
+        <v>2230.996244291804</v>
+      </c>
+      <c r="J22" s="26">
+        <v>325.45226274100776</v>
+      </c>
+      <c r="K22" s="27">
+        <v>43.107869370941962</v>
+      </c>
+      <c r="L22" s="27">
+        <v>37.186780177534203</v>
+      </c>
+      <c r="M22" s="27">
+        <v>43.161110242435349</v>
+      </c>
+      <c r="N22" s="27">
+        <v>50.223989690408523</v>
+      </c>
+      <c r="O22" s="27">
+        <v>58.085709259915717</v>
+      </c>
+      <c r="P22" s="27">
+        <v>63.795888574113057</v>
+      </c>
+      <c r="Q22" s="27">
+        <v>531.90472606014316</v>
+      </c>
+      <c r="R22" s="27">
+        <v>321.32062576251911</v>
+      </c>
+      <c r="S22" s="27">
+        <v>48.869761698040584</v>
+      </c>
+      <c r="T22" s="28">
+        <v>33.814031631509401</v>
+      </c>
+      <c r="U22" s="28">
+        <v>40.76161100521297</v>
+      </c>
+      <c r="V22" s="28">
+        <v>47.338400540390992</v>
+      </c>
+      <c r="W22" s="28">
+        <v>53.306835373203455</v>
+      </c>
+      <c r="X22" s="28">
+        <v>53.289556586051049</v>
+      </c>
+      <c r="Y22" s="28">
+        <v>51.466354200462519</v>
+      </c>
+      <c r="Z22" s="28">
+        <v>47.175351343568202</v>
+      </c>
+      <c r="AA22" s="28">
+        <v>39.157470315119674</v>
+      </c>
+      <c r="AB22" s="32">
+        <v>32.943030782113624</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="26">
+        <v>544.36500000000001</v>
+      </c>
+      <c r="C23" s="26">
+        <v>558.40200000000004</v>
+      </c>
+      <c r="D23" s="26">
+        <v>593.96100000000001</v>
+      </c>
+      <c r="E23" s="26">
+        <v>671.13800000000003</v>
+      </c>
+      <c r="F23" s="26">
+        <v>725.73800000000006</v>
+      </c>
+      <c r="G23" s="26">
+        <v>727.31799999999998</v>
+      </c>
+      <c r="H23" s="26">
+        <v>718.64300000000003</v>
+      </c>
+      <c r="I23" s="26">
+        <v>682.26900000000001</v>
+      </c>
+      <c r="J23" s="26">
+        <v>564.58199999999999</v>
+      </c>
+      <c r="K23" s="27">
+        <v>495.61799999999999</v>
+      </c>
+      <c r="L23" s="27">
+        <v>491.75299999999999</v>
+      </c>
+      <c r="M23" s="27">
+        <v>519.30499999999995</v>
+      </c>
+      <c r="N23" s="27">
+        <v>548.06899999999996</v>
+      </c>
+      <c r="O23" s="27">
+        <v>553.66999999999996</v>
+      </c>
+      <c r="P23" s="27">
+        <v>554.19500000000005</v>
+      </c>
+      <c r="Q23" s="27">
+        <v>573.51400000000001</v>
+      </c>
+      <c r="R23" s="27">
+        <v>550.601</v>
+      </c>
+      <c r="S23" s="27">
+        <v>474.90899999999999</v>
+      </c>
+      <c r="T23" s="28">
+        <v>448.36</v>
+      </c>
+      <c r="U23" s="28">
+        <v>494.99200000000002</v>
+      </c>
+      <c r="V23" s="28">
+        <v>504.839</v>
+      </c>
+      <c r="W23" s="28">
+        <v>510.25299999999999</v>
+      </c>
+      <c r="X23" s="28">
+        <v>513.13</v>
+      </c>
+      <c r="Y23" s="28">
+        <v>515.15200000000004</v>
+      </c>
+      <c r="Z23" s="28">
+        <v>496.27199999999999</v>
+      </c>
+      <c r="AA23" s="28">
+        <v>489.22300000000001</v>
+      </c>
+      <c r="AB23" s="32">
+        <v>452.084</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="39">
+        <v>1868.3789999999999</v>
+      </c>
+      <c r="C24" s="39">
+        <v>882.92</v>
+      </c>
+      <c r="D24" s="39">
+        <v>846.26599999999996</v>
+      </c>
+      <c r="E24" s="39">
+        <v>937.57100000000003</v>
+      </c>
+      <c r="F24" s="39">
+        <v>1086.6379999999999</v>
+      </c>
+      <c r="G24" s="39">
+        <v>1182.604</v>
+      </c>
+      <c r="H24" s="39">
+        <v>8718.4779999999992</v>
+      </c>
+      <c r="I24" s="39">
+        <v>5624.0069999999996</v>
+      </c>
+      <c r="J24" s="39">
+        <v>1756.93</v>
+      </c>
+      <c r="K24" s="40">
+        <v>699.32100000000003</v>
+      </c>
+      <c r="L24" s="40">
+        <v>694.81500000000005</v>
+      </c>
+      <c r="M24" s="40">
+        <v>723.55700000000002</v>
+      </c>
+      <c r="N24" s="40">
+        <v>768.101</v>
+      </c>
+      <c r="O24" s="40">
+        <v>832.52200000000005</v>
+      </c>
+      <c r="P24" s="40">
+        <v>907.04</v>
+      </c>
+      <c r="Q24" s="40">
+        <v>1974.5139999999999</v>
+      </c>
+      <c r="R24" s="40">
+        <v>1387.0350000000001</v>
+      </c>
+      <c r="S24" s="40">
+        <v>694.63599999999997</v>
+      </c>
+      <c r="T24" s="41">
+        <v>614.39400000000001</v>
+      </c>
+      <c r="U24" s="41">
+        <v>668.72799999999995</v>
+      </c>
+      <c r="V24" s="41">
+        <v>715.13599999999997</v>
+      </c>
+      <c r="W24" s="41">
+        <v>751.52300000000002</v>
+      </c>
+      <c r="X24" s="41">
+        <v>754.54200000000003</v>
+      </c>
+      <c r="Y24" s="41">
+        <v>744.25800000000004</v>
+      </c>
+      <c r="Z24" s="41">
+        <v>709.92</v>
+      </c>
+      <c r="AA24" s="41">
+        <v>658.79899999999998</v>
+      </c>
+      <c r="AB24" s="42">
+        <v>608.72699999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A27" s="64">
+        <v>43961</v>
+      </c>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="66"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="43"/>
+      <c r="Y27" s="43"/>
+      <c r="Z27" s="43"/>
+      <c r="AA27" s="43"/>
+      <c r="AB27" s="43"/>
+    </row>
+    <row r="28" spans="1:28" ht="21" x14ac:dyDescent="0.4">
+      <c r="A28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="59">
+        <v>10</v>
+      </c>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="59"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="60"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="44"/>
+      <c r="V28" s="44"/>
+      <c r="W28" s="44"/>
+      <c r="X28" s="44"/>
+      <c r="Y28" s="44"/>
+      <c r="Z28" s="44"/>
+      <c r="AA28" s="44"/>
+      <c r="AB28" s="44"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="57"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
+      <c r="W29" s="45"/>
+      <c r="X29" s="45"/>
+      <c r="Y29" s="45"/>
+      <c r="Z29" s="45"/>
+      <c r="AA29" s="45"/>
+      <c r="AB29" s="45"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="22">
+        <v>8</v>
+      </c>
+      <c r="C30" s="22">
+        <v>9</v>
+      </c>
+      <c r="D30" s="22">
+        <v>10</v>
+      </c>
+      <c r="E30" s="22">
+        <v>11</v>
+      </c>
+      <c r="F30" s="22">
+        <v>12</v>
+      </c>
+      <c r="G30" s="22">
+        <v>13</v>
+      </c>
+      <c r="H30" s="22">
+        <v>14</v>
+      </c>
+      <c r="I30" s="22">
+        <v>15</v>
+      </c>
+      <c r="J30" s="22">
+        <v>16</v>
+      </c>
+      <c r="K30" s="23">
+        <v>8</v>
+      </c>
+      <c r="L30" s="23">
+        <v>9</v>
+      </c>
+      <c r="M30" s="23">
+        <v>10</v>
+      </c>
+      <c r="N30" s="23">
+        <v>11</v>
+      </c>
+      <c r="O30" s="23">
+        <v>12</v>
+      </c>
+      <c r="P30" s="23">
+        <v>13</v>
+      </c>
+      <c r="Q30" s="23">
+        <v>14</v>
+      </c>
+      <c r="R30" s="23">
+        <v>15</v>
+      </c>
+      <c r="S30" s="30">
+        <v>16</v>
+      </c>
+      <c r="T30" s="45"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="45"/>
+      <c r="W30" s="45"/>
+      <c r="X30" s="45"/>
+      <c r="Y30" s="45"/>
+      <c r="Z30" s="45"/>
+      <c r="AA30" s="45"/>
+      <c r="AB30" s="45"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="24">
+        <v>399.85653181818174</v>
+      </c>
+      <c r="C31" s="24">
+        <v>413.75467272727229</v>
+      </c>
+      <c r="D31" s="24">
+        <v>427.2872863636365</v>
+      </c>
+      <c r="E31" s="24">
+        <v>456.55902272727286</v>
+      </c>
+      <c r="F31" s="24">
+        <v>488.08003181818185</v>
+      </c>
+      <c r="G31" s="24">
+        <v>542.30265681818196</v>
+      </c>
+      <c r="H31" s="24">
+        <v>601.11076136363681</v>
+      </c>
+      <c r="I31" s="24">
+        <v>637.72959318181825</v>
+      </c>
+      <c r="J31" s="24">
+        <v>599.95063863636346</v>
+      </c>
+      <c r="K31" s="25">
+        <v>391.71292954545413</v>
+      </c>
+      <c r="L31" s="25">
+        <v>421.47221590909083</v>
+      </c>
+      <c r="M31" s="25">
+        <v>436.95577954545507</v>
+      </c>
+      <c r="N31" s="25">
+        <v>450.0440522727273</v>
+      </c>
+      <c r="O31" s="25">
+        <v>451.39815454545493</v>
+      </c>
+      <c r="P31" s="25">
+        <v>442.70457954545475</v>
+      </c>
+      <c r="Q31" s="25">
+        <v>425.90259090909109</v>
+      </c>
+      <c r="R31" s="25">
+        <v>400.57040000000006</v>
+      </c>
+      <c r="S31" s="31">
+        <v>368.3970295454551</v>
+      </c>
+      <c r="T31" s="45"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="45"/>
+      <c r="W31" s="45"/>
+      <c r="X31" s="45"/>
+      <c r="Y31" s="45"/>
+      <c r="Z31" s="45"/>
+      <c r="AA31" s="45"/>
+      <c r="AB31" s="45"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="27">
+        <v>41.934533304280095</v>
+      </c>
+      <c r="C32" s="27">
+        <v>43.855547026317154</v>
+      </c>
+      <c r="D32" s="27">
+        <v>41.131907478665845</v>
+      </c>
+      <c r="E32" s="27">
+        <v>45.513841929705471</v>
+      </c>
+      <c r="F32" s="27">
+        <v>57.26567802658208</v>
+      </c>
+      <c r="G32" s="27">
+        <v>79.68516177464015</v>
+      </c>
+      <c r="H32" s="27">
+        <v>104.44300225396198</v>
+      </c>
+      <c r="I32" s="27">
+        <v>122.88121754649266</v>
+      </c>
+      <c r="J32" s="27">
+        <v>118.45884156247124</v>
+      </c>
+      <c r="K32" s="28">
+        <v>60.198731650131357</v>
+      </c>
+      <c r="L32" s="28">
+        <v>71.753516194880774</v>
+      </c>
+      <c r="M32" s="28">
+        <v>76.636299973568455</v>
+      </c>
+      <c r="N32" s="28">
+        <v>82.256578354898394</v>
+      </c>
+      <c r="O32" s="28">
+        <v>82.32677985407868</v>
+      </c>
+      <c r="P32" s="28">
+        <v>78.672199180161314</v>
+      </c>
+      <c r="Q32" s="28">
+        <v>74.049574699310028</v>
+      </c>
+      <c r="R32" s="28">
+        <v>62.689922859653755</v>
+      </c>
+      <c r="S32" s="32">
+        <v>51.768312732167985</v>
+      </c>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="45"/>
+      <c r="Y32" s="45"/>
+      <c r="Z32" s="45"/>
+      <c r="AA32" s="45"/>
+      <c r="AB32" s="45"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="27">
+        <v>300.53800000000001</v>
+      </c>
+      <c r="C33" s="27">
+        <v>313.61799999999999</v>
+      </c>
+      <c r="D33" s="27">
+        <v>337.327</v>
+      </c>
+      <c r="E33" s="27">
+        <v>358.197</v>
+      </c>
+      <c r="F33" s="27">
+        <v>353.185</v>
+      </c>
+      <c r="G33" s="27">
+        <v>361.096</v>
+      </c>
+      <c r="H33" s="27">
+        <v>373.61399999999998</v>
+      </c>
+      <c r="I33" s="27">
+        <v>393.89400000000001</v>
+      </c>
+      <c r="J33" s="27">
+        <v>377.82900000000001</v>
+      </c>
+      <c r="K33" s="28">
+        <v>286.64499999999998</v>
+      </c>
+      <c r="L33" s="28">
+        <v>282.14100000000002</v>
+      </c>
+      <c r="M33" s="28">
+        <v>310.96600000000001</v>
+      </c>
+      <c r="N33" s="28">
+        <v>294.988</v>
+      </c>
+      <c r="O33" s="28">
+        <v>299.27699999999999</v>
+      </c>
+      <c r="P33" s="28">
+        <v>291.13099999999997</v>
+      </c>
+      <c r="Q33" s="28">
+        <v>284.52100000000002</v>
+      </c>
+      <c r="R33" s="28">
+        <v>286.75900000000001</v>
+      </c>
+      <c r="S33" s="32">
+        <v>275.29000000000002</v>
+      </c>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="45"/>
+      <c r="W33" s="45"/>
+      <c r="X33" s="45"/>
+      <c r="Y33" s="45"/>
+      <c r="Z33" s="45"/>
+      <c r="AA33" s="45"/>
+      <c r="AB33" s="45"/>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="27">
+        <v>547.95000000000005</v>
+      </c>
+      <c r="C34" s="27">
+        <v>567.58199999999999</v>
+      </c>
+      <c r="D34" s="27">
+        <v>542.07899999999995</v>
+      </c>
+      <c r="E34" s="27">
+        <v>581.36599999999999</v>
+      </c>
+      <c r="F34" s="27">
+        <v>707.75699999999995</v>
+      </c>
+      <c r="G34" s="27">
+        <v>799.476</v>
+      </c>
+      <c r="H34" s="27">
+        <v>959.93499999999995</v>
+      </c>
+      <c r="I34" s="27">
+        <v>1129.106</v>
+      </c>
+      <c r="J34" s="27">
+        <v>1006.123</v>
+      </c>
+      <c r="K34" s="28">
+        <v>591.58199999999999</v>
+      </c>
+      <c r="L34" s="28">
+        <v>664.37300000000005</v>
+      </c>
+      <c r="M34" s="28">
+        <v>681.17700000000002</v>
+      </c>
+      <c r="N34" s="28">
+        <v>691.41</v>
+      </c>
+      <c r="O34" s="28">
+        <v>716.18799999999999</v>
+      </c>
+      <c r="P34" s="28">
+        <v>695.09699999999998</v>
+      </c>
+      <c r="Q34" s="28">
+        <v>679.09900000000005</v>
+      </c>
+      <c r="R34" s="28">
+        <v>593.98299999999995</v>
+      </c>
+      <c r="S34" s="32">
+        <v>535.56799999999998</v>
+      </c>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="45"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="45"/>
+      <c r="AB34" s="45"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="29"/>
+      <c r="R35" s="29"/>
+      <c r="S35" s="33"/>
+      <c r="T35" s="46"/>
+      <c r="U35" s="46"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="46"/>
+      <c r="X35" s="46"/>
+      <c r="Y35" s="46"/>
+      <c r="Z35" s="46"/>
+      <c r="AA35" s="46"/>
+      <c r="AB35" s="46"/>
+    </row>
+    <row r="36" spans="1:28" ht="21" x14ac:dyDescent="0.4">
+      <c r="A36" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="59">
+        <v>15</v>
+      </c>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="59"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="59"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="59"/>
+      <c r="N36" s="59"/>
+      <c r="O36" s="59"/>
+      <c r="P36" s="59"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="59"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="44"/>
+      <c r="X36" s="44"/>
+      <c r="Y36" s="44"/>
+      <c r="Z36" s="44"/>
+      <c r="AA36" s="44"/>
+      <c r="AB36" s="44"/>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="56"/>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="56"/>
+      <c r="R37" s="56"/>
+      <c r="S37" s="57"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
+      <c r="AA37" s="45"/>
+      <c r="AB37" s="45"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="22">
+        <v>8</v>
+      </c>
+      <c r="C38" s="22">
+        <v>9</v>
+      </c>
+      <c r="D38" s="22">
+        <v>10</v>
+      </c>
+      <c r="E38" s="22">
+        <v>11</v>
+      </c>
+      <c r="F38" s="22">
+        <v>12</v>
+      </c>
+      <c r="G38" s="22">
+        <v>13</v>
+      </c>
+      <c r="H38" s="22">
+        <v>14</v>
+      </c>
+      <c r="I38" s="22">
+        <v>15</v>
+      </c>
+      <c r="J38" s="22">
+        <v>16</v>
+      </c>
+      <c r="K38" s="23">
+        <v>8</v>
+      </c>
+      <c r="L38" s="23">
+        <v>9</v>
+      </c>
+      <c r="M38" s="23">
+        <v>10</v>
+      </c>
+      <c r="N38" s="23">
+        <v>11</v>
+      </c>
+      <c r="O38" s="23">
+        <v>12</v>
+      </c>
+      <c r="P38" s="23">
+        <v>13</v>
+      </c>
+      <c r="Q38" s="23">
+        <v>14</v>
+      </c>
+      <c r="R38" s="23">
+        <v>15</v>
+      </c>
+      <c r="S38" s="30">
+        <v>16</v>
+      </c>
+      <c r="T38" s="45"/>
+      <c r="U38" s="45"/>
+      <c r="V38" s="45"/>
+      <c r="W38" s="45"/>
+      <c r="X38" s="45"/>
+      <c r="Y38" s="45"/>
+      <c r="Z38" s="45"/>
+      <c r="AA38" s="45"/>
+      <c r="AB38" s="45"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="24">
+        <v>522.95647272727308</v>
+      </c>
+      <c r="C39" s="24">
+        <v>537.91462272727244</v>
+      </c>
+      <c r="D39" s="24">
+        <v>555.91023409090872</v>
+      </c>
+      <c r="E39" s="24">
+        <v>581.31215681818151</v>
+      </c>
+      <c r="F39" s="24">
+        <v>613.49427954545422</v>
+      </c>
+      <c r="G39" s="24">
+        <v>668.04479772727314</v>
+      </c>
+      <c r="H39" s="24">
+        <v>731.91092045454491</v>
+      </c>
+      <c r="I39" s="24">
+        <v>771.80538636363679</v>
+      </c>
+      <c r="J39" s="24">
+        <v>724.845511363637</v>
+      </c>
+      <c r="K39" s="25">
+        <v>519.96256818181814</v>
+      </c>
+      <c r="L39" s="25">
+        <v>545.04867954545443</v>
+      </c>
+      <c r="M39" s="25">
+        <v>565.40321136363616</v>
+      </c>
+      <c r="N39" s="25">
+        <v>576.42325454545471</v>
+      </c>
+      <c r="O39" s="25">
+        <v>576.52500454545452</v>
+      </c>
+      <c r="P39" s="25">
+        <v>568.27938181818229</v>
+      </c>
+      <c r="Q39" s="25">
+        <v>549.73124090909062</v>
+      </c>
+      <c r="R39" s="25">
+        <v>525.23568636363666</v>
+      </c>
+      <c r="S39" s="31">
+        <v>492.49940681818208</v>
+      </c>
+      <c r="T39" s="45"/>
+      <c r="U39" s="45"/>
+      <c r="V39" s="45"/>
+      <c r="W39" s="45"/>
+      <c r="X39" s="45"/>
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45"/>
+      <c r="AA39" s="45"/>
+      <c r="AB39" s="45"/>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="27">
+        <v>46.32082399991549</v>
+      </c>
+      <c r="C40" s="27">
+        <v>43.815054815612797</v>
+      </c>
+      <c r="D40" s="27">
+        <v>44.290450142078043</v>
+      </c>
+      <c r="E40" s="27">
+        <v>48.697897935816002</v>
+      </c>
+      <c r="F40" s="27">
+        <v>59.508954551632641</v>
+      </c>
+      <c r="G40" s="27">
+        <v>80.908915090957876</v>
+      </c>
+      <c r="H40" s="27">
+        <v>107.35990651789969</v>
+      </c>
+      <c r="I40" s="27">
+        <v>128.05703934968574</v>
+      </c>
+      <c r="J40" s="27">
+        <v>121.18959569579545</v>
+      </c>
+      <c r="K40" s="28">
+        <v>63.606131592835595</v>
+      </c>
+      <c r="L40" s="28">
+        <v>72.673538243933621</v>
+      </c>
+      <c r="M40" s="28">
+        <v>82.241254556065329</v>
+      </c>
+      <c r="N40" s="28">
+        <v>87.480934141694604</v>
+      </c>
+      <c r="O40" s="28">
+        <v>85.598754954220624</v>
+      </c>
+      <c r="P40" s="28">
+        <v>81.7424591344258</v>
+      </c>
+      <c r="Q40" s="28">
+        <v>75.215284018071898</v>
+      </c>
+      <c r="R40" s="28">
+        <v>64.683597486014506</v>
+      </c>
+      <c r="S40" s="32">
+        <v>54.032211335839065</v>
+      </c>
+      <c r="T40" s="45"/>
+      <c r="U40" s="45"/>
+      <c r="V40" s="45"/>
+      <c r="W40" s="45"/>
+      <c r="X40" s="45"/>
+      <c r="Y40" s="45"/>
+      <c r="Z40" s="45"/>
+      <c r="AA40" s="45"/>
+      <c r="AB40" s="45"/>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="27">
+        <v>419.45299999999997</v>
+      </c>
+      <c r="C41" s="27">
+        <v>422.57299999999998</v>
+      </c>
+      <c r="D41" s="27">
+        <v>437.86200000000002</v>
+      </c>
+      <c r="E41" s="27">
+        <v>454.32799999999997</v>
+      </c>
+      <c r="F41" s="27">
+        <v>469.226</v>
+      </c>
+      <c r="G41" s="27">
+        <v>513.29999999999995</v>
+      </c>
+      <c r="H41" s="27">
+        <v>519.10299999999995</v>
+      </c>
+      <c r="I41" s="27">
+        <v>484.13900000000001</v>
+      </c>
+      <c r="J41" s="27">
+        <v>478.38299999999998</v>
+      </c>
+      <c r="K41" s="28">
+        <v>395.82600000000002</v>
+      </c>
+      <c r="L41" s="28">
+        <v>416.983</v>
+      </c>
+      <c r="M41" s="28">
+        <v>410.75</v>
+      </c>
+      <c r="N41" s="28">
+        <v>392.58600000000001</v>
+      </c>
+      <c r="O41" s="28">
+        <v>404.30900000000003</v>
+      </c>
+      <c r="P41" s="28">
+        <v>429.774</v>
+      </c>
+      <c r="Q41" s="28">
+        <v>417.00200000000001</v>
+      </c>
+      <c r="R41" s="28">
+        <v>399.995</v>
+      </c>
+      <c r="S41" s="32">
+        <v>406.05399999999997</v>
+      </c>
+      <c r="T41" s="45"/>
+      <c r="U41" s="45"/>
+      <c r="V41" s="45"/>
+      <c r="W41" s="45"/>
+      <c r="X41" s="45"/>
+      <c r="Y41" s="45"/>
+      <c r="Z41" s="45"/>
+      <c r="AA41" s="45"/>
+      <c r="AB41" s="45"/>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="27">
+        <v>664.49699999999996</v>
+      </c>
+      <c r="C42" s="27">
+        <v>673.58399999999995</v>
+      </c>
+      <c r="D42" s="27">
+        <v>666.99699999999996</v>
+      </c>
+      <c r="E42" s="27">
+        <v>724.50199999999995</v>
+      </c>
+      <c r="F42" s="27">
+        <v>780.38499999999999</v>
+      </c>
+      <c r="G42" s="27">
+        <v>892.27499999999998</v>
+      </c>
+      <c r="H42" s="27">
+        <v>1074.6130000000001</v>
+      </c>
+      <c r="I42" s="27">
+        <v>1148.338</v>
+      </c>
+      <c r="J42" s="27">
+        <v>1197.847</v>
+      </c>
+      <c r="K42" s="28">
+        <v>737.58399999999995</v>
+      </c>
+      <c r="L42" s="28">
+        <v>816.74599999999998</v>
+      </c>
+      <c r="M42" s="28">
+        <v>846.37</v>
+      </c>
+      <c r="N42" s="28">
+        <v>837.572</v>
+      </c>
+      <c r="O42" s="28">
+        <v>858.726</v>
+      </c>
+      <c r="P42" s="28">
+        <v>834.62699999999995</v>
+      </c>
+      <c r="Q42" s="28">
+        <v>820.28800000000001</v>
+      </c>
+      <c r="R42" s="28">
+        <v>738.20100000000002</v>
+      </c>
+      <c r="S42" s="32">
+        <v>654.17499999999995</v>
+      </c>
+      <c r="T42" s="45"/>
+      <c r="U42" s="45"/>
+      <c r="V42" s="45"/>
+      <c r="W42" s="45"/>
+      <c r="X42" s="45"/>
+      <c r="Y42" s="45"/>
+      <c r="Z42" s="45"/>
+      <c r="AA42" s="45"/>
+      <c r="AB42" s="45"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="33"/>
+      <c r="T43" s="46"/>
+      <c r="U43" s="46"/>
+      <c r="V43" s="46"/>
+      <c r="W43" s="46"/>
+      <c r="X43" s="46"/>
+      <c r="Y43" s="46"/>
+      <c r="Z43" s="46"/>
+      <c r="AA43" s="46"/>
+      <c r="AB43" s="46"/>
+    </row>
+    <row r="44" spans="1:28" ht="21" x14ac:dyDescent="0.4">
+      <c r="A44" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="59">
+        <v>20</v>
+      </c>
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
+      <c r="L44" s="59"/>
+      <c r="M44" s="59"/>
+      <c r="N44" s="59"/>
+      <c r="O44" s="59"/>
+      <c r="P44" s="59"/>
+      <c r="Q44" s="59"/>
+      <c r="R44" s="59"/>
+      <c r="S44" s="60"/>
+      <c r="T44" s="44"/>
+      <c r="U44" s="44"/>
+      <c r="V44" s="44"/>
+      <c r="W44" s="44"/>
+      <c r="X44" s="44"/>
+      <c r="Y44" s="44"/>
+      <c r="Z44" s="44"/>
+      <c r="AA44" s="44"/>
+      <c r="AB44" s="44"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="O45" s="56"/>
+      <c r="P45" s="56"/>
+      <c r="Q45" s="56"/>
+      <c r="R45" s="56"/>
+      <c r="S45" s="57"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="22">
+        <v>8</v>
+      </c>
+      <c r="C46" s="22">
+        <v>9</v>
+      </c>
+      <c r="D46" s="22">
+        <v>10</v>
+      </c>
+      <c r="E46" s="22">
+        <v>11</v>
+      </c>
+      <c r="F46" s="22">
+        <v>12</v>
+      </c>
+      <c r="G46" s="22">
+        <v>13</v>
+      </c>
+      <c r="H46" s="22">
+        <v>14</v>
+      </c>
+      <c r="I46" s="22">
+        <v>15</v>
+      </c>
+      <c r="J46" s="22">
+        <v>16</v>
+      </c>
+      <c r="K46" s="23">
+        <v>8</v>
+      </c>
+      <c r="L46" s="23">
+        <v>9</v>
+      </c>
+      <c r="M46" s="23">
+        <v>10</v>
+      </c>
+      <c r="N46" s="23">
+        <v>11</v>
+      </c>
+      <c r="O46" s="23">
+        <v>12</v>
+      </c>
+      <c r="P46" s="23">
+        <v>13</v>
+      </c>
+      <c r="Q46" s="23">
+        <v>14</v>
+      </c>
+      <c r="R46" s="23">
+        <v>15</v>
+      </c>
+      <c r="S46" s="30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="24">
+        <v>652.78706363636377</v>
+      </c>
+      <c r="C47" s="24">
+        <v>666.76828409090888</v>
+      </c>
+      <c r="D47" s="24">
+        <v>681.03159090909026</v>
+      </c>
+      <c r="E47" s="24">
+        <v>708.64510909090882</v>
+      </c>
+      <c r="F47" s="24">
+        <v>738.6938977272722</v>
+      </c>
+      <c r="G47" s="24">
+        <v>795.58016590909074</v>
+      </c>
+      <c r="H47" s="24">
+        <v>855.27558409090886</v>
+      </c>
+      <c r="I47" s="24">
+        <v>893.47342272727246</v>
+      </c>
+      <c r="J47" s="24">
+        <v>853.5148181818181</v>
+      </c>
+      <c r="K47" s="25">
+        <v>643.74759318181816</v>
+      </c>
+      <c r="L47" s="25">
+        <v>670.85762045454544</v>
+      </c>
+      <c r="M47" s="25">
+        <v>692.58822045454497</v>
+      </c>
+      <c r="N47" s="25">
+        <v>702.38926818181801</v>
+      </c>
+      <c r="O47" s="25">
+        <v>706.68184545454551</v>
+      </c>
+      <c r="P47" s="25">
+        <v>695.94599545454514</v>
+      </c>
+      <c r="Q47" s="25">
+        <v>676.87536818181809</v>
+      </c>
+      <c r="R47" s="25">
+        <v>652.62700227272751</v>
+      </c>
+      <c r="S47" s="31">
+        <v>620.91578636363647</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="27">
+        <v>51.52489452023832</v>
+      </c>
+      <c r="C48" s="27">
+        <v>52.852297989393577</v>
+      </c>
+      <c r="D48" s="27">
+        <v>50.813086729864892</v>
+      </c>
+      <c r="E48" s="27">
+        <v>54.498786409023893</v>
+      </c>
+      <c r="F48" s="27">
+        <v>63.124848442216823</v>
+      </c>
+      <c r="G48" s="27">
+        <v>83.376774200027583</v>
+      </c>
+      <c r="H48" s="27">
+        <v>110.08837422892087</v>
+      </c>
+      <c r="I48" s="27">
+        <v>130.80862259132755</v>
+      </c>
+      <c r="J48" s="27">
+        <v>125.41144066262341</v>
+      </c>
+      <c r="K48" s="28">
+        <v>66.57642541575504</v>
+      </c>
+      <c r="L48" s="28">
+        <v>77.572350900889759</v>
+      </c>
+      <c r="M48" s="28">
+        <v>83.925513612245808</v>
+      </c>
+      <c r="N48" s="28">
+        <v>88.164336560839402</v>
+      </c>
+      <c r="O48" s="28">
+        <v>87.909798455084726</v>
+      </c>
+      <c r="P48" s="28">
+        <v>85.954727666244338</v>
+      </c>
+      <c r="Q48" s="28">
+        <v>78.617876922872512</v>
+      </c>
+      <c r="R48" s="28">
+        <v>68.95266472524834</v>
+      </c>
+      <c r="S48" s="32">
+        <v>58.153020856354765</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="27">
+        <v>552.04899999999998</v>
+      </c>
+      <c r="C49" s="27">
+        <v>558.96199999999999</v>
+      </c>
+      <c r="D49" s="27">
+        <v>567.43600000000004</v>
+      </c>
+      <c r="E49" s="27">
+        <v>588.05799999999999</v>
+      </c>
+      <c r="F49" s="27">
+        <v>626.77499999999998</v>
+      </c>
+      <c r="G49" s="27">
+        <v>629.16399999999999</v>
+      </c>
+      <c r="H49" s="27">
+        <v>661.75300000000004</v>
+      </c>
+      <c r="I49" s="27">
+        <v>654.68899999999996</v>
+      </c>
+      <c r="J49" s="27">
+        <v>640.03200000000004</v>
+      </c>
+      <c r="K49" s="28">
+        <v>520.26800000000003</v>
+      </c>
+      <c r="L49" s="28">
+        <v>525.54</v>
+      </c>
+      <c r="M49" s="28">
+        <v>531.00800000000004</v>
+      </c>
+      <c r="N49" s="28">
+        <v>532.88599999999997</v>
+      </c>
+      <c r="O49" s="28">
+        <v>559.69000000000005</v>
+      </c>
+      <c r="P49" s="28">
+        <v>540.62699999999995</v>
+      </c>
+      <c r="Q49" s="28">
+        <v>522.87</v>
+      </c>
+      <c r="R49" s="28">
+        <v>539.66800000000001</v>
+      </c>
+      <c r="S49" s="32">
+        <v>508.846</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="40">
+        <v>804.63699999999994</v>
+      </c>
+      <c r="C50" s="40">
+        <v>823.76300000000003</v>
+      </c>
+      <c r="D50" s="40">
+        <v>833.35299999999995</v>
+      </c>
+      <c r="E50" s="40">
+        <v>884.30700000000002</v>
+      </c>
+      <c r="F50" s="40">
+        <v>949.31899999999996</v>
+      </c>
+      <c r="G50" s="40">
+        <v>1048.213</v>
+      </c>
+      <c r="H50" s="40">
+        <v>1189.143</v>
+      </c>
+      <c r="I50" s="40">
+        <v>1284.3440000000001</v>
+      </c>
+      <c r="J50" s="40">
+        <v>1222.193</v>
+      </c>
+      <c r="K50" s="41">
+        <v>847.46600000000001</v>
+      </c>
+      <c r="L50" s="41">
+        <v>923.78</v>
+      </c>
+      <c r="M50" s="41">
+        <v>952.72199999999998</v>
+      </c>
+      <c r="N50" s="41">
+        <v>986.38199999999995</v>
+      </c>
+      <c r="O50" s="41">
+        <v>970.18100000000004</v>
+      </c>
+      <c r="P50" s="41">
+        <v>989.53899999999999</v>
+      </c>
+      <c r="Q50" s="41">
+        <v>907.52499999999998</v>
+      </c>
+      <c r="R50" s="41">
+        <v>872.02200000000005</v>
+      </c>
+      <c r="S50" s="42">
+        <v>782.71500000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="B44:S44"/>
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="K45:S45"/>
+    <mergeCell ref="A27:S27"/>
+    <mergeCell ref="B28:S28"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="K29:S29"/>
+    <mergeCell ref="B36:S36"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="K37:S37"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="K11:S11"/>
+    <mergeCell ref="T11:AB11"/>
+    <mergeCell ref="B18:AB18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="K19:S19"/>
+    <mergeCell ref="T19:AB19"/>
+    <mergeCell ref="A1:AB1"/>
+    <mergeCell ref="B2:AB2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="K3:S3"/>
+    <mergeCell ref="T3:AB3"/>
+    <mergeCell ref="B10:AB10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
dodanie wykresów i zrzutów ekranu do prezentacji
</commit_message>
<xml_diff>
--- a/doc/projekt/Wyniki_symulacji/Symulacje_podsumowanie.xlsx
+++ b/doc/projekt/Wyniki_symulacji/Symulacje_podsumowanie.xlsx
@@ -433,6 +433,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -470,23 +477,16 @@
     <xf numFmtId="16" fontId="4" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="4" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="4" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1061,11 +1061,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188054880"/>
-        <c:axId val="188052528"/>
+        <c:axId val="120753704"/>
+        <c:axId val="119666360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188054880"/>
+        <c:axId val="120753704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -1180,12 +1180,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188052528"/>
+        <c:crossAx val="119666360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188052528"/>
+        <c:axId val="119666360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1298,7 +1298,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188054880"/>
+        <c:crossAx val="120753704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1374,7 +1374,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2045,11 +2045,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="465662520"/>
-        <c:axId val="465662128"/>
+        <c:axId val="122311640"/>
+        <c:axId val="122306544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="465662520"/>
+        <c:axId val="122311640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -2164,12 +2164,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465662128"/>
+        <c:crossAx val="122306544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="465662128"/>
+        <c:axId val="122306544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2282,7 +2282,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465662520"/>
+        <c:crossAx val="122311640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2358,7 +2358,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3029,11 +3029,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="464370448"/>
-        <c:axId val="464368488"/>
+        <c:axId val="122308896"/>
+        <c:axId val="122312424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="464370448"/>
+        <c:axId val="122308896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -3148,12 +3148,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464368488"/>
+        <c:crossAx val="122312424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="464368488"/>
+        <c:axId val="122312424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3266,7 +3266,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464370448"/>
+        <c:crossAx val="122308896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3342,7 +3342,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3905,11 +3905,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="192200088"/>
-        <c:axId val="192209104"/>
+        <c:axId val="119669496"/>
+        <c:axId val="119666752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="192200088"/>
+        <c:axId val="119669496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -4024,12 +4024,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192209104"/>
+        <c:crossAx val="119666752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="192209104"/>
+        <c:axId val="119666752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4142,7 +4142,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192200088"/>
+        <c:crossAx val="119669496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4902,11 +4902,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="461538992"/>
-        <c:axId val="461539776"/>
+        <c:axId val="119668320"/>
+        <c:axId val="121005880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="461538992"/>
+        <c:axId val="119668320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -5021,12 +5021,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="461539776"/>
+        <c:crossAx val="121005880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="461539776"/>
+        <c:axId val="121005880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5139,7 +5139,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="461538992"/>
+        <c:crossAx val="119668320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5215,7 +5215,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -5899,11 +5899,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="192200480"/>
-        <c:axId val="192197736"/>
+        <c:axId val="121007840"/>
+        <c:axId val="121004312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="192200480"/>
+        <c:axId val="121007840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -6018,12 +6018,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192197736"/>
+        <c:crossAx val="121004312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="192197736"/>
+        <c:axId val="121004312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6136,7 +6136,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192200480"/>
+        <c:crossAx val="121007840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6212,7 +6212,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -6896,11 +6896,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="460948224"/>
-        <c:axId val="460949792"/>
+        <c:axId val="121005488"/>
+        <c:axId val="121005096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="460948224"/>
+        <c:axId val="121005488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -7015,12 +7015,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="460949792"/>
+        <c:crossAx val="121005096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="460949792"/>
+        <c:axId val="121005096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7133,7 +7133,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="460948224"/>
+        <c:crossAx val="121005488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7209,7 +7209,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -7896,11 +7896,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="466564616"/>
-        <c:axId val="466561872"/>
+        <c:axId val="121007448"/>
+        <c:axId val="121001960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="466564616"/>
+        <c:axId val="121007448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -8015,12 +8015,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466561872"/>
+        <c:crossAx val="121001960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="466561872"/>
+        <c:axId val="121001960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8133,7 +8133,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466564616"/>
+        <c:crossAx val="121007448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8209,7 +8209,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -8400,31 +8400,31 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>507.46347045454507</c:v>
+                  <c:v>309.91721818181793</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>438.13881363636386</c:v>
+                  <c:v>328.03074999999961</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>460.09569999999951</c:v>
+                  <c:v>361.59595909090956</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>531.24007272727317</c:v>
+                  <c:v>398.41242499999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>621.36957499999971</c:v>
+                  <c:v>429.70733636363639</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>671.15724318181844</c:v>
+                  <c:v>446.63005681818203</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2801.3484363636339</c:v>
+                  <c:v>752.68142727272777</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3110.9478477272733</c:v>
+                  <c:v>760.40187499999945</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>589.08129318181818</c:v>
+                  <c:v>334.87098636363623</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8896,11 +8896,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="458501352"/>
-        <c:axId val="458500176"/>
+        <c:axId val="121002744"/>
+        <c:axId val="121003136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="458501352"/>
+        <c:axId val="121002744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -9015,12 +9015,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="458500176"/>
+        <c:crossAx val="121003136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="458500176"/>
+        <c:axId val="121003136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9133,7 +9133,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="458501352"/>
+        <c:crossAx val="121002744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9209,7 +9209,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -9896,11 +9896,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="463264320"/>
-        <c:axId val="463265496"/>
+        <c:axId val="121003920"/>
+        <c:axId val="122311248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="463264320"/>
+        <c:axId val="121003920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -10015,12 +10015,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463265496"/>
+        <c:crossAx val="122311248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="463265496"/>
+        <c:axId val="122311248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10133,7 +10133,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463264320"/>
+        <c:crossAx val="121003920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10209,7 +10209,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -10880,11 +10880,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188049784"/>
-        <c:axId val="188050176"/>
+        <c:axId val="122309680"/>
+        <c:axId val="122312032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188049784"/>
+        <c:axId val="122309680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -10999,12 +10999,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188050176"/>
+        <c:crossAx val="122312032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188050176"/>
+        <c:axId val="122312032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11117,7 +11117,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188049784"/>
+        <c:crossAx val="122309680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11193,7 +11193,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -17324,10 +17324,10 @@
       <xdr:rowOff>10884</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>97969</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>108856</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>453126</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>178713</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17348,16 +17348,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>446314</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>174171</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>337456</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>364671</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>87086</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>353785</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17388,13 +17388,13 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>32657</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>32657</xdr:rowOff>
+      <xdr:rowOff>32656</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>424543</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>54428</xdr:rowOff>
+      <xdr:colOff>469457</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>178713</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17424,9 +17424,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>587828</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>21770</xdr:rowOff>
+      <xdr:colOff>632742</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>146057</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17451,14 +17451,14 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>185056</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
-      <xdr:colOff>391886</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>43542</xdr:rowOff>
+      <xdr:colOff>436800</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>167827</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17489,13 +17489,13 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>-1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>391886</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>141514</xdr:rowOff>
+      <xdr:colOff>436800</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>58971</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17521,13 +17521,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>108857</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>32659</xdr:rowOff>
+      <xdr:rowOff>32658</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>348343</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
+      <xdr:colOff>393257</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>15429</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17553,13 +17553,13 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>511628</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>293914</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>141514</xdr:rowOff>
+      <xdr:colOff>338828</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>58970</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17593,10 +17593,10 @@
       <xdr:rowOff>99061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>53341</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>116760</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9261</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17619,16 +17619,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>513080</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>132080</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>335200</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>49900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17652,15 +17652,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>55880</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>157400</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>151500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17949,8 +17949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y61" sqref="Y61"/>
+    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17959,110 +17959,112 @@
     <col min="2" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" customWidth="1"/>
+    <col min="15" max="16" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="53"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="56"/>
     </row>
     <row r="2" spans="1:28" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
-      <c r="B2" s="58">
+      <c r="B2" s="61">
         <v>43871</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="59"/>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="60"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="63"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="56" t="s">
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="57"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="60"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -18616,71 +18618,71 @@
     </row>
     <row r="13" spans="1:28" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="1"/>
-      <c r="B13" s="58">
+      <c r="B13" s="61">
         <v>43961</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
-      <c r="U13" s="59"/>
-      <c r="V13" s="59"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="59"/>
-      <c r="Y13" s="59"/>
-      <c r="Z13" s="59"/>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="60"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62"/>
+      <c r="T13" s="62"/>
+      <c r="U13" s="62"/>
+      <c r="V13" s="62"/>
+      <c r="W13" s="62"/>
+      <c r="X13" s="62"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="63"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="48" t="s">
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="49" t="s">
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="U14" s="49"/>
-      <c r="V14" s="49"/>
-      <c r="W14" s="49"/>
-      <c r="X14" s="49"/>
-      <c r="Y14" s="49"/>
-      <c r="Z14" s="49"/>
-      <c r="AA14" s="49"/>
-      <c r="AB14" s="50"/>
+      <c r="U14" s="52"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="52"/>
+      <c r="X14" s="52"/>
+      <c r="Y14" s="52"/>
+      <c r="Z14" s="52"/>
+      <c r="AA14" s="52"/>
+      <c r="AB14" s="53"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -19234,34 +19236,34 @@
     </row>
     <row r="24" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="67">
+      <c r="B25" s="48">
         <v>400</v>
       </c>
-      <c r="C25" s="67">
+      <c r="C25" s="48">
         <v>400</v>
       </c>
-      <c r="D25" s="67">
+      <c r="D25" s="48">
         <v>400</v>
       </c>
-      <c r="E25" s="67">
+      <c r="E25" s="48">
         <v>400</v>
       </c>
-      <c r="F25" s="67">
+      <c r="F25" s="48">
         <v>400</v>
       </c>
-      <c r="G25" s="67">
+      <c r="G25" s="48">
         <v>400</v>
       </c>
-      <c r="H25" s="67">
+      <c r="H25" s="48">
         <v>400</v>
       </c>
-      <c r="I25" s="67">
+      <c r="I25" s="48">
         <v>400</v>
       </c>
-      <c r="J25" s="68">
+      <c r="J25" s="49">
         <v>400</v>
       </c>
     </row>
@@ -19286,7 +19288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J52" sqref="A52:J52"/>
     </sheetView>
   </sheetViews>
@@ -19299,106 +19301,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="61">
+      <c r="A1" s="64">
         <v>43871</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="63"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="68"/>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="59"/>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="60"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="63"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="56" t="s">
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="57"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="60"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -19864,71 +19866,71 @@
       <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
-      <c r="S10" s="59"/>
-      <c r="T10" s="59"/>
-      <c r="U10" s="59"/>
-      <c r="V10" s="59"/>
-      <c r="W10" s="59"/>
-      <c r="X10" s="59"/>
-      <c r="Y10" s="59"/>
-      <c r="Z10" s="59"/>
-      <c r="AA10" s="59"/>
-      <c r="AB10" s="60"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="62"/>
+      <c r="V10" s="62"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="63"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55" t="s">
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="55"/>
-      <c r="T11" s="56" t="s">
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="U11" s="56"/>
-      <c r="V11" s="56"/>
-      <c r="W11" s="56"/>
-      <c r="X11" s="56"/>
-      <c r="Y11" s="56"/>
-      <c r="Z11" s="56"/>
-      <c r="AA11" s="56"/>
-      <c r="AB11" s="57"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="59"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="59"/>
+      <c r="Y11" s="59"/>
+      <c r="Z11" s="59"/>
+      <c r="AA11" s="59"/>
+      <c r="AB11" s="60"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -20394,71 +20396,71 @@
       <c r="A18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="59"/>
-      <c r="X18" s="59"/>
-      <c r="Y18" s="59"/>
-      <c r="Z18" s="59"/>
-      <c r="AA18" s="59"/>
-      <c r="AB18" s="60"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="62"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="62"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="62"/>
+      <c r="W18" s="62"/>
+      <c r="X18" s="62"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="62"/>
+      <c r="AB18" s="63"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="55" t="s">
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="55"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55"/>
-      <c r="R19" s="55"/>
-      <c r="S19" s="55"/>
-      <c r="T19" s="56" t="s">
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="U19" s="56"/>
-      <c r="V19" s="56"/>
-      <c r="W19" s="56"/>
-      <c r="X19" s="56"/>
-      <c r="Y19" s="56"/>
-      <c r="Z19" s="56"/>
-      <c r="AA19" s="56"/>
-      <c r="AB19" s="57"/>
+      <c r="U19" s="59"/>
+      <c r="V19" s="59"/>
+      <c r="W19" s="59"/>
+      <c r="X19" s="59"/>
+      <c r="Y19" s="59"/>
+      <c r="Z19" s="59"/>
+      <c r="AA19" s="59"/>
+      <c r="AB19" s="60"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -20892,27 +20894,27 @@
     </row>
     <row r="26" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A27" s="61">
+      <c r="A27" s="64">
         <v>43961</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="64"/>
-      <c r="P27" s="64"/>
-      <c r="Q27" s="64"/>
-      <c r="R27" s="64"/>
-      <c r="S27" s="65"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="66"/>
       <c r="T27" s="43"/>
       <c r="U27" s="43"/>
       <c r="V27" s="43"/>
@@ -20927,26 +20929,26 @@
       <c r="A28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="60"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="62"/>
+      <c r="R28" s="62"/>
+      <c r="S28" s="63"/>
       <c r="T28" s="44"/>
       <c r="U28" s="44"/>
       <c r="V28" s="44"/>
@@ -20959,28 +20961,28 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="56" t="s">
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="56"/>
-      <c r="S29" s="57"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="59"/>
+      <c r="R29" s="59"/>
+      <c r="S29" s="60"/>
       <c r="T29" s="45"/>
       <c r="U29" s="45"/>
       <c r="V29" s="45"/>
@@ -21365,26 +21367,26 @@
       <c r="A36" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="59" t="s">
+      <c r="B36" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="59"/>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
-      <c r="R36" s="59"/>
-      <c r="S36" s="60"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="63"/>
       <c r="T36" s="44"/>
       <c r="U36" s="44"/>
       <c r="V36" s="44"/>
@@ -21397,28 +21399,28 @@
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="56" t="s">
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="57"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
+      <c r="S37" s="60"/>
       <c r="T37" s="45"/>
       <c r="U37" s="45"/>
       <c r="V37" s="45"/>
@@ -21803,26 +21805,26 @@
       <c r="A44" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="59" t="s">
+      <c r="B44" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
-      <c r="K44" s="59"/>
-      <c r="L44" s="59"/>
-      <c r="M44" s="59"/>
-      <c r="N44" s="59"/>
-      <c r="O44" s="59"/>
-      <c r="P44" s="59"/>
-      <c r="Q44" s="59"/>
-      <c r="R44" s="59"/>
-      <c r="S44" s="60"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="62"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="62"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="62"/>
+      <c r="R44" s="62"/>
+      <c r="S44" s="63"/>
       <c r="T44" s="44"/>
       <c r="U44" s="44"/>
       <c r="V44" s="44"/>
@@ -21835,28 +21837,28 @@
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="B45" s="55" t="s">
+      <c r="B45" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="56" t="s">
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="58"/>
+      <c r="K45" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="56"/>
-      <c r="P45" s="56"/>
-      <c r="Q45" s="56"/>
-      <c r="R45" s="56"/>
-      <c r="S45" s="57"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="59"/>
+      <c r="O45" s="59"/>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="59"/>
+      <c r="R45" s="59"/>
+      <c r="S45" s="60"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
@@ -22155,49 +22157,39 @@
     </row>
     <row r="51" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="67">
+      <c r="B52" s="48">
         <v>400</v>
       </c>
-      <c r="C52" s="67">
+      <c r="C52" s="48">
         <v>400</v>
       </c>
-      <c r="D52" s="67">
+      <c r="D52" s="48">
         <v>400</v>
       </c>
-      <c r="E52" s="67">
+      <c r="E52" s="48">
         <v>400</v>
       </c>
-      <c r="F52" s="67">
+      <c r="F52" s="48">
         <v>400</v>
       </c>
-      <c r="G52" s="67">
+      <c r="G52" s="48">
         <v>400</v>
       </c>
-      <c r="H52" s="67">
+      <c r="H52" s="48">
         <v>400</v>
       </c>
-      <c r="I52" s="67">
+      <c r="I52" s="48">
         <v>400</v>
       </c>
-      <c r="J52" s="68">
+      <c r="J52" s="49">
         <v>400</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B45:J45"/>
-    <mergeCell ref="K45:S45"/>
-    <mergeCell ref="A27:S27"/>
-    <mergeCell ref="B28:S28"/>
-    <mergeCell ref="B36:S36"/>
-    <mergeCell ref="B44:S44"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="K37:S37"/>
-    <mergeCell ref="B29:J29"/>
-    <mergeCell ref="K29:S29"/>
     <mergeCell ref="A1:AB1"/>
     <mergeCell ref="B2:AB2"/>
     <mergeCell ref="B18:AB18"/>
@@ -22211,9 +22203,19 @@
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="K3:S3"/>
     <mergeCell ref="T3:AB3"/>
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="K45:S45"/>
+    <mergeCell ref="A27:S27"/>
+    <mergeCell ref="B28:S28"/>
+    <mergeCell ref="B36:S36"/>
+    <mergeCell ref="B44:S44"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="K37:S37"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="K29:S29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -22222,8 +22224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AO79" sqref="AO79"/>
+    <sheetView topLeftCell="L46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T79" sqref="T79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22235,106 +22237,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="61">
+      <c r="A1" s="64">
         <v>43871</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="63"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="68"/>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="59"/>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="60"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="63"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="56" t="s">
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="57"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="60"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -22454,31 +22456,31 @@
         <v>591.01364090909101</v>
       </c>
       <c r="K5" s="24">
-        <v>507.46347045454507</v>
+        <v>309.91721818181793</v>
       </c>
       <c r="L5" s="24">
-        <v>438.13881363636386</v>
+        <v>328.03074999999961</v>
       </c>
       <c r="M5" s="24">
-        <v>460.09569999999951</v>
+        <v>361.59595909090956</v>
       </c>
       <c r="N5" s="24">
-        <v>531.24007272727317</v>
+        <v>398.41242499999998</v>
       </c>
       <c r="O5" s="24">
-        <v>621.36957499999971</v>
+        <v>429.70733636363639</v>
       </c>
       <c r="P5" s="24">
-        <v>671.15724318181844</v>
+        <v>446.63005681818203</v>
       </c>
       <c r="Q5" s="24">
-        <v>2801.3484363636339</v>
+        <v>752.68142727272777</v>
       </c>
       <c r="R5" s="24">
-        <v>3110.9478477272733</v>
+        <v>760.40187499999945</v>
       </c>
       <c r="S5" s="24">
-        <v>589.08129318181818</v>
+        <v>334.87098636363623</v>
       </c>
       <c r="T5" s="25">
         <v>284.92667954545482</v>
@@ -22540,31 +22542,31 @@
         <v>330.35615354577067</v>
       </c>
       <c r="K6" s="27">
-        <v>311.1756852749466</v>
+        <v>44.17931005031631</v>
       </c>
       <c r="L6" s="27">
-        <v>49.54087755161904</v>
+        <v>26.573975332570807</v>
       </c>
       <c r="M6" s="27">
-        <v>40.938433190153866</v>
+        <v>33.840552606638909</v>
       </c>
       <c r="N6" s="27">
-        <v>44.048195236252397</v>
+        <v>39.946753644931498</v>
       </c>
       <c r="O6" s="27">
-        <v>60.846859061371887</v>
+        <v>48.015234868447195</v>
       </c>
       <c r="P6" s="27">
-        <v>85.093945356307628</v>
+        <v>54.792513607554817</v>
       </c>
       <c r="Q6" s="27">
-        <v>3387.9101732187551</v>
+        <v>532.77906699831772</v>
       </c>
       <c r="R6" s="27">
-        <v>2231.5414789391025</v>
+        <v>320.84579733991336</v>
       </c>
       <c r="S6" s="27">
-        <v>329.19271792211686</v>
+        <v>44.588173288163176</v>
       </c>
       <c r="T6" s="28">
         <v>21.268747885551946</v>
@@ -22626,31 +22628,31 @@
         <v>338.03500000000003</v>
       </c>
       <c r="K7" s="27">
-        <v>304.59899999999999</v>
+        <v>258.577</v>
       </c>
       <c r="L7" s="27">
-        <v>323.93200000000002</v>
+        <v>266.40199999999999</v>
       </c>
       <c r="M7" s="27">
-        <v>342.80500000000001</v>
+        <v>282.67899999999997</v>
       </c>
       <c r="N7" s="27">
-        <v>405.988</v>
+        <v>312.11700000000002</v>
       </c>
       <c r="O7" s="27">
-        <v>413.45800000000003</v>
+        <v>322.74599999999998</v>
       </c>
       <c r="P7" s="27">
-        <v>477.339</v>
+        <v>322.24799999999999</v>
       </c>
       <c r="Q7" s="27">
-        <v>483.57400000000001</v>
+        <v>339.76499999999999</v>
       </c>
       <c r="R7" s="27">
-        <v>430.245</v>
+        <v>293.82799999999997</v>
       </c>
       <c r="S7" s="27">
-        <v>356.87900000000002</v>
+        <v>265.86500000000001</v>
       </c>
       <c r="T7" s="28">
         <v>239.57599999999999</v>
@@ -22712,31 +22714,31 @@
         <v>1485.865</v>
       </c>
       <c r="K8" s="27">
-        <v>1731.027</v>
+        <v>466.77199999999999</v>
       </c>
       <c r="L8" s="27">
-        <v>614.50699999999995</v>
+        <v>411.37400000000002</v>
       </c>
       <c r="M8" s="27">
-        <v>598.072</v>
+        <v>452.99400000000003</v>
       </c>
       <c r="N8" s="27">
-        <v>672.47699999999998</v>
+        <v>534.89300000000003</v>
       </c>
       <c r="O8" s="27">
-        <v>820.89</v>
+        <v>568.80399999999997</v>
       </c>
       <c r="P8" s="27">
-        <v>944.66700000000003</v>
+        <v>612.11500000000001</v>
       </c>
       <c r="Q8" s="27">
-        <v>8443.0740000000005</v>
+        <v>1702.8510000000001</v>
       </c>
       <c r="R8" s="27">
-        <v>5302.9960000000001</v>
+        <v>1117.077</v>
       </c>
       <c r="S8" s="27">
-        <v>1479.0070000000001</v>
+        <v>442.70699999999999</v>
       </c>
       <c r="T8" s="28">
         <v>336.02600000000001</v>
@@ -22800,71 +22802,71 @@
       <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
-      <c r="S10" s="59"/>
-      <c r="T10" s="59"/>
-      <c r="U10" s="59"/>
-      <c r="V10" s="59"/>
-      <c r="W10" s="59"/>
-      <c r="X10" s="59"/>
-      <c r="Y10" s="59"/>
-      <c r="Z10" s="59"/>
-      <c r="AA10" s="59"/>
-      <c r="AB10" s="60"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="62"/>
+      <c r="V10" s="62"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="63"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55" t="s">
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="55"/>
-      <c r="T11" s="56" t="s">
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="U11" s="56"/>
-      <c r="V11" s="56"/>
-      <c r="W11" s="56"/>
-      <c r="X11" s="56"/>
-      <c r="Y11" s="56"/>
-      <c r="Z11" s="56"/>
-      <c r="AA11" s="56"/>
-      <c r="AB11" s="57"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="59"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="59"/>
+      <c r="Y11" s="59"/>
+      <c r="Z11" s="59"/>
+      <c r="AA11" s="59"/>
+      <c r="AB11" s="60"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -23330,71 +23332,71 @@
       <c r="A18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="59"/>
-      <c r="X18" s="59"/>
-      <c r="Y18" s="59"/>
-      <c r="Z18" s="59"/>
-      <c r="AA18" s="59"/>
-      <c r="AB18" s="60"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="62"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="62"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="62"/>
+      <c r="W18" s="62"/>
+      <c r="X18" s="62"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="62"/>
+      <c r="AB18" s="63"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="55" t="s">
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="55"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55"/>
-      <c r="R19" s="55"/>
-      <c r="S19" s="55"/>
-      <c r="T19" s="56" t="s">
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="U19" s="56"/>
-      <c r="V19" s="56"/>
-      <c r="W19" s="56"/>
-      <c r="X19" s="56"/>
-      <c r="Y19" s="56"/>
-      <c r="Z19" s="56"/>
-      <c r="AA19" s="56"/>
-      <c r="AB19" s="57"/>
+      <c r="U19" s="59"/>
+      <c r="V19" s="59"/>
+      <c r="W19" s="59"/>
+      <c r="X19" s="59"/>
+      <c r="Y19" s="59"/>
+      <c r="Z19" s="59"/>
+      <c r="AA19" s="59"/>
+      <c r="AB19" s="60"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -23828,27 +23830,27 @@
     </row>
     <row r="26" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:28" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A27" s="61">
+      <c r="A27" s="64">
         <v>43961</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="64"/>
-      <c r="P27" s="64"/>
-      <c r="Q27" s="64"/>
-      <c r="R27" s="64"/>
-      <c r="S27" s="65"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="66"/>
       <c r="T27" s="43"/>
       <c r="U27" s="43"/>
       <c r="V27" s="43"/>
@@ -23863,26 +23865,26 @@
       <c r="A28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="60"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="62"/>
+      <c r="R28" s="62"/>
+      <c r="S28" s="63"/>
       <c r="T28" s="44"/>
       <c r="U28" s="44"/>
       <c r="V28" s="44"/>
@@ -23895,28 +23897,28 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="56" t="s">
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="56"/>
-      <c r="S29" s="57"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="59"/>
+      <c r="R29" s="59"/>
+      <c r="S29" s="60"/>
       <c r="T29" s="45"/>
       <c r="U29" s="45"/>
       <c r="V29" s="45"/>
@@ -24301,26 +24303,26 @@
       <c r="A36" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="59" t="s">
+      <c r="B36" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="59"/>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
-      <c r="R36" s="59"/>
-      <c r="S36" s="60"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="63"/>
       <c r="T36" s="44"/>
       <c r="U36" s="44"/>
       <c r="V36" s="44"/>
@@ -24333,28 +24335,28 @@
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="56" t="s">
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="57"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
+      <c r="S37" s="60"/>
       <c r="T37" s="45"/>
       <c r="U37" s="45"/>
       <c r="V37" s="45"/>
@@ -24739,26 +24741,26 @@
       <c r="A44" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="59" t="s">
+      <c r="B44" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
-      <c r="K44" s="59"/>
-      <c r="L44" s="59"/>
-      <c r="M44" s="59"/>
-      <c r="N44" s="59"/>
-      <c r="O44" s="59"/>
-      <c r="P44" s="59"/>
-      <c r="Q44" s="59"/>
-      <c r="R44" s="59"/>
-      <c r="S44" s="60"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="62"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="62"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="62"/>
+      <c r="R44" s="62"/>
+      <c r="S44" s="63"/>
       <c r="T44" s="44"/>
       <c r="U44" s="44"/>
       <c r="V44" s="44"/>
@@ -24771,28 +24773,28 @@
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="B45" s="55" t="s">
+      <c r="B45" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="56" t="s">
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="58"/>
+      <c r="K45" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="56"/>
-      <c r="P45" s="56"/>
-      <c r="Q45" s="56"/>
-      <c r="R45" s="56"/>
-      <c r="S45" s="57"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="59"/>
+      <c r="O45" s="59"/>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="59"/>
+      <c r="R45" s="59"/>
+      <c r="S45" s="60"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
@@ -25091,52 +25093,39 @@
     </row>
     <row r="51" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="67">
+      <c r="B52" s="48">
         <v>400</v>
       </c>
-      <c r="C52" s="67">
+      <c r="C52" s="48">
         <v>400</v>
       </c>
-      <c r="D52" s="67">
+      <c r="D52" s="48">
         <v>400</v>
       </c>
-      <c r="E52" s="67">
+      <c r="E52" s="48">
         <v>400</v>
       </c>
-      <c r="F52" s="67">
+      <c r="F52" s="48">
         <v>400</v>
       </c>
-      <c r="G52" s="67">
+      <c r="G52" s="48">
         <v>400</v>
       </c>
-      <c r="H52" s="67">
+      <c r="H52" s="48">
         <v>400</v>
       </c>
-      <c r="I52" s="67">
+      <c r="I52" s="48">
         <v>400</v>
       </c>
-      <c r="J52" s="68">
+      <c r="J52" s="49">
         <v>400</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B10:AB10"/>
-    <mergeCell ref="A1:AB1"/>
-    <mergeCell ref="B2:AB2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="K3:S3"/>
-    <mergeCell ref="T3:AB3"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="K11:S11"/>
-    <mergeCell ref="T11:AB11"/>
-    <mergeCell ref="B18:AB18"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="K19:S19"/>
-    <mergeCell ref="T19:AB19"/>
     <mergeCell ref="B44:S44"/>
     <mergeCell ref="B45:J45"/>
     <mergeCell ref="K45:S45"/>
@@ -25147,9 +25136,22 @@
     <mergeCell ref="B36:S36"/>
     <mergeCell ref="B37:J37"/>
     <mergeCell ref="K37:S37"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="K11:S11"/>
+    <mergeCell ref="T11:AB11"/>
+    <mergeCell ref="B18:AB18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="K19:S19"/>
+    <mergeCell ref="T19:AB19"/>
+    <mergeCell ref="B10:AB10"/>
+    <mergeCell ref="A1:AB1"/>
+    <mergeCell ref="B2:AB2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="K3:S3"/>
+    <mergeCell ref="T3:AB3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -25158,8 +25160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
dodanie nowych zdjęć i korekta wykresów
</commit_message>
<xml_diff>
--- a/doc/projekt/Wyniki_symulacji/Symulacje_podsumowanie.xlsx
+++ b/doc/projekt/Wyniki_symulacji/Symulacje_podsumowanie.xlsx
@@ -477,16 +477,16 @@
     <xf numFmtId="16" fontId="4" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="4" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="4" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -560,7 +560,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1061,11 +1060,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120753704"/>
-        <c:axId val="119666360"/>
+        <c:axId val="131614328"/>
+        <c:axId val="131675928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120753704"/>
+        <c:axId val="131614328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -1113,7 +1112,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1180,12 +1178,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119666360"/>
+        <c:crossAx val="131675928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119666360"/>
+        <c:axId val="131675928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1229,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1298,7 +1295,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120753704"/>
+        <c:crossAx val="131614328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1312,7 +1309,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1557,31 +1553,31 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>420.70145454545485</c:v>
+                  <c:v>441.72873181818193</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>456.59014090909096</c:v>
+                  <c:v>460.67873636363652</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>482.40016590909107</c:v>
+                  <c:v>495.48949545454553</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500.50382500000029</c:v>
+                  <c:v>531.33928863636413</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>505.33353863636319</c:v>
+                  <c:v>565.59052727272717</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>497.76450454545449</c:v>
+                  <c:v>579.83076136363638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>480.49092954545466</c:v>
+                  <c:v>886.17373181818209</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>451.64454545454572</c:v>
+                  <c:v>892.81167954545504</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>414.67259772727311</c:v>
+                  <c:v>468.91997272727247</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1671,31 +1667,31 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>411.2405499999997</c:v>
+                  <c:v>435.9562636363633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>440.77440909090922</c:v>
+                  <c:v>453.35875454545459</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>462.57894318181809</c:v>
+                  <c:v>487.67595454545483</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>475.44435681818175</c:v>
+                  <c:v>524.38026818181811</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>481.47893409090887</c:v>
+                  <c:v>556.20868409090895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>475.12503636363664</c:v>
+                  <c:v>575.19830681818155</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>459.86006363636329</c:v>
+                  <c:v>880.61192272727351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>435.26703409090942</c:v>
+                  <c:v>888.24685909090886</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>406.15855454545436</c:v>
+                  <c:v>461.67656363636371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2045,11 +2041,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="122311640"/>
-        <c:axId val="122306544"/>
+        <c:axId val="132382016"/>
+        <c:axId val="132384368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122311640"/>
+        <c:axId val="132382016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -2164,12 +2160,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122306544"/>
+        <c:crossAx val="132384368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122306544"/>
+        <c:axId val="132384368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2282,7 +2278,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122311640"/>
+        <c:crossAx val="132382016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3029,11 +3025,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="122308896"/>
-        <c:axId val="122312424"/>
+        <c:axId val="132385544"/>
+        <c:axId val="133160048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122308896"/>
+        <c:axId val="132385544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -3148,12 +3144,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122312424"/>
+        <c:crossAx val="133160048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122312424"/>
+        <c:axId val="133160048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3266,7 +3262,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122308896"/>
+        <c:crossAx val="132385544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3404,7 +3400,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3905,11 +3900,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119669496"/>
-        <c:axId val="119666752"/>
+        <c:axId val="131674360"/>
+        <c:axId val="131674752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119669496"/>
+        <c:axId val="131674360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -3957,7 +3952,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4024,12 +4018,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119666752"/>
+        <c:crossAx val="131674752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119666752"/>
+        <c:axId val="131674752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4075,7 +4069,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4142,7 +4135,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119669496"/>
+        <c:crossAx val="131674360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4156,7 +4149,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4902,11 +4894,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119668320"/>
-        <c:axId val="121005880"/>
+        <c:axId val="131675536"/>
+        <c:axId val="131676320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119668320"/>
+        <c:axId val="131675536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -5021,12 +5013,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121005880"/>
+        <c:crossAx val="131676320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121005880"/>
+        <c:axId val="131676320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5139,7 +5131,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119668320"/>
+        <c:crossAx val="131675536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5641,31 +5633,31 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>420.70145454545485</c:v>
+                  <c:v>441.72873181818193</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>456.59014090909096</c:v>
+                  <c:v>460.67873636363652</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>482.40016590909107</c:v>
+                  <c:v>495.48949545454553</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500.50382500000029</c:v>
+                  <c:v>531.33928863636413</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>505.33353863636319</c:v>
+                  <c:v>565.59052727272717</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>497.76450454545449</c:v>
+                  <c:v>579.83076136363638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>480.49092954545466</c:v>
+                  <c:v>886.17373181818209</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>451.64454545454572</c:v>
+                  <c:v>892.81167954545504</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>414.67259772727311</c:v>
+                  <c:v>468.91997272727247</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5899,11 +5891,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121007840"/>
-        <c:axId val="121004312"/>
+        <c:axId val="131673576"/>
+        <c:axId val="131673968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121007840"/>
+        <c:axId val="131673576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -6018,12 +6010,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121004312"/>
+        <c:crossAx val="131673968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121004312"/>
+        <c:axId val="131673968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6136,7 +6128,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121007840"/>
+        <c:crossAx val="131673576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6896,11 +6888,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121005488"/>
-        <c:axId val="121005096"/>
+        <c:axId val="132379664"/>
+        <c:axId val="132383192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121005488"/>
+        <c:axId val="132379664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -7015,12 +7007,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121005096"/>
+        <c:crossAx val="132383192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121005096"/>
+        <c:axId val="132383192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7133,7 +7125,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121005488"/>
+        <c:crossAx val="132379664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7896,11 +7888,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121007448"/>
-        <c:axId val="121001960"/>
+        <c:axId val="132379272"/>
+        <c:axId val="132383584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121007448"/>
+        <c:axId val="132379272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -8015,12 +8007,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121001960"/>
+        <c:crossAx val="132383584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121001960"/>
+        <c:axId val="132383584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8133,7 +8125,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121007448"/>
+        <c:crossAx val="132379272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8522,31 +8514,31 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>411.2405499999997</c:v>
+                  <c:v>435.9562636363633</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>440.77440909090922</c:v>
+                  <c:v>453.35875454545459</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>462.57894318181809</c:v>
+                  <c:v>487.67595454545483</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>475.44435681818175</c:v>
+                  <c:v>524.38026818181811</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>481.47893409090887</c:v>
+                  <c:v>556.20868409090895</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>475.12503636363664</c:v>
+                  <c:v>575.19830681818155</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>459.86006363636329</c:v>
+                  <c:v>880.61192272727351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>435.26703409090942</c:v>
+                  <c:v>888.24685909090886</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>406.15855454545436</c:v>
+                  <c:v>461.67656363636371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8896,11 +8888,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121002744"/>
-        <c:axId val="121003136"/>
+        <c:axId val="132383976"/>
+        <c:axId val="132380448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121002744"/>
+        <c:axId val="132383976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -9015,12 +9007,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121003136"/>
+        <c:crossAx val="132380448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121003136"/>
+        <c:axId val="132380448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9133,7 +9125,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121002744"/>
+        <c:crossAx val="132383976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9896,11 +9888,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121003920"/>
-        <c:axId val="122311248"/>
+        <c:axId val="132384760"/>
+        <c:axId val="132385936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121003920"/>
+        <c:axId val="132384760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -10015,12 +10007,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122311248"/>
+        <c:crossAx val="132385936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122311248"/>
+        <c:axId val="132385936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10133,7 +10125,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121003920"/>
+        <c:crossAx val="132384760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10880,11 +10872,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="122309680"/>
-        <c:axId val="122312032"/>
+        <c:axId val="132381624"/>
+        <c:axId val="132380840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122309680"/>
+        <c:axId val="132381624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -10999,12 +10991,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122312032"/>
+        <c:crossAx val="132380840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122312032"/>
+        <c:axId val="132380840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11117,7 +11109,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122309680"/>
+        <c:crossAx val="132381624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19288,8 +19280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView topLeftCell="E49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J52" sqref="A52:J52"/>
+    <sheetView topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21:S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19304,33 +19296,33 @@
       <c r="A1" s="64">
         <v>43871</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="68"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="66"/>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -20580,31 +20572,31 @@
         <v>740.69885454545465</v>
       </c>
       <c r="K21" s="24">
-        <v>420.70145454545485</v>
+        <v>441.72873181818193</v>
       </c>
       <c r="L21" s="24">
-        <v>456.59014090909096</v>
+        <v>460.67873636363652</v>
       </c>
       <c r="M21" s="24">
-        <v>482.40016590909107</v>
+        <v>495.48949545454553</v>
       </c>
       <c r="N21" s="24">
-        <v>500.50382500000029</v>
+        <v>531.33928863636413</v>
       </c>
       <c r="O21" s="24">
-        <v>505.33353863636319</v>
+        <v>565.59052727272717</v>
       </c>
       <c r="P21" s="24">
-        <v>497.76450454545449</v>
+        <v>579.83076136363638</v>
       </c>
       <c r="Q21" s="24">
-        <v>480.49092954545466</v>
+        <v>886.17373181818209</v>
       </c>
       <c r="R21" s="24">
-        <v>451.64454545454572</v>
+        <v>892.81167954545504</v>
       </c>
       <c r="S21" s="24">
-        <v>414.67259772727311</v>
+        <v>468.91997272727247</v>
       </c>
       <c r="T21" s="25">
         <v>420.91791136363628</v>
@@ -20666,31 +20658,31 @@
         <v>355.40791843315776</v>
       </c>
       <c r="K22" s="27">
-        <v>49.700885369824185</v>
+        <v>56.535938390912285</v>
       </c>
       <c r="L22" s="27">
-        <v>42.050532242040262</v>
+        <v>59.926350464118848</v>
       </c>
       <c r="M22" s="27">
-        <v>39.135446323687027</v>
+        <v>56.913924694107507</v>
       </c>
       <c r="N22" s="27">
-        <v>36.954734434805246</v>
+        <v>55.724431062868568</v>
       </c>
       <c r="O22" s="27">
-        <v>36.388874772272459</v>
+        <v>50.383255972234664</v>
       </c>
       <c r="P22" s="27">
-        <v>35.886178905116147</v>
+        <v>47.306385869909406</v>
       </c>
       <c r="Q22" s="27">
-        <v>38.284111873499604</v>
+        <v>484.88022136103478</v>
       </c>
       <c r="R22" s="27">
-        <v>43.511795450209704</v>
+        <v>358.92789600754793</v>
       </c>
       <c r="S22" s="27">
-        <v>51.29702671117527</v>
+        <v>83.694009527544495</v>
       </c>
       <c r="T22" s="28">
         <v>50.243057274791205</v>
@@ -20752,31 +20744,31 @@
         <v>432.87</v>
       </c>
       <c r="K23" s="27">
-        <v>306.49400000000003</v>
+        <v>323.11</v>
       </c>
       <c r="L23" s="27">
-        <v>334.49900000000002</v>
+        <v>312.709</v>
       </c>
       <c r="M23" s="27">
-        <v>377.49700000000001</v>
+        <v>337.40300000000002</v>
       </c>
       <c r="N23" s="27">
-        <v>397.25099999999998</v>
+        <v>373.65199999999999</v>
       </c>
       <c r="O23" s="27">
-        <v>397.505</v>
+        <v>421.84800000000001</v>
       </c>
       <c r="P23" s="27">
-        <v>385.64800000000002</v>
+        <v>435.62</v>
       </c>
       <c r="Q23" s="27">
-        <v>377.04599999999999</v>
+        <v>482.85599999999999</v>
       </c>
       <c r="R23" s="27">
-        <v>339.59800000000001</v>
+        <v>392.108</v>
       </c>
       <c r="S23" s="27">
-        <v>303.12299999999999</v>
+        <v>315.71100000000001</v>
       </c>
       <c r="T23" s="28">
         <v>310.27</v>
@@ -20838,31 +20830,31 @@
         <v>1724.2460000000001</v>
       </c>
       <c r="K24" s="40">
-        <v>521.99699999999996</v>
+        <v>567.50900000000001</v>
       </c>
       <c r="L24" s="40">
-        <v>559.81100000000004</v>
+        <v>602.79600000000005</v>
       </c>
       <c r="M24" s="40">
-        <v>584.08199999999999</v>
+        <v>650.95799999999997</v>
       </c>
       <c r="N24" s="40">
-        <v>600.27099999999996</v>
+        <v>660.63699999999994</v>
       </c>
       <c r="O24" s="40">
-        <v>596.17200000000003</v>
+        <v>707.702</v>
       </c>
       <c r="P24" s="40">
-        <v>594.52599999999995</v>
+        <v>713.17899999999997</v>
       </c>
       <c r="Q24" s="40">
-        <v>582.65300000000002</v>
+        <v>1776.329</v>
       </c>
       <c r="R24" s="40">
-        <v>556.38499999999999</v>
+        <v>1330.405</v>
       </c>
       <c r="S24" s="40">
-        <v>519.774</v>
+        <v>671.74099999999999</v>
       </c>
       <c r="T24" s="41">
         <v>528.78399999999999</v>
@@ -20897,24 +20889,24 @@
       <c r="A27" s="64">
         <v>43961</v>
       </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="65"/>
-      <c r="M27" s="65"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="65"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="65"/>
-      <c r="R27" s="65"/>
-      <c r="S27" s="66"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="67"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="67"/>
+      <c r="R27" s="67"/>
+      <c r="S27" s="68"/>
       <c r="T27" s="43"/>
       <c r="U27" s="43"/>
       <c r="V27" s="43"/>
@@ -22190,6 +22182,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="K45:S45"/>
+    <mergeCell ref="A27:S27"/>
+    <mergeCell ref="B28:S28"/>
+    <mergeCell ref="B36:S36"/>
+    <mergeCell ref="B44:S44"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="K37:S37"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="K29:S29"/>
     <mergeCell ref="A1:AB1"/>
     <mergeCell ref="B2:AB2"/>
     <mergeCell ref="B18:AB18"/>
@@ -22203,16 +22205,6 @@
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="K3:S3"/>
     <mergeCell ref="T3:AB3"/>
-    <mergeCell ref="B45:J45"/>
-    <mergeCell ref="K45:S45"/>
-    <mergeCell ref="A27:S27"/>
-    <mergeCell ref="B28:S28"/>
-    <mergeCell ref="B36:S36"/>
-    <mergeCell ref="B44:S44"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="K37:S37"/>
-    <mergeCell ref="B29:J29"/>
-    <mergeCell ref="K29:S29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
@@ -22224,8 +22216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView topLeftCell="L46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T79" sqref="T79"/>
+    <sheetView topLeftCell="A46" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="S61" sqref="S61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22240,33 +22232,33 @@
       <c r="A1" s="64">
         <v>43871</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="68"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="66"/>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -22986,31 +22978,31 @@
         <v>718.55398863636378</v>
       </c>
       <c r="K13" s="24">
-        <v>411.2405499999997</v>
+        <v>435.9562636363633</v>
       </c>
       <c r="L13" s="24">
-        <v>440.77440909090922</v>
+        <v>453.35875454545459</v>
       </c>
       <c r="M13" s="24">
-        <v>462.57894318181809</v>
+        <v>487.67595454545483</v>
       </c>
       <c r="N13" s="24">
-        <v>475.44435681818175</v>
+        <v>524.38026818181811</v>
       </c>
       <c r="O13" s="24">
-        <v>481.47893409090887</v>
+        <v>556.20868409090895</v>
       </c>
       <c r="P13" s="24">
-        <v>475.12503636363664</v>
+        <v>575.19830681818155</v>
       </c>
       <c r="Q13" s="24">
-        <v>459.86006363636329</v>
+        <v>880.61192272727351</v>
       </c>
       <c r="R13" s="24">
-        <v>435.26703409090942</v>
+        <v>888.24685909090886</v>
       </c>
       <c r="S13" s="24">
-        <v>406.15855454545436</v>
+        <v>461.67656363636371</v>
       </c>
       <c r="T13" s="25">
         <v>411.53037727272755</v>
@@ -23072,31 +23064,31 @@
         <v>324.44402199905977</v>
       </c>
       <c r="K14" s="27">
-        <v>27.372436876081746</v>
+        <v>43.402187000506345</v>
       </c>
       <c r="L14" s="27">
-        <v>34.943121051059293</v>
+        <v>30.472296421380229</v>
       </c>
       <c r="M14" s="27">
-        <v>42.738020632292304</v>
+        <v>37.777079133895334</v>
       </c>
       <c r="N14" s="27">
-        <v>47.540808054848263</v>
+        <v>42.413514363483252</v>
       </c>
       <c r="O14" s="27">
-        <v>47.948359462176569</v>
+        <v>52.60891295422968</v>
       </c>
       <c r="P14" s="27">
-        <v>46.779099078444531</v>
+        <v>59.851882705732798</v>
       </c>
       <c r="Q14" s="27">
-        <v>41.095023374279947</v>
+        <v>532.59570579908393</v>
       </c>
       <c r="R14" s="27">
-        <v>32.99968191074997</v>
+        <v>322.0138959928305</v>
       </c>
       <c r="S14" s="27">
-        <v>26.203909479429385</v>
+        <v>45.331122976647706</v>
       </c>
       <c r="T14" s="28">
         <v>27.414406121864403</v>
@@ -23158,31 +23150,31 @@
         <v>451.17899999999997</v>
       </c>
       <c r="K15" s="27">
-        <v>353.23399999999998</v>
+        <v>380.14400000000001</v>
       </c>
       <c r="L15" s="27">
-        <v>384.58800000000002</v>
+        <v>382.267</v>
       </c>
       <c r="M15" s="27">
-        <v>387.68200000000002</v>
+        <v>405.77699999999999</v>
       </c>
       <c r="N15" s="27">
-        <v>388.52600000000001</v>
+        <v>427.01799999999997</v>
       </c>
       <c r="O15" s="27">
-        <v>392.572</v>
+        <v>447.84899999999999</v>
       </c>
       <c r="P15" s="27">
-        <v>391.78100000000001</v>
+        <v>453.351</v>
       </c>
       <c r="Q15" s="27">
-        <v>382.86399999999998</v>
+        <v>442.18200000000002</v>
       </c>
       <c r="R15" s="27">
-        <v>375.22</v>
+        <v>433.089</v>
       </c>
       <c r="S15" s="27">
-        <v>341.89600000000002</v>
+        <v>372.31799999999998</v>
       </c>
       <c r="T15" s="28">
         <v>348.47500000000002</v>
@@ -23244,31 +23236,31 @@
         <v>1571.027</v>
       </c>
       <c r="K16" s="27">
-        <v>474.74</v>
+        <v>579.27800000000002</v>
       </c>
       <c r="L16" s="27">
-        <v>530.12099999999998</v>
+        <v>540.85500000000002</v>
       </c>
       <c r="M16" s="27">
-        <v>577.09900000000005</v>
+        <v>594.09299999999996</v>
       </c>
       <c r="N16" s="27">
-        <v>613.42499999999995</v>
+        <v>644.577</v>
       </c>
       <c r="O16" s="27">
-        <v>617.31399999999996</v>
+        <v>699.38900000000001</v>
       </c>
       <c r="P16" s="27">
-        <v>608.92999999999995</v>
+        <v>757.83399999999995</v>
       </c>
       <c r="Q16" s="27">
-        <v>585.55700000000002</v>
+        <v>1866.692</v>
       </c>
       <c r="R16" s="27">
-        <v>516.07100000000003</v>
+        <v>1260.511</v>
       </c>
       <c r="S16" s="27">
-        <v>465.91500000000002</v>
+        <v>565.25199999999995</v>
       </c>
       <c r="T16" s="28">
         <v>478.01600000000002</v>
@@ -23833,24 +23825,24 @@
       <c r="A27" s="64">
         <v>43961</v>
       </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="65"/>
-      <c r="M27" s="65"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="65"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="65"/>
-      <c r="R27" s="65"/>
-      <c r="S27" s="66"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="67"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="67"/>
+      <c r="R27" s="67"/>
+      <c r="S27" s="68"/>
       <c r="T27" s="43"/>
       <c r="U27" s="43"/>
       <c r="V27" s="43"/>
@@ -25126,6 +25118,19 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B10:AB10"/>
+    <mergeCell ref="A1:AB1"/>
+    <mergeCell ref="B2:AB2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="K3:S3"/>
+    <mergeCell ref="T3:AB3"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="K11:S11"/>
+    <mergeCell ref="T11:AB11"/>
+    <mergeCell ref="B18:AB18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="K19:S19"/>
+    <mergeCell ref="T19:AB19"/>
     <mergeCell ref="B44:S44"/>
     <mergeCell ref="B45:J45"/>
     <mergeCell ref="K45:S45"/>
@@ -25136,19 +25141,6 @@
     <mergeCell ref="B36:S36"/>
     <mergeCell ref="B37:J37"/>
     <mergeCell ref="K37:S37"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="K11:S11"/>
-    <mergeCell ref="T11:AB11"/>
-    <mergeCell ref="B18:AB18"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="K19:S19"/>
-    <mergeCell ref="T19:AB19"/>
-    <mergeCell ref="B10:AB10"/>
-    <mergeCell ref="A1:AB1"/>
-    <mergeCell ref="B2:AB2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="K3:S3"/>
-    <mergeCell ref="T3:AB3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>

</xml_diff>